<commit_message>
hide labels on graphs
</commit_message>
<xml_diff>
--- a/Faculty_Proposal_Abstracts.xlsx
+++ b/Faculty_Proposal_Abstracts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28706"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ucirvine.sharepoint.com/sites/BioSci-Contracts&amp;Grants-Team/Shared Documents/BioSci Research Development/Faculty-Keyword-Inventory-Project/faculty-mapped-mesh-terms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2821" documentId="11_D808F5E3348CBFB07090EECA229B558F1A7CE9CF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{79737B86-9845-2F43-91B0-D4094ED0012D}"/>
+  <xr:revisionPtr revIDLastSave="2962" documentId="11_D808F5E3348CBFB07090EECA229B558F1A7CE9CF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC3DA726-BCDB-420B-AC82-CF6DE0290F4C}"/>
   <bookViews>
-    <workbookView xWindow="28820" yWindow="-3100" windowWidth="40960" windowHeight="21100" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pre-Award README" sheetId="6" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1588" uniqueCount="868">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1675" uniqueCount="919">
   <si>
     <t>Instructions for Adding Proposals to Spreadsheet</t>
   </si>
@@ -3452,12 +3452,287 @@
   <si>
     <t>Humans; Compulsive Behavior; Data Aggregation; Data Collection; Physicians</t>
   </si>
+  <si>
+    <t>Lander, Arthur</t>
+  </si>
+  <si>
+    <t>Dr. Lander will be responsible for the analysis and interpretation of single-cell RNA sequencing data obtained from the analysis of the transition zone. He will also assist with the design of the experiments to collect such data. Analysis tasks will include normalization and clustering of raw data; assignment of cells based on donor cells and/or sex; integration and/or projection of data; statistical analysis of cell apportionment to different classes; analysis of cell state transitions using pseudotime, RNA velocity, or integrated methods; and analysis of cell state stability (entropy) and “tipping points”. He will also develop dynamical models, as necessary, to capture and predict chondrocyte state transitions. This work will be carried out jointly by Dr. Lander and a post-doc working under his supervision. Results will be presented on a regular basis to the PI, and Dr. Lander will participate in the design of experiments to validate or follow up on this analysis.</t>
+  </si>
+  <si>
+    <t>Male; RNA; Entropy; Chondrocytes; Follow-Up Studies; Cluster Analysis; Sequence Analysis, RNA; Data Analysis</t>
+  </si>
+  <si>
+    <t>Mortazavi, Ali</t>
+  </si>
+  <si>
+    <t>This project investigates the role of RNA modifications in the aging brain and their potential involvement in
+Alzheimer's Disease (AD). Using advanced long-read direct RNA sequencing, we will profile key RNA modifications—
+m6A, pseudouridine, inosine, and 5-methylcytosine—in the cortex and cerebellum of aged healthy and AD-affected
+individuals, as well as in mouse models of AD. The cortex is typically affected in AD, whereas the cerebellum is not,
+providing a unique comparative framework. By integrating these findings with publicly available data, we aim to identify
+conserved modification signatures across species, focusing on both protein-coding and long non-coding RNA genes. This
+research seeks to uncover novel molecular pathways involved in neurodegeneration, potentially leading to new diagnostic
+and therapeutic strategies.</t>
+  </si>
+  <si>
+    <t>Mice; Animals; 5-Methylcytosine; RNA, Long Noncoding; Pseudouridine; Alzheimer Disease; 6-methyladenine; Brain; Cerebellum; Sequence Analysis, RNA; Aging</t>
+  </si>
+  <si>
+    <t>Our understanding of cell lineages is currently being challenged. Cell plasticity appears to be more prevalent than previously thought and cell fate switching, even among fully differentiated cells is being more fully uncovered and understood. For example, ‘paligenosis’ is an emerging concept whereby fully differentiated cells revert to a stem cell like state and give rise to a multitude of cell types in part due to mTOR signaling. These observations have important implications for bone fracture healing. Multiple differentiation events occur for the bone to heal. Initially, the mechanical environment directs cell fate decisions within the periosteum. Mechanical stability directs differentiation of osteoblasts and intramembranous ossification, while instability directs differentiation of chondrocytes and endochondral ossification. Concomitantly, the stem cell compartment is maintained, and a renewed stem cell pool will eventually populate the periosteum that covers the new bone. At later stages of endochondral ossification chondrocytes become osteoblasts as the cartilage transforms into bone. Disruptions to these distinct events can lead to delayed or failed healing, which is often associated with increased fibrosis of the fracture site. In this application we propose to examine the process of differentiation of periosteal cells in response to the mechanical environment (Aim1), to assess transformation of chondrocytes into osteoblasts (Aim 2), and maintenance of the stem cell pool and population of the newly formed periosteum by stem cells (Aim 3). This work utilizes a systems biology approach to examine molecular mechanisms that underlie these cell fate decisions, and in parallel a more standard hypothesis-based approach. We focus on the role of Nf1 and Sox2 during differentiation of periosteal cells and the transformation of chondrocytes into osteoblasts. Our preliminary data show that deletion of Nf1 from the developing periosteum leads to a fibrous non-union after fracture, and we focus on the role of mTOR in mediating these outcomes. Our data also show that Sox2 is necessary for endochondral ossification, and we test the requirement of Sox2 in hypertrophic chondrocytes for transformation to osteoblasts. Finally, we examine a role for Sox2 in maintaining the stem cell compartment in the periosteum using a set of loss-of-function experiments in serial fracture repair. In summary, combining a systems biology approach with hypothesis testing is a powerful way to develop deep understanding of the processes regulating cell differentiation during fracture healing.</t>
+  </si>
+  <si>
+    <t>Chondrocytes; Osteogenesis; Cell Lineage; Periosteum; Fracture Healing; Cell Plasticity; Preliminary Data; Cell Differentiation; Cartilage; Osteoblasts; Stem Cells; TOR Serine-Threonine Kinases</t>
+  </si>
+  <si>
+    <t>Grill, Joshua</t>
+  </si>
+  <si>
+    <t>Tau protein is an attractive AD therapeutic target because the amount and anatomical distribution of insoluble tau at autopsy is strongly correlated with the symptoms and severity of disease during life. Multiple tau therapies are now in clinical trials for AD, with many new agents entering the clinic. New approaches to accelerating their clinical development are urgently needed. A variety of AD biomarkers now exist, including CSF and plasma beta amyloid ratios and phosphorylated tau (P-tau) levels, and amyloid and tau PET tracers, providing tools to measure pharmacodynamic effects of amyloid and tau therapies on the core biology of AD. The goal of the Alzheimer’s Tau Platform (ATP) trial is to conduct a randomized, placebo controlled, Phase 2 platform trial in preclinical-prodromal AD that will simultaneously test at least two different tau-directed therapies, alone or in combination with an anti-amyloid therapy, to determine safety, tolerability, and biological based proof of concept based on the tau PET tracer 18F MK6240 and other tau biomarkers. Platform trials create efficiencies through generation of a common clinical trial protocol and shared placebo groups to allow a greater number of therapies to be tested in less time with less expense than by conducting multiple independent trials. This trial will test 5 therapeutic hypotheses involving combinations of 3 drugs versus placebo: Two tau therapies will be studied in a 2 x 3 factorial design (placebo vs. anti-amyloid [n=2] x two tau therapies or placebo [n=3]) for 24 months, in six parallel arms. The key inclusion criteria for ATP will be &gt;20 centiloids of amyloid PET uptake, 18F MK6240 temporal ROI SUVr &gt;1.25, with a global Clinical Dementia Rating (CDR) of 0 or 0.5 and MMSE &gt;23. Using these criteria, we estimate that 150 participants per arm will be necessary to have 80% power to detect a 30% slowing in the accumulation 18F MK6240 signal over 24 months of blinded therapy. Key secondary endpoints will be changes in plasma P-tau species (-217, etc.) and neurofilament light chain (NfL), clinical rating scales and volumetric MRI. Leveraging the experience and resources of the NIH AD Clinical Trial Consortium (ACTC), we propose to enroll 900 participants at ~100 ACTC sites over 24 months, randomize them 5:1 drug:placebo for 24 months of blinded treatment, followed by a 24 month open label extension. We aim to: 1) test the ability of two tau-directed therapies, either alone or in combination with an anti-amyloid therapy, to slow the accumulation of tau PET signal over 24 months as compared to placebo or anti-amyloid therapy alone; 2) test the safety and tolerability of 24 months of blinded therapy followed by an optional 24 month open label extension of combination tau/anti-amyloid therapy; and 3) explore the ability of each of two tau directed therapies to slow disease progression as measured by CSF and plasma biomarkers (plasma P-tau, NfL), volumetric MRI and clinical assessments (Preclinical Alzheimer’s Composite [PACC], etc.). If successful, the ATP will provide data for decision-making about which tau therapies or combinations to pursue in larger efficacy studies, an ongoing resource to test new therapeutic approaches beyond tau, and will improve understanding of AD biology.</t>
+  </si>
+  <si>
+    <t>Humans; Amyloid beta-Peptides; tau Proteins; Alzheimer Disease; Goals; Intermediate Filaments; Amyloid; Mental Status and Dementia Tests; Biomarkers; Magnetic Resonance Imaging; Autopsy; Disease Progression; Severity of Illness Index; Biology; Adenosine Triphosphate; Randomized Controlled Trials as Topic; Clinical Trials, Phase II as Topic</t>
+  </si>
+  <si>
+    <t>LaFerla, Frank</t>
+  </si>
+  <si>
+    <t>The theme of University of California Irvine Alzheimer’s Disease Research Center (UCI ADRC) is accelerating
+discovery in Alzheimer’s disease (AD) and AD Related Disorders (ADRD) research across special populations.
+The UCI ADRC plays a distinctive role in the ADRC network, with a rich history of studying unique groups that
+have been underrepresented in AD/ADRD research. We have been a leader in research on individuals 90 years
+and older and our center was one of the first to study participants with Down syndrome (DS), groups at increased
+risk for dementia but often excluded from research. We have focused strongly on the underrepresented but
+rapidly growing populations of older Asian American and Hispanic individuals and have helped establish the first
+national registry of Asian American individuals to support inclusion in AD/ADRD research. We ensure data from
+these populations are available to the entire ADRC network through our Clinical Core, which emphasizes the
+earliest signs of disease, including mild behavioral impairment; and our unique special population DS Core and
+Oldest-Old Core. These invaluable resources synergize with our six other ADRC cores and our Research
+Education Component in a center that is highly collaborative. Our Neuropathology Core has shared tissue from
+&gt;1500 donated brains with &gt;120 investigators worldwide. Our induced Pluripotent Stem Cell Core was the first
+of its kind in the ADRC network and has shared iPSCs with &gt;70 laboratories worldwide and supported more than
+$125M in NIH-funded projects. Our Data Management and Statistical Core supports ADRC investigators through
+applied research and develops improved statistical methods. Our Biomarker Core implements state-of-the-art
+tools while researching ways to make biomarker information more accessible. Our Outreach Recruitment and
+Engagement Core has strong ties to the diverse local community and is a leader in the science of recruitment.
+The Administrative Core of UCI ADRC has consistently provided strategic leadership to ensure that our center
+constantly innovates, collaborates, and educates.</t>
+  </si>
+  <si>
+    <t>Humans; Aged, 80 and over; Down Syndrome; Alzheimer Disease; Data Management; Asian; Induced Pluripotent Stem Cells; Laboratories; Leadership; Brain; Registries; Biomarkers; Hispanic or Latino</t>
+  </si>
+  <si>
+    <t>Busciglio, Jorge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AD is characterized by progressive decline of cognitive functions due to the accumulation of extracellular plaques of Amyloid β (Aβ) and intraneuronal tangles composed of hyperphosphorylated forms of the microtubule associated protein tau (MAPT) (1). The amyloid precursor protein (APP) is a single transmembrane protein playing a central role in AD. APP is the only source of Aβ and is required for the cellular responses to Aβ, in part by signaling through heterotrimeric Go protein (2). Moreover, APP pathogenic mutations cause familiar forms of AD (FAD). These mutations were useful for generating in vitro and in vivo models of AD and helped for the design of diagnostic techniques for early detection of AD (3). However, FAD APP mutations were not equally successful in developing therapies to slow, halt or prevent AD pathology in humans.  In contrast to FAD APP mutations, naturally occurring non-pathogenic (or benign) APP mutations have received much less attention. This is surprising considering the existence of a non-pathogenic APP mutation that protects against AD, improving cognition in very elderly people (4).   In this project, we focus on the non-synonymous APP c.2198A&gt;C variation that was found in an individual from the Mandenka population (5), which encodes for His658Pro substitution (APP695 numbering)(M-APP). We hypothesize that M-APP protects against AD by reducing neuronal sensitivity to Aβ neurotoxicity by affecting Go protein signaling.  Since more than 30% of US Food and Drug Administration (FDA)-approved pharmaceutical drugs target GCRPs (11) we posit that APP-Go signaling is a molecular target for developing protective therapies for AD. To examine these hypotheses, we propose the following aims:  Aim 1. To address the mechanism by which M-APP affects Go protein signaling. Using molecular and imaging techniques we will address whether M-APP specifically affects binding to Gαo subunit and/or the activation of Go protein (that is, the exchange of GDP for GTP).   Aim 2. To design M-APP-derived peptides emulating the effects of holo M-APP at Go protein signaling. As proof of principle for the therapeutic potential of M-APP for AD, we will design M-APP-derived peptides and test their efficacy to modulate APP-Go protein signaling in response to Aβ.   Aim 3. To evaluate the therapeutic potential of modulating APP-Go signaling using human cellular models of AD.  We will test the therapeutic efficacy of M-APP-derived peptides in two cellular human models of AD: 1) primary human cortical cultures derived from euploid human fetal tissue (HFT) which develops AD-like features in response to Aβ-treatment; and  2) primary human cortical cultures derived from HFT with trisomy 21 that spontaneously develops AD-like features. These experiments will determine the potential of targeting APP-Go signaling as a therapeutic strategy for AD.  Collectively, these experiments will generate critical in vitro data addressing the potential of targeting APP-Go signaling as a therapeutic approach for AD. </t>
+  </si>
+  <si>
+    <t>Humans; Aged; Amyloid beta-Protein Precursor; Down Syndrome; United States Food and Drug Administration; Membrane Proteins; Cognition; Fetus; Mutation; Pharmaceutical Preparations; Peptides; Guanosine Triphosphate</t>
+  </si>
+  <si>
+    <t>Given the high incidence of COVID-19 neurological symptoms and the risk of long-term neuropathology in susceptible populations of patients, it is imperative to characterize the effects of SARS-CoV2 on brain cells, to elucidate the mechanisms underlying these effects, and to identify the populations susceptible to neurologic disease following infection. Equally important is to establish the relationships between SARS-CoV2 invasiveness and neurotropism on one hand, and the intrinsic ability of neural cells to mount an anti-viral response and clear up the virus on the other hand. Down Syndrome (DS) represents one of the most susceptible populations of COVID-19 patients, and thus a unique human genetic condition for investigating the cellular and molecular mechanisms underlying susceptibility of neurologically vulnerable individuals to SARS-CoV2 infection.  We hypothesize that neuro-invasiveness of SARS-CoV2 is facilitated in persons with DS due to neuroinflammation-driven disruption of the blood-brain barrier (BBB), which in turn increases the probability of direct SARS-CoV2 infection of neural cells. Once in the brain, the ability of SARS-CoV2 to infect and replicate will depend on the basal and induced interferon system activity, which ultimately will define the consequences of infection for Alzheimer’s disease (AD) neuropathology. The interferon system hyperactivation in DS might have a complex multiphasic effect on the outcome of SARS-CoV2 infection. To test this hypothesis, we propose three Specific Aims: (1) To elucidate the mechanistic relationships between SARS-CoV2 infectivity and interferon system-mediated antiviral response in human cortical cells with and without Hsa21 triplication; (2) To investigate the acute and longer-lasting consequences of viral infection on AD pathological hallmarks in T21 cortical cultures and brain specimens in relations to interferon system activity; (3) To investigate how the Amyloid-Tau-Neurodegeneration AT(N)29 biomarkers in DS individuals with COVID-19 history change in relations to their interferon system activity and the blood-brain barrier integrity.  We will employ a multidisciplinary and complementary approach, which includes in vitro studies, studies of postmortem brain specimens, and analyses of dataset and clinical plasma biomarkers. Combination of biochemical and molecular biology methods, super resolution confocal microscopy and existing clinical dataset analyses will be used to elucidate the relationships between inter-dependent mechanisms that underly neuro-invasiveness of SARS-CoV2, AD neuropathology in DS and the interferon system-mediated anti-viral defense mechanisms. Understanding these relationships is critical to predict infection outcome and to develop therapeutic strategies for protecting the vulnerable nervous system from virus-mediated damage.</t>
+  </si>
+  <si>
+    <t>Humans; Interferons; Blood-Brain Barrier; RNA, Viral; Neuroinflammatory Diseases; Down Syndrome; Alzheimer Disease; Incidence; COVID-19; Brain; Nervous System Diseases; Biomarkers; Antiviral Agents; Probability; Defense Mechanisms; Molecular Biology; Human Genetics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The goal of the University of California, Irvine MODEL-AD U54 Center is to develop novel mouse models of lateonset Alzheimer’s disease (LOAD), to deeply phenotype these and to make all data and mouse strains available to enable researchers to select the optimal mouse model and timepoints for therapeutic and intervention testing, as well as testing of hypotheses concerning mechanisms of LOAD. During the past five years, we have generated and deeply phenotyped mice with one component of our base genetic platform in which the Aß region of the App gene was converted from the rodent to the human sequence, and we have recently introduced the second component, a humanized MAPT (TAU) locus produced via gene-replacement. We have also used CRISPR and genome replacement to model and validate nine GWAS identified LOAD risk loci and have characterized mice with each of these both on a wild-type and 5xFAD background to determine their effects on plaque generation and damage exerted on the brain in response to pathology. In this continuation, we will use the results of these analyses to identify the combinations of LOAD risk variants most likely to phenocopy LOAD and introduce them on two complementary hAb-KI, hTAU, hAPOE4 platform lines, designed to mimic sub-types of AD that have been recently defined. To ensure translationability, we have an expanded focus on biomarkers and alignment with human phenotypes. To that end we have established a new Core – the Neuroimaging and neurovascular core (NIVC), which will provide brain imaging modalities currently employed in human AD subjects to align phenotypes in our mice with human disease progression. We have also expanded our fluid biomarker analysis efforts to include CSF, as well as plasma lipidomics and metabolomics to be compared to human AD plasma signatures. Similarly, our bioinformatics and data management efforts have been expanded to include single cell and nucleus RNA-seq and ATAC-seq, as well as spatial transcriptomics to enable alignment of data from our models with human AD signatures, but also to understand the mechanisms underlying disease progression in our mice. We are utilizing a comprehensive approach to evaluate our mice across their lifespans, which includes behavioral/cognitive assessment, electrophysiological analysis, super-resolution synaptic imaging, neuroimaging, bulk and single-cell RNA-seq, single cell level spatial transcriptomic analysis, unbiased proteomics, and microbiome and metabolome investigations. The UCI MODEL-AD Center will leverage the resources of our NIA-funded Alzheimer’s Disease Research Center combined with AMP-AD and other human AD datasets to facilitate comparisons to the human condition to identify the best mouse models to evaluate further. All data and models will be made available without restrictions, via The Jackson Labs, and data will be explorable via the modeladexplorer.org website, and raw data freely available for download via the AD Knowledge Portal. </t>
+  </si>
+  <si>
+    <t>Humans; Mice; Animals; Transcriptome; RNA-Seq; Data Management; Lipidomics; Alzheimer Disease; Longevity; Chromatin Immunoprecipitation Sequencing; Rodentia; Clustered Regularly Interspaced Short Palindromic Repeats; Genome-Wide Association Study; Goals; Mobile Applications; Proteomics; Single-Cell Gene Expression Analysis; Gene Expression Profiling; Brain; Phenotype; Neuroimaging; Biomarkers; Metabolome; Disease Progression; Microbiota; Cognition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Down syndrome (DS) is a developmental genetic condition caused by trisomy of human chromosome 21. DS occurs in approximately 1 in 600-1000 live births and affects more than 300,000 individuals in the USA. Neuropathological and clinical features of Alzheimer’s disease (AD) present early in life through the seventh decade in a predictable sequence of events, and include amyloid plaques, neurofibrillary tangles, NGF dysmetabolism and cholinergic basal forebrain degeneration, CNS inflammation, and cognitive decline. DS is an outstanding natural genetic model for the study of AD pathophysiology, AD biomarkers and to conduct preventive clinical trials. Despite the molecular and genetic similarities between AD and DS, there exists a paucity of information on the biological mechanisms underlying the onset of cognitive decline in adults with DS.  Our overall goal is to investigate the pathophysiological mechanisms and novel biomarkers in different stages of AD in DS by capitalizing on our ongoing successful collaboration between the teams of Jorge Busciglio (University of California, Irvine, USA), Claudio Cuello (McGill University, Montreal, Canada), Thomas Wisniewski (New York University, NY, USA) and Juan Fortea (Hospital of Sant Pau, Barcelona, Spain). To address our overarching objective, we have outlined three guiding AIMS:  1. To elucidate the relationships between AT(N) hallmarks, CNS inflammation and NGF dysmetabolism across the continuum of AD in DS;  2. To investigate to what extent NGF dysmetabolism and CNS inflammation are represented in plasma and CSF, and in neuronal- and astrocytic-derived extracellular vesicles (EVs) from brain tissue, primary cultures, and body fluids along the AD continuum in DS; and  3. To generate a framework for the temporal ordering of NGF dysmetabolism and CNS inflammation biomarkers within a cohort of adults with DS with multimodal AT(N) biomarkers.  Together, these Aims are focused in testing our central hypothesis that CNS inflammation and NGF metabolic dysfunction are early and central pathophysiological mechanisms leading to neurodegeneration and cognitive decline in AD. We will use a combination of unbiased discovery (transcriptomics and proteomics) and targeted biomarker analyses to uncover the molecular pathobiological progression of AD in DS in the different stages of AD taking full advantage of the predictable sequence of core AD biomarker changes in DS. The combination of neuropathological, cellular, and clinical studies using the same biomarkers will lead to a detailed characterization of AD stages that will enable a precision medicine approach that will inform future preventive trials and assist in the prediction of the onset and evolution of AD dementia and in the identification of novel therapeutic targets in this vulnerable population. </t>
+  </si>
+  <si>
+    <t>Adult; Down Syndrome; Trisomy; Alzheimer Disease; Precision Medicine; Neurofibrillary Tangles; Plaque, Amyloid; Proteomics; Vulnerable Populations; Basal Forebrain; Goals; Live Birth; Models, Genetic; New York; Spain; Universities; Chromosomes, Human, Pair 21; Extracellular Vesicles; Body Fluids; Biomarkers; Cognitive Dysfunction; Gene Expression Profiling; Humans; Female; Pregnancy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">■ I. Scientific goals. The overall goal of this proposal is to employ the power of full-length single molecule transcriptomics and RNA modification analysis, toward a better understanding of changes in RNA during longitudinal progression of neurodegenerative diseases.  We will continue our work using Huntington’s disease as a paradigm due to its known genetic nature24 and include FTD in later years based on new connections between these diseases at the level of dysregulation of TDP43,  cryptic exon expression and other dysregulated RBPs. Using this innovative approach, we will focus on two main parts of the project: ■ II. Research Outline:  Aim 1: Characterize primary transcriptome over time. Part 1a. – mouse. Our initial goals were to develop a pipeline to better understand how RNA molecules are differentially processed and expressed during disease onset as a function of time. We have generated preliminary data supporting feasibility of full-length, single molecule sequencing of mouse brain tissue RNA utilizing new methods for RNA isolation and computational and experimental pipelines developed10,12,13,25 in the Spitale lab to analyze long-read RNA sequencing data and accurately reconstruct spliced isoforms and abundance. Further, integration of differential short-read sequencing with altered m6A modification show differences in exon usage26 and potential RBP motif occupancy between HD and control animals (See Progress Report).  We will extend our analyses to include longitudinal assessment of single molecule long and short read RNAseq in striatum and cortex from HD fragment and knockin mice, wellestablished in the Thompson lab (e.g. 27–30) over time, evaluate aberrant splicing and cryptic exon usage, and determine whether these changes are reflective of altered RBP binding and TDP43 dysfunction.  We will also use novel chemical biology tools to investigate RNA dynamics of celltype specific RNAs using metabolic labeling and tracking. Part 1b.  Human iPSC. We will apply the methods developed in Part 1a in HD mice to HD and control iPSCs differentiated initially to neurons, for which we have numerous patient lines and expertise. These lines include control repeat length lines and expanded repeat lines with both adult onset and juvenile onset CAG repeats from both males and females.31–34 For these studies we will also utilize two novel sets of cell lines generated in the last year. 1) isogenic iPSC line with 53 or 18CAG repeats with a TurboID tag35 CRISPR engineered into the huntingtin locus to be used for CLIPseq/mass-spec experiments to identify RBPs bound to specific transcripts. TurboID is a biotin ligase that will label HTT RBP interactors and we have now developed a method for enrichment of RBP-RNA targets. This will allow us to investigate how HTT and mHTT regulates alternative splicing events through interactions with RBPs.   2) Isogenic CZI/iNDI lines with 19, 53 and 77 CAG repeats CRISPR-engineered within the KOLF2.1 line by Bill Skarnes (JAX), which can be directly compared to lines with TDP43 or C9 mutations from the iNDI portfolio.  Lines can be differentiated to astrocytes and microglia to also investigate cell type specific changes in RNA dynamics. For instance, expression of cryptic exons appear to have cell-type specific differences and variability.36  Aim 2. Determining the RNA modification landscape. We aim to increase our understanding of the relationship between disease state, RNA modifications and RNA processing and abundance. To do so, we will use Collaborative Pair developed chemical methods for enrichment of RNA modifications and transcriptomics for mapping. We focus on three chemical modifications of RNA: (1) methylation of adenosine (m6A), which is known to control RNA abundance by recruitment of RNA decay proteins. (2) Pseudouridylation (Ψ), which is has been reported to Ψs within mRNA may be of most importance in modulating transcript stability and protein translation. (3) Adenosine-to-Inosine editing, which is known to control protein re-coding and 3’-UTR regulation (See Figure 1B).7,22,23 Mass spectrometry: Using protocols developed during our Phase 1 project (see Progress Report), we will use isolated RNA from Aim 1 (time points and samples) and characterize RNA modification status of each of the marks using mass spectrometry analysis. As demonstrated in our Progress Report, we have developed highly sensitive LC-MS protocols for quantifying m6A abundance in RNA samples, observing a statistically significant difference between HD and WT samples. We will extend this analysis to the other modifications listed above. This will reveal the potential for global misregulation of RNA modification status. Transcriptome-wide mapping: We will use our developed and well-characterized methods of tagging each of these modifications and mapping their occupancy, transcriptome-wide.11,14,25 Using our established prototocols for RNA isolation from mouse brain and iPS -derived neurons (Aim 1), we will compare the RNA modification occupancy maps in WT and HD samples. This aim, on its own, will be significant because it will represent the first full analysis of RNA modifications over time in HD and WT samples. As demonstrated in our Progress Report, we have established robust enrichment, library construction, mapping, and enrichment score calling computational approaches that enable us to define the site of RNA modification.  Integrative analysis: Data generated in Aim 1 will be integrated with data herein, with the goal of understanding the relationship between alternative RNA processing and RNA abundance, related to modification status. As the modification enzymes are known for m6A deposition, Ψ isomerization, and A→I editing, we are well-positioned to systematically knock down each enzyme (shRNA; siRNA; CRISPR), to characterize global changes to the RNA modification status, and changes in RNA expression and alternative splicing.  Aim 3. Comparison of RNAs to patient samples. Our goal for this project is to transfer the richness of our datasets from the mouse and iPSC-based RNA analysis into clinical applicability and across disease.  Brain samples obtained from HD and unaffected individuals will be used to compare to our RNA analyses. We will utilize our tools to validate alternative splicing, RNA modifications, and changes associated with the mouse longitudinal analysis to patient samples (HD patient samples and controls). We will relate patient outcome, severity, and disease stage to RNA signatures of alternative splicing and RNA modification to derive potential RNA signatures that translate directly from the mouse model  and iPCS-neurons in culture to the human condition. We will also carry out analysis of brain tissue from human FTD (provided by Bill Seeley, personal communication) to compare to HD, with a specific emphasis on splicing that creates TDP43dependent cryptic exon usage. Such signatures would enable follow-up mechanistic analyses of alterations in RNA processing, expression, and modification and how these changes relate to the disease state. Given the encouraging results for drugs that can target splicing in SMA, clinical trials in HD (Novartis) and emergence of multiple companies targeting splicing for neurodegenerative disease, they will also ultimately enable the development of drugs that can target splicing, RNA processing and RNA modifications. Future. Future studies will incorporate outcomes of the Phase 1 studies with the growing understanding of the landscape of enzymes involved in RNA modifications and available methodologies to genetically perturb targets through CRISPR engineering and viral delivery approaches.  For instance, one can target enzymes involved in modulating m6A marks or A to I editing as in vitro and in vivo perturbations to investigate their impact on RNA dynamics. Through the CZI network ,a future goal would be to collaboratively develop novel high throughput readouts (e.g. reporters)  that can be used in CRISPRi and CRISPRa screens.  ■ III. Tools &amp; Resources:  We strive to build broadly applicable tools for the CZI network to better understand RNA structure and function, with applicable focus on neurodegenerative disease. We will merge our mechanistic work with real-world application through patient-derived sample analysis. This represents a paradigm for CZI investigators to characterize RNA function in their focused disease. Regents for generating RNA datasets and analytical frameworks for analyses will be made available for analysis of any cell type (normal or of neurodegenerative). Both partners are committed to understanding basic causal mechanisms and ultimately in the application of this knowledge to drug development.  We have profoundly benefitted from being part of the CZI Challenge Network and continuing within the NDCN would be a critical component of this research trajectory and further enable dissemination of the biochemical tools and patient datasets we are developing into the neurodegenerative disease community. </t>
+  </si>
+  <si>
+    <t>Humans; Female; Animals; Mice; Male; RNA, Small Interfering; RNA, Messenger; Biotin; Goals; Pharmaceutical Preparations; Alternative Splicing; Transcriptome; Liquid Chromatography-Mass Spectrometry; Neurodegenerative Diseases; Adenosine; Astrocytes; Microglia; 6-methyladenine; Chromatography, Liquid; Clustered Regularly Interspaced Short Palindromic Repeats; Feasibility Studies; Follow-Up Studies; Frontotemporal Dementia; Induced Pluripotent Stem Cells; Isomerism; Preliminary Data; Research Report; Tandem Mass Spectrometry; Sequence Analysis, RNA; Gene Expression Profiling; RNA Stability; Protein Isoforms; Protein Biosynthesis; Communication; Cell Line; Methylation; Drug Development; Exons; Mutation; Biology; Inosine; Ligases; Brain; Clinical Trials, Phase I as Topic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Huntington’s disease (HD) is characterized by gradual and progressive pathological changes at the molecular, cellular, tissue and neuronal circuit levels. We propose a multidisciplinary approach to identify and decipher the mechanisms of pathogenesis using human and mouse HD models. Our hypothesis is that pathological changes in key molecular and subcellular components and their interactions create time-dependent abnormal cellular dysfunction leading to circuit degeneration in HD. Furthermore, we posit that defining these changes and how they intersect will support identification of new effective therapeutic approaches. While much has been reported about cellular processes linked to neurodegeneration in HD, we still lack a clear understanding of how pathological phenotypes and processes are integrated and coordinated, how they impact organelle structure and function, and how specific molecular pathways intersect to disrupt neuronal structure, function and survival. To address these important challenges, and to clarify the pathogenic significance of changes more accurately in neuronal structure and function, we will identify multi-scale HD “signatures”, defined as a set of ultrastructural, cellular and molecular readouts representative of HD phenotypes in vulnerable neurons. Mechanisms that contribute to the formation of these signatures will be determined using directed perturbations to explore cause and effect relationships. We will formulate a quantiative system for these readouts towards degenerative phenotypes to help assess mechanism-targeted interventions designed to be clinically feasible. Specific Aims include: Aim 1: Identification of ultrastructural signatures to create an “HD structure database” in multiple HD neuron models: Studies of HD Pathology. We will use CryoET imaging and novel AI algorithms to identify and quantify ultrastructural signatures of disease (e.g., aberrant organelles) in HD models (human iPSC-derived cell types and cerebroids, mouse brain tissues, and synaptosomes). We will expand necessary structural analyses to integrate functional insights to reveal testable hypotheses for synaptic and neuronal dysfunction in HD. Aim 2: Mechanistic investigation of individual organelle and processes contributing to generation of neuronal HD signatures: Studies of HD Pathogenesis. We will design integrative measurements implemented in Aim 1 to confirm and/or modify our mechanistic models affecting a series of interconnected biological processes linked to HD pathogenesis, which form the basis of our next step in mechanism-based intervention strategy development. Aim 3: Preclinical mechanism-based therapeutic interventions: Innovations in HD Treatment. Applying informative quantitative measures, including each of the assay systems described in Aims 1 and 2, we will evaluate therapeutic interventions in vivo in animal models to slow or reverse HD disease progression to provide a rationale quantitative basis for HD preclinical studies.  </t>
+  </si>
+  <si>
+    <t>Humans; Mice; Animals; Synaptosomes; Induced Pluripotent Stem Cells; Neurons; Models, Animal; Organelles; Biological Phenomena; Brain; Disease Progression; Phenotype; Artificial Intelligence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Down syndrome (DS) is a developmental genetic condition caused by trisomy of human chromosome 21. DS occurs in approximately 1 in 600-1000 live births and is estimated to affect more than 300,000 individuals in the USA. Neuropathological and clinical features of Alzheimer’s disease (AD) present early in life through the sixth decade, and include amyloid plaques, neurofibrillary tangles, NGF dysmetabolism and cholinergic basal forebrain degeneration, CNS inflammation, and cognitive decline leading to AD dementia. Despite the molecular and genetic similarities between AD and DS, there exists a paucity of information on the biological mechanisms underlying the onset of cognitive decline in adults with DS. The study of AD preclinical phase is crucial for the development of treatments that could slow down or stop the progression of the disease.  The overall goal of this proposal is to investigate pathophysiological mechanisms and novel biomarkers at the earliest preclinical stages of AD in DS by capitalizing on our ongoing successful collaboration between the teams of Jorge Busciglio (University of California, Irvine, USA), Claudio Cuello (McGill University, Montreal, Canada), Thomas Wisniewski (New York University, NY, USA) and Juan Fortea (Hospital of Sant Pau, Barcelona, Spain). To address our overarching objective, we have outlined three guiding AIMS focused in testing our central hypothesis that the earliest accumulation of intracellular Aβ in DS brains causes CNS inflammation and accelerates NGF metabolic dysfunction prior to extracellular Aβ plaque deposition, eventually negatively impacting cognitive states: Aim 1: To establish the mechanisms and molecular interactions of CNS inflammation and NGF dysmetabolism across the continuum of AD in DS; Aim 2: To investigate to which extent NGF dysmetabolism and CNS inflammation are represented in free plasma and CSF, and in relation with neuronal and astrocytic extracellular vesicles (EVs) derived from brain tissue and body fluids across the AD continuum in DS; and Aim 3: To integrate CNS inflammation and NGF dysmetabolism into a global model of AD pathogenesis comprising AT(N) biomarkers.  The proposed studies use a multidisciplinary and complementary approach, which includes biochemical analysis of plasma, CSF and EVs as a new biofluid, neuropathological assessments, proteomics, in vitro cellular/molecular analyses, and a well-characterized cohort of DS individuals to uncover the molecular pathobiological mechanisms for DS/AD. The results will assist in the prediction of the onset and evolution of AD dementia and in the identification of novel therapeutic targets.  </t>
+  </si>
+  <si>
+    <t>Down Syndrome; Trisomy; Alzheimer Disease; Neurofibrillary Tangles; Plaque, Amyloid; Basal Forebrain; Goals; Live Birth; New York; Proteomics; Spain; Universities; Chromosomes, Human, Pair 21; Extracellular Vesicles; Body Fluids; Inflammation; Cholinergic Agents; Cognitive Dysfunction; Biomarkers; Cognition; Humans; Pregnancy; Female</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Down syndrome (DS) is a developmental genetic condition caused by trisomy of human chromosome 211-6. DS occurs in approximately 1 in 600-1000 live births and affects more than 300,000 individuals in the USA. Neuropathological and clinical features of Alzheimer’s disease (AD) present early in life through the seventh decade in a predictable sequence of events, and include amyloid plaques, neurofibrillary tangles, nerve growth factor (NGF) dysmetabolism and cholinergic basal forebrain degeneration, CNS inflammation, and cognitive decline1-10. DS is an outstanding natural genetic model for the study of AD pathophysiology, AD biomarkers research and to conduct preventive clinical trials. Despite the molecular and genetic similarities between AD and DS, there exists a paucity of information on the biological mechanisms underlying the onset of cognitive decline in adults with DS. For this INCLUDE application, our overall goal is to investigate DS-specific  pathophysiological mechanisms of AD and identify novel biomarkers within and outside of the AT(N) framework, with a special focus on immune and NGF dysregulation at different stages of AD pathology in DS by capitalizing on the ongoing highly successful collaboration between our teams: Jorge Busciglio (University of California, Irvine, USA), Claudio Cuello (McGill University, Montreal, Canada), Thomas Wisniewski (New York University, NY, USA) and Juan Fortea (Hospital of Sant Pau, Barcelona, Spain)7-9, 11, 12.  We propose to test the central hypothesis that CNS inflammation and NGF metabolic dysfunction are early and key pathophysiological mechanisms leading to neurodegeneration, accelerated aging and cognitive decline in DS. As detailed below, we will utilize a novel approach combining unbiased discovery (transcriptomics and proteomics) (Aim 1) and targeted biomarker analyses (Aim 2), using multiple complementary model systems, to establish a model of the temporal relationship between immune and NGF dysregulation and AD-related neurodegenerative changes in persons with DS (Aim 3). This will be achieved by correlating our findings with AD pathology, related biofluidic and imaging biomarker data from among the largest well characterized, DS patient population found globally. We propose the following 3 aims: Aim 1: To elucidate the relationships between immune deregulation and NGF dysmetabolism with AT(N) hallmarks in the DS brain and in human trisomy 21 cortical cultures.  Aim 2: To investigate the presence of immune dysregulation and NGF dysmetabolism markers in plasma and CSF and in extracellular vesicles derived from brain tissue, primary cultures and body fluids across the AD continuum in DS.  Aim 3: To establish the temporal ordering of immune dysregulation and NGF dysmetabolism with respect to the AT(N) framework within a cohort of adults with DS assessed longitudinally with multimodal biomarkers. The comprehensive combination of neuropathological, cellular, and clinical studies using the same biomarkers will lead to a detailed characterization of the role of immune and trophic factor alterations in the development of AD pathology and associated cognitive decline in DS.  Guided by the INCLUDE initiative goals, the results will inform future preventive trials and assist in the prediction of the onset and evolution of AD dementia and in the identification of potential novel biomarkers and therapeutic targets in this vulnerable population. </t>
+  </si>
+  <si>
+    <t>Humans; Adult; Down Syndrome; Trisomy; Nerve Growth Factor; Goals; Alzheimer Disease; Neurofibrillary Tangles; Plaque, Amyloid; Proteomics; Vulnerable Populations; Basal Forebrain; Live Birth; Models, Genetic; New York; Spain; Universities; Extracellular Vesicles; Aging; Body Fluids; Biomarkers; Cognitive Dysfunction; Gene Expression Profiling; Cognition; Female; Pregnancy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Background  Answer ALS is one of the largest concerted and coordinated collaborative efforts bringing together many disciplines and data types. Over1000 subject motor neuron samples are being generated, and the data derived from these lines are being analyzed for signatures that define significant pathways and networks. One challenge in discovering these appropriate cellular signatures is finding a protocol that can scale to accommodate 1000 lines and still model features of the motor neurons located in participants.  Since starting this project, the team has made considerable progress toward the high-level goal of advancing research in this area. Currently, we have eight leading ALS Clinics around the US that have enrolled over 1000 ALS patients and 100 controls in the Program. Of those participants, we have sequenced 888 (866 available for download) genomes which concludes the whole genome sequencing portion of the project. In addition, we have generated 623 motor neuron lines using the 32-day protocol for use in the primary assays, and we have over 600 stem cell (iPSC) lines available for scientists to use in their research.  The OMICs labs have received over 700 samples for processing as of June 2022. Of the ~700 processed samples, 590 are unique Answer ALS participant samples and 88 technical controls with the remaining repeat Study batches. Therefore, the Program is asking to have 590 unique data sets for each OMIC available in Azure staging by December 31, 2022. In addition, the Answer ALS team continues to support the second-generation data portal that allows users to access, filter, and download the data.  This statement of work covers July 1, 2023, through December 2024. During this time, the OMICs centers will receive and process approximately 500 lines through to data QC. We aim to release around 700 complete datasets to the public by Dec 31, 2023, for each OMIC assay.  As the new lines become available, the team will begin processing, sequencing, and QC the data generated from these subjects.  </t>
+  </si>
+  <si>
+    <t>Humans; Induced Pluripotent Stem Cells; Goals; Motor Neurons; Neurons, Efferent; Whole Genome Sequencing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It is with great enthusiasm and gratitude that we submit this proposal for funding to the Diane and Guilford Glazer Foundation. As you know, the UC Irvine Institute for Memory Impairments and Neurological Disorders (UCI MIND) is a world-renowned research organization devoted to the study of Alzheimer’s disease (AD) and Alzheimer’s disease-related dementias (ADRD). This includes a more than 30 year history of being at the cutting edge of discoveries related to AD/ADRD. Our more than 50 renowned faculty include basic and well as clinical research scientists and the mission of UCI MIND is to bring these transdisciplinary investigators together to perform collaborative and indeed synergistic research to accelerate pursuit of solutions for these burdensome neurodegenerative diseases.  In this proposal titled “Investigating Mild Behavior Impairment,” we propose to leverage our cohort of more than 300 individuals who have enrolled in longitudinal observational research at UCI MIND to better elucidate the earliest symptoms associated with AD/ADRD.  Mild Behavior Impairment (MBI) is a relatively recently developed clinical construct, proposed to ensure that patients with neurological conditions such as Alzheimer’s who do not first present with typical symptoms such as memory loss are not missed. MBI can include subtle behavioral symptoms such as apathy, anxiety, anhedonia, and depression, as well as more overt symptoms such as agitation, delusions, hallucinations, and changes in personality. In all cases, patients with MBI are at risk for misdiagnosis as late onset psychiatric conditions (e.g., schizophrenia) when in fact they suffer from a neurodegenerative condition such as AD. UCI MIND Director of Clinical Research Dr. David Sultzer is a geriatric psychiatrist and an international leader and collaborative architect of the MBI construct. In the work funded by the Glazer Foundation, Dr. Sultzer will lead innovative research to better understand MBI at UCI.  Dr. Sultzer aided in the developing the “MBI checklist” a novel tool to better capture the presence or absence of mild behavioral symptoms in people with or at risk for cognitive impairment and dementia. With support from the Glazer Foundation, we will collect the MBI checklist from our entire research cohort and perform a variety of novel analyses not otherwise possible. These will include: • Determine whether MBI severity is associated with diagnostic categories. Among our cohort of participants, some are unimpaired, some have mild cognitive impairment (MCI), and some have full blown dementia. We will assess whether the severity of MBI is associated with these diagnostic categories, assessing the hypothesis that greater diagnostic severity is associated with greater MBI severity.  • Assess the relationship between MBI and AD biomarkers in the cerebrospinal fluid. In addition to our large cohort of participants, UCI MIND has a long and successful history of securing biomarker assessments, including measures of cerebrospinal fluid (CSF; examined through lumbar puncture), from research participants. This positions us to assess the relationship between MBI severity and AD biomarkers in CSF (amyloid beta [Ab], phosphorylated tau [p-tau], and total tau[t-tau]). We will begin by determining whether such relationships exist, particularly among individuals who do not meet clinical criteria for MCI or dementia. We hypothesize that MBI severity is associated with a biomarker signature in CSF among individuals who do not meet diagnostic criteria for AD.  • Determine the longitudinal course of MBI. Requiring multiple years of follow-up, we will be well positioned to understand the stability and importance of change over time in MBI presentation. We plan to assess MBI routinely in our large annual follow-up longitudinal study. We anticipate that this will allow UCI MIND to produce some of the first findings based on longitudinal assessments in the field. We hypothesize that changes in MBI will precede cognitive changes, particularly in participants with no demonstrable cognitive impairment.  In conclusion, with support from the Glazer Foundation, UCI MIND will be positioned to continue our leadership in AD/ADRD research, particularly in the area of MBI. We would be thrilled to establish periodic reports, including in-person presentations of our progress to the Foundation leadership and look forward to a productive long-term relationship.  </t>
+  </si>
+  <si>
+    <t>Given the high incidence of COVID-19 neurological symptoms and the risk of long-term neuropathology in susceptible populations of patients, it is imperative to characterize the effects of SARS-CoV2 on brain cells, to elucidate the mechanisms underlying these effects, and to identify the populations susceptible to neurologic disease following infection. Equally important is to establish the relationships between SARS-CoV2 invasiveness and neurotropism on one hand, and the intrinsic ability of neural cells to mount an anti-viral response and clear up the virus on the other hand. Down Syndrome (DS) represents one of the most susceptible populations of COVID-19 patients, and thus a unique human genetic condition for investigating the cellular and molecular mechanisms underlying susceptibility of neurologically vulnerable individuals to SARSCoV2 infection. We hypothesize that neuro-invasiveness of SARS-CoV2 is facilitated in persons with DS due to neuroinflammation-driven disruption of the blood-brain barrier (BBB), which in turn increases the probability of direct SARS-CoV2 infection of neural cells. Once in the brain, the ability of SARS-CoV2 to infect and replicate will depend on the basal and induced interferon system activity, which ultimately will define the consequences of infection for Alzheimer’s disease (AD) neuropathology. The interferon system hyperactivation in DS might have a complex multiphasic effect on the outcome of SARS-CoV2 infection. To test this hypothesis, we propose three Specific Aims: (2) (1) To elucidate the mechanistic relationships between the susceptibility of human cortical cells to SARS-CoV-2 infection and interferon system activity in these cells; To investigate the acute and longer-lasting consequences of viral infection on AD pathological hallmarks in trisomy-21 (T21) cortical cultures and brain specimens; (3) In a cohort of DS patients, to investigate the relationships between plasma biomarkers that reflect interferon system activity and A myloidT auN eurodegeneration AT(N) biomarkers that reflect AD pathology. We will employ a multidisciplinary and complementary approach, which includes in vitro studies, studies of postmortem brain specimens, and analyses of dataset and clinical plasma biomarkers. Combination of biochemical and molecular biology methods, super resolution confocal microscopy and existing clinical dataset analyses will be used to elucidate the relationships between inter-dependent mechanisms that underly neuroinvasiveness of SARS-CoV2, AD neuropathology in DS and the interferon system-mediated anti-viral defense mechanisms. Understanding these relationships is critical to predict infection outcome and to develop therapeutic strategies for protecting the vulnerable nervous system from virus-mediated damage.</t>
+  </si>
+  <si>
+    <t>Humans; Aged; Amyloid beta-Peptides; Neurodegenerative Diseases; Apathy; Schizophrenia; Spinal Puncture; Leadership; Anhedonia; Alzheimer Disease; Checklist; Follow-Up Studies; Delusions; Depression; Longitudinal Studies; Psychiatrists; Cognitive Dysfunction; Anxiety; Memory Disorders; Hallucinations; Faculty; Cognition; Biomarkers; Diagnostic Errors</t>
+  </si>
+  <si>
+    <t>Kawas, Claudia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The 90+ Study was initiated January 1, 2003 as a population-based sample of oldest-old survivors of the Leisure World Cohort Study (LWCS, enrollment 1981-1984). With more than 1,800 participants, The 90+ Study is one of the largest and longest studies in the world of dementia, cognitive decline, disability, and frailty in the oldestold. People over 90 are the fastest segment of the population and have the greatest public health impact as the risk of dementia is extraordinarily high in these individuals, reaching a staggering 40% per year in centenarians. However, many oldest old maintain superior cognitive performance well into their tenth decade and beyond (cognitive resilience), often in the presence of neuropathological changes (cognitive resilience in the presence of pathology). Lifestyle, co-morbid conditions, genetics, and other factors have been implicated in this cognitive resilience but have not been well studied. In this application, we extend our studies to investigate cognitive resilience in these remarkable individuals. In Aim 1, we consider early (30 years earlier in the LWCS) and late (at age 90+) lifestyle and other factors in relation to cognitive resilience. Factors related to the maintenance of superior cognitive abilities in the presence of pathology are investigated in Aim 2. Taking advantage of our large cohort of 90+ year-olds in our imaging studies, we prospectively follow individuals without dementia to estimate incidence of dementia and rates of cognitive decline in relation to MRI and PET biomarkers in Aim 3. We analyze the role of low levels of multiple neuropathologic changes in the expression of dementia in Aim 4. Finally, with this application, we will recruit the last living LWCS participants eligible for our study, and complete ascertainment of all previously established outcomes in The 90+ Study (dementia, CIND, MCI, frailty, disability, and mortality). We will make this dataset spanning almost four decades publicly available to the research community (Aim5). With our extensive database, unique large cohort of well-characterized individuals, extensive and multidisciplinary longitudinal follow-up, and innovative neuropathological and neuroimaging investigations, we are ideally positioned to do studies of dementia and resilience in the oldest-old. Identifying factors related to cognitive resilience and dementia, including modifiable lifestyle factors and imaging biomarkers, would contribute to our understanding of aging in health and disease and provide potential targets for interventions to promote successful aging. </t>
+  </si>
+  <si>
+    <t>Humans; Aged, 80 and over; Cohort Studies; Centenarians; Frailty; Public Health; Follow-Up Studies; Incidence; Resilience, Psychological; Cognitive Dysfunction; Cognition; Neuroimaging; Aging; Magnetic Resonance Imaging; Dementia; Biomarkers; Life Style; Positron-Emission Tomography</t>
+  </si>
+  <si>
+    <t>Blurton-Jones, Mathew</t>
+  </si>
+  <si>
+    <t xml:space="preserve">he defining pathological hallmarks of Alzheimer’s Disease (AD) were first described over a hundred years ago, however many of the critical steps that underlie disease development and pathological progression remain unclear. A prime example of this knowledge gap relates to our lack of understanding as to how amyloid pathology drives the subsequent development of neurofibrillary tangles. An abundance of genetic, biochemical, pathological, and cognitive data underlies the hypothesis that an imbalance between the production and clearance of amyloid β-42 peptide (Aβ42) promotes Aβ aggregation and initiates AD pathogenesis1-3. Aβ plaque deposition in turn leads to a cascade of events including neuroinflammation which promote the hyperphosphorylation, aggregation and deposition of the microtubule binding protein tau, leading to the development of  neurofibrillary tangles1,4 followed by synaptic loss, neuronal cell death and cognitive impairment. Genome wide association studies (GWAS) combined with data obtained from human studies and mouse modelling suggest that microglia are strongly tied to AD susceptibility through numerous functions, including phagocytosis, metabolic fitness, and cytokine/chemokine signaling5-7. As whole genome sequencing datasets continue to grow, so too does the possibility of finding rare variants that could provide resilience to the development and progression of these pathologies. Yet understanding the mechanisms by which rare variants influence resilience as they could impact one or many aspects of disease pathogenesis8,9. Accordingly, novel cell and animal models of AD are needed to provide unique, translationally relevant opportunities to decipher the mechanisms that underlie resilience, which could in turn be used to identify promising new therapeutic targets. One of the most striking examples of a rare variant that promotes resilience is the rare variant of Apolipoprotein E (APOE), ApoE3 Christchurch10,11. This mutation was first identified in a patient that carried a dominantly inherited Presenilin 1 mutation yet remained cognitively sharp 3 decades past her expected age of developing AD symptoms. While the patient exhibited extensive Ab plaque pathology, she exhibited limited tangle pathology in regions of brain normally affected in AD (i.e frontal cortex) and did not develop significant cognitive impairments. Brain regions free of tau pathology harbored homeostatic astrocytes and microglia expressing genes involved in acute immune responses12. This observation, combined with recent data from transgenic mice13 further supports the notion that the Christchurch mutation disrupts the normally exacerbating influence of amyloid pathology on neurofibrillary tangle development. APOE is the strongest genetic risk factor for AD. The apoE protein has important roles in lipid homeostasis including the shuttling of cholesterol and lipids between cells in brain14. Numerous reports have identified the isoform and cell-specific effects of apoE on AD and an emerging body of evidence suggests that microglial apoE plays critical roles in AD pathogenesis14-16. In particular, microglial lipid metabolism regulated by apoE has emerged as a critical player in regulating neuroinflammation, especially in the context of amyloid-induced acceleration of tau pathology.  A major challenge in studying microglia cells is that murine microglia fail to recapitulate some key aspects of the human condition due to species-specific variations in both amino acid sequence and function. The murine orthologue of ApoE markedly differs from human APOE as it lacks disease-associated isoforms17,18. Moreover, even though amyloidosis and tauopathy induce an apoE-mediated response in microglia, major differences between human and mouse microglia, including their different disease associated microglia (DAM) phenotypes, highlights the importance of using complimentary human systems to examine this. Induced pluripotent stem cell (iPSC)derived microglia (iMG) have improved our ability to model and study human-specific genes19,20. However, microglia are highly sensitive to their environment and manifest numerous transcriptomic deficiencies when kept in isolation from the brain20,21. The Blurton-Jones lab has sought to address this challenge by developing chimeric mouse models to study iPSC-derived microglia within a surrogate brain environment22. This novel technology allows for application of AD mouse models such as the 5XFAD model of amyloidosis or PS19 model of tauopathy in a unique setting wherein the interactions between xenotransplanted human microglia (xMGs) and disease pathogenesis can be thoroughly investigated.
+APOE modulates multiple pathways in the brain including Aβ and tau clearance, lipid metabolism and immune responses27-30. Emerging studies show that microglia, particularly plaque-associated microglia24, produce and secrete abundant amounts of apoE. Human microglia also express high levels of receptors that interact with apoE (e.g LRP-1, LDLR, VLDLR, and various heparin sulfate proteoglycans), suggesting that microglial apoE not only modulates other cell types, but likely also influences microglial function via autocrine signaling15. We therefore hypothesize that the protective effects of the apoE Christchurch variant are mediated in part by modulating autocrine microglial responses, and that apoE3-Ch microglia will i) increase the clearance of neurotoxic Aβ species, ii) exhibit decreased pro-inflammatory states, and iii) diminish tau phosphorylation, uptake, and spread. To test this overarching hypothesis, we will perform a series of functional and metabolic assays on human isogenic iPSC-derived microglia (iMG) expressing apoE3 or apoE3-Ch in vitro and study the interactions between human microglia and combined amyloid and tau pathologies in vivo (Figure. 1).  ApoE3-Ch was associated with limited tau pathology and neurodegeneration despite high amyloid burden in the PSEN1 E280A carrier, suggesting that APOE-Ch is highly protective against amyloid-driven tau pathology. Additionally, apoE is a crucial lipid transporter in the brain, playing key roles in regulating lipid metabolism. Accordingly, we hypothesize that specific expression of apoE3-Ch in microglia induces significant autocrine changes in microglial function, transcription, and metabolic state. Using complementary in vitro and in vivo platforms, we will explore this hypothesis.  Aim.1. Does the APOE3-Ch mutation alter the response of human microglia to disease related challenges including fibrillar Aβ, myelin and tau oligomers? Taking advantage of previously established in vitro platforms in our lab19,31,  as well as others32, we will explore the impact of APOE-Ch on challenged microglia by investigating changes in i) cell function (phagocytosis and tau spread assays), ii) gene transcription (scRNAseq) and iii) metabolic state and iv) proinflammatory cytokine production.   Aim.2. Does expression of apoE3-Ch in human microglia influence amyloid pathology, Aβ-mediated exacerbation of neurofibrillary tangles and formation of rod microglia in PS-5X mice? Human studies point to crucial roles of APOE in Aβ-induced tau pathogenesis in AD28,33,34. Moreover, the APOE3-Ch variant was associated with limited tau pathology despite severely elevated levels of Aβ in a human patient10,12. We therefore aim to examine the impact of human microglial-derived apoE3-Ch on AD pathogenesis in vivo, including the effects on i) Ab and tau pathologies, ii) cytokine and chemokine production, iii) biochemistry of aggregated proteins and iv) pathology-associated alterations in human and murine gene expression via spatial transcriptomics. Our ultimate goal in this aim is to decipher the mechanisms through which microglia-specific expression of apoE3-Ch can modulate Aβ-induced exacerbation of tau pathology. </t>
+  </si>
+  <si>
+    <t>Humans; Male; Female; Animals; Mice; peptide A; Phosphorylation; Genome-Wide Association Study; Apolipoprotein E3; Neurofibrillary Tangles; Microglia; heparin proteoglycan; Induced Pluripotent Stem Cells; Lipid Metabolism; Amino Acid Sequence; Cytokines; Alzheimer Disease; Transcriptome; Neuroinflammatory Diseases; Astrocytes; Myelin Sheath; Presenilin-1; Resilience, Psychological; Goals; Single-Cell Gene Expression Analysis; Apolipoproteins E; Homeostasis; Brain; Amyloidosis; Phenotype; Models, Animal; Protein Isoforms; Mutation; Chemokines; Microtubules; Phagocytosis; Cell Death; Whole Genome Sequencing; Cholesterol; Cognitive Dysfunction; Frontal Lobe; Risk Factors; Cognition</t>
+  </si>
+  <si>
+    <t>Nie, Qing</t>
+  </si>
+  <si>
+    <t>In biological tissues, cells are continually receiving inflows of biochemical signals in the form of cell-cell
+communication (CCC), which are processed through intracellular gene regulatory networks (GRNs), that, in turn,
+may cause an outflow of signals that affect other cells. These flows of “cause and effect” relations, which are
+spatiotemporal in nature and drive every biological process, are often instigators of diseases. Single-cell
+genomics technologies that profile genes and their activities at the individual cell level provide an unprecedented
+opportunity to systematically screen such cellular flows.
+During the past four years, computational tools have been developed for CCC or GRN inference using
+nonspatial single-cell (sc) RNA-seq data, and more recently, some of these tools have been specialized for
+spatial transcriptome (ST) data. While those methods, such as ours (CellChat for scRNA-seq, COMMOT for ST),
+are effective in uncovering CCC links between two given groups of cells, no studies have addressed the
+important question: how one CCC link between cells may affect another intercellular CCC link and, if so, through
+which intracellular GRNs, the latter of which can be inferred using, for example, our method, SpliceJAC.
+This application will focus on addressing the question of inferring cellular flows from non-spatial scRNA-seq
+and ST data. The first aim will be to use causal structure learning models to learn intercellular flows driven by
+CCC directly from either scRNA-seq data equipped with biological time or perturbations or ST data where the
+action range of CCC can be constrained. The second aim will integrate coarse-grained models of intercellular
+flows with detailed models of intercellular GRNs that account for signal inflow and outflow, while extending RNA
+velocity models to ST to construct a cell-state transition landscape in space. The third aim is to validate the
+developed methodologies using an experimental system of cortical organoids whose underlying signal
+interactions can be perturbed and tracked over space and time using traditional wet lab techniques in conjunction
+with newly generated scRNA-seq and ST data.
+The study premise is based on our novel and extensive preliminary results in CCC and GRN inference
+and cell-state landscape reconstruction. The proposed studies are significant because they will create the first
+multiscale frameworks that infer cellular flows directly from high-dimensional transcriptomics data by linking
+intercellular communication to intracellular GRNs, generating novel insights into the causal mechanisms that
+allow information to flow within and across biological tissue. These studies are innovative because the proposed
+tools will extract important spatiotemporal information from static scRNA-seq and ST data that have previously
+been impossible to obtain. They will connect several important mathematical and computational concepts,
+including causal structure learning, topological data analysis, multilayer networks, and dynamical systems, that
+will have broad applications in single-cell and spatial genomics.</t>
+  </si>
+  <si>
+    <t>Transcriptome; Gene Regulatory Networks; RNA-Seq; Single-Cell Gene Expression Analysis; Gene Expression Profiling; Data Analysis; Biological Phenomena; Cell Communication</t>
+  </si>
+  <si>
+    <t>Cells communicate locally within tissue and between different parts of the body to maintain biological functions.
+There are two major different communication mechanisms: a) short-range interactions involving signal ligands
+that are diffused into extracellular space and bind to receptors on cells or transmitted via direct cell-to-cell contact;
+and b) long-range interactions involving metabolism and endocrine molecules that are transported through
+extracellular fluids, such as the bloodstream or cerebrospinal fluid, from one part of the body to another. Crosstalk
+often occurs between different communication signals within or across these two kinds of interactions to regulate
+shared downstream targets (e.g., transcriptional factors) to coordinate multiple biological functions.
+Recently, various computational tools, including ours, have enabled inference and analysis of cell-cell
+communication via short-range interactions using single-cell RNA-sequencing and spatial transcriptomics data.
+However, there are no tools to infer cell communication induced by long-range interactions, which are known to
+be critical to metabolic and endocrine diseases, as well as digestive and kidney diseases.
+This application will focus on addressing three major unaddressed challenges to infer long-range interactions
+using spatial transcriptomics data and other existing single-cell omics data. First, we will develop a database and
+a tool to systematically screen metabolic communication between cells in spatial tissues using a novel Flow
+Optimal Transport method. Second, we will develop methods to uncover communication between different
+organs by using mechanistic modeling combined with machine learning. Third, we will screen and quantify
+crosstalk between different organs, signaling pathways, and different types of long-range and short-range
+molecules using a hypergraph learning approach.
+The study premise is based on our experience with developing tools for short-range interactions, novel and
+extensive preliminary results on long-range interaction inference, and a detailed plan with strong preliminary data
+for validation and benchmarking The proposed studies are significant because they will create the first set of
+comprehensive integrated tools that can infer metabolic communication flow and organ-organ communication
+mediated by crosstalk among multiple pathways by fully utilizing various types of single-cell and spatial omics
+data. The proposed studies are innovative because these new tools will have multiple novel functionalities that
+can derive crucial biological information that is currently impossible to obtain. The study will result in several
+novel methodologies in multiscale modeling, optimal transport, and deep learning with broad applications in
+omics data analysis and beyond. Just as CellChat and COMMOT, developed by us, generated unprecedented
+biological discoveries related to short-range interactions, this study will generate unprecedented biological
+discoveries related to cell communication, and open new avenues for developing inference and modeling tools
+of various mechanisms in cell communication.</t>
+  </si>
+  <si>
+    <t>Extracellular Fluid; Extracellular Space; Benchmarking; Deep Learning; Preliminary Data; Endocrine System Diseases; Signal Transduction; Cell Communication; Gene Expression Profiling; Kidney Diseases; RNA; Humans</t>
+  </si>
+  <si>
+    <t>In response to RFA-DA-23-039 (BRAIN Initiative: Theories, Models and Methods for Analysis of Complex
+Data from the Brain), we propose to develop an integrative computational model utilizing single-cell and spatial
+omics data supported by experimental benchmarking, to create a new conceptual understanding of cell-typespecific
+intercellular communications and interactions in brain regions. Cell-cell communication (CCC) in the
+brain is uniquely composed of local and long-range neural communication. CCC impacts the transcriptome via
+induced signaling cascades through gene regulatory networks (GRNs). Conversely, the transcriptome impacts
+CCC via translation of the required cellular machinery for CCC. During the past four years, computational tools
+have been developed for CCC and GRN inference using nonspatial single-cell (sc) RNA-seq data, and more
+recently, some of these tools have been adopted for spatial transcriptome (ST) data. While these computational
+methods including our recently developed tools (CellChat for scRNA-seq, COMMOT for ST) are effective in
+uncovering CCC networks, nearly no studies have attempted to focus on brain-specific cell-cell communication.
+At present our very recent method NeuronChat appears to be the only and first CCC inference method directed
+specifically toward the brain. Most neural communication (synaptic communication) takes place in processes
+distal to neuronal cell bodies. Many important biological processes, which are not addressed in NeuronChat, are
+crucial to neuron communication, such as neuromodulators induced by glial communication, the ligand-receptor
+downstream GRNs, spatial connectivity, and sub-cell type specific communication. This application will address
+those gaps by developing a comprehensive neural communication inference framework utilizing scRNA-seq and
+spatial transcriptomics data. In Aim 1 we will develop an integrative multiscale model to infer brain-specific
+intercellular communications from single-cell transcriptomes. The first aim will incorporate neuromodulation into
+our inferred CCC model, followed by inference of the gene regulatory networks associated with neuron
+communication. We will infer cell type subgroups with differential projection targets and develop tools to
+systematically analyze differential communication patterns induced by neurological disorders. In Aim 2, we will
+develop an integrative framework for analysis of spatial co-locational impacts on neural communication. The
+second aim will incorporate spatial models of neuromodulation and infer spatial communication patterns within
+the brain. The proposed studies are significant because they will create the first computational model of brain
+CCC from the perspective of the transcriptome. The proposed tools will integrate multiple novel inference
+methods for neuron communication, enabling analyses in ways that were previously impossible. This work will
+connect the fundamental molecular interactions within neurons, to the complex neural circuitry which drives brain
+function.</t>
+  </si>
+  <si>
+    <t>Transcriptome; Cell Body; Benchmarking; Gene Regulatory Networks; Ligands; RNA-Seq; Single-Cell Gene Expression Analysis; Neurons; Cell Communication; Nervous System Diseases; Neurotransmitter Agents; Humans</t>
+  </si>
+  <si>
+    <t>This project aims to develop a software package for integrated analysis of cell-cell communication from singlecell
+and spatial gene expression data, including inference, interpretation, and visualization. PI Nie’s lab at UCI
+has extensive experience in developing computational methods for cell-cell communication analysis and
+collaborating with experimentalists on in-depth study of various biological systems. Nie’s lab will focus on 1)
+designing and developing user interfaces, 2) unifying various related databases such as ligand-receptor
+databases and intra-cellular pathways, and 3) develop comprehensive tutorials on applications to various
+biological systems and technologies. Cang’s lab will focus on 1) optimizing the underlying algorithms, 2)
+developing data-structures for efficient storage of cell-cell communication analysis results, and 3) visualization
+utilities. Nie’s lab and Cang’s lab will work closely to implement their cell-cell communication methods including
+CellChat and COMMOT, into python packages following a unified architecture.</t>
+  </si>
+  <si>
+    <t>Ligands; Gene Expression; Software</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3574,7 +3849,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -3593,13 +3868,23 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -3935,82 +4220,82 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" ht="21.95">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" ht="18.95">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" ht="18">
       <c r="A3" s="9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" ht="18">
       <c r="A4" s="10" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" ht="18">
       <c r="A6" s="9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" ht="18">
       <c r="A7" s="10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1">
       <c r="A8" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" ht="18.95">
       <c r="A10" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" ht="18">
       <c r="A11" s="9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" ht="18">
       <c r="A12" s="10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" ht="18">
       <c r="A13" s="10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" ht="18">
       <c r="A15" s="12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" ht="18">
       <c r="A16" s="11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="18">
       <c r="A18" s="9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2">
       <c r="B20" s="6"/>
     </row>
   </sheetData>
@@ -4027,13 +4312,13 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" s="4" t="s">
         <v>14</v>
       </c>
@@ -4041,7 +4326,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" s="4" t="s">
         <v>16</v>
       </c>
@@ -4049,7 +4334,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="32.1">
       <c r="A3" s="4" t="s">
         <v>18</v>
       </c>
@@ -4057,7 +4342,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" s="4" t="s">
         <v>20</v>
       </c>
@@ -4065,7 +4350,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5" s="4" t="s">
         <v>22</v>
       </c>
@@ -4087,23 +4372,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AF44EFF-A679-48DE-87D3-4A4765F6BA38}">
-  <dimension ref="A1:F390"/>
+  <dimension ref="A1:F412"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A285" workbookViewId="0">
-      <selection activeCell="F351" sqref="F351"/>
+    <sheetView tabSelected="1" topLeftCell="A392" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F412" sqref="F412"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="255.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="255.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -4123,7 +4408,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -4143,7 +4428,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -4163,7 +4448,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -4180,7 +4465,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>41</v>
       </c>
@@ -4197,7 +4482,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -4214,7 +4499,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -4234,7 +4519,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>49</v>
       </c>
@@ -4254,7 +4539,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>53</v>
       </c>
@@ -4274,7 +4559,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>57</v>
       </c>
@@ -4294,7 +4579,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>61</v>
       </c>
@@ -4314,7 +4599,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>64</v>
       </c>
@@ -4334,7 +4619,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>68</v>
       </c>
@@ -4354,7 +4639,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>71</v>
       </c>
@@ -4374,7 +4659,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>68</v>
       </c>
@@ -4394,7 +4679,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>76</v>
       </c>
@@ -4414,7 +4699,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>79</v>
       </c>
@@ -4434,7 +4719,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>82</v>
       </c>
@@ -4454,7 +4739,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>85</v>
       </c>
@@ -4474,7 +4759,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>88</v>
       </c>
@@ -4494,7 +4779,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>88</v>
       </c>
@@ -4514,7 +4799,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>93</v>
       </c>
@@ -4534,7 +4819,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>88</v>
       </c>
@@ -4554,7 +4839,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>98</v>
       </c>
@@ -4574,7 +4859,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
         <v>76</v>
       </c>
@@ -4594,7 +4879,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>103</v>
       </c>
@@ -4614,7 +4899,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>68</v>
       </c>
@@ -4634,7 +4919,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>107</v>
       </c>
@@ -4654,7 +4939,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>79</v>
       </c>
@@ -4674,7 +4959,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
         <v>112</v>
       </c>
@@ -4694,7 +4979,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6">
       <c r="A31" t="s">
         <v>115</v>
       </c>
@@ -4714,7 +4999,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6">
       <c r="A32" t="s">
         <v>118</v>
       </c>
@@ -4734,7 +5019,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6">
       <c r="A33" t="s">
         <v>121</v>
       </c>
@@ -4754,7 +5039,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6">
       <c r="A34" t="s">
         <v>124</v>
       </c>
@@ -4774,7 +5059,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6">
       <c r="A35" t="s">
         <v>68</v>
       </c>
@@ -4794,7 +5079,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6">
       <c r="A36" t="s">
         <v>118</v>
       </c>
@@ -4814,7 +5099,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6">
       <c r="A37" t="s">
         <v>131</v>
       </c>
@@ -4834,7 +5119,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6">
       <c r="A38" t="s">
         <v>79</v>
       </c>
@@ -4854,7 +5139,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6">
       <c r="A39" t="s">
         <v>136</v>
       </c>
@@ -4874,7 +5159,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6">
       <c r="A40" t="s">
         <v>88</v>
       </c>
@@ -4894,7 +5179,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6">
       <c r="A41" t="s">
         <v>68</v>
       </c>
@@ -4914,7 +5199,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6">
       <c r="A42" t="s">
         <v>44</v>
       </c>
@@ -4934,7 +5219,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6">
       <c r="A43" t="s">
         <v>37</v>
       </c>
@@ -4954,7 +5239,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6">
       <c r="A44" t="s">
         <v>145</v>
       </c>
@@ -4974,7 +5259,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6">
       <c r="A45" t="s">
         <v>98</v>
       </c>
@@ -4994,7 +5279,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6">
       <c r="A46" t="s">
         <v>150</v>
       </c>
@@ -5014,7 +5299,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6">
       <c r="A47" t="s">
         <v>153</v>
       </c>
@@ -5034,7 +5319,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6">
       <c r="A48" t="s">
         <v>156</v>
       </c>
@@ -5054,7 +5339,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6">
       <c r="A49" t="s">
         <v>159</v>
       </c>
@@ -5074,7 +5359,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6">
       <c r="A50" t="s">
         <v>162</v>
       </c>
@@ -5094,7 +5379,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6">
       <c r="A51" t="s">
         <v>162</v>
       </c>
@@ -5114,7 +5399,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6">
       <c r="A52" t="s">
         <v>166</v>
       </c>
@@ -5134,7 +5419,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6">
       <c r="A53" t="s">
         <v>115</v>
       </c>
@@ -5154,7 +5439,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6">
       <c r="A54" t="s">
         <v>61</v>
       </c>
@@ -5174,7 +5459,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6">
       <c r="A55" t="s">
         <v>93</v>
       </c>
@@ -5194,7 +5479,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6">
       <c r="A56" t="s">
         <v>175</v>
       </c>
@@ -5214,7 +5499,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6">
       <c r="A57" t="s">
         <v>71</v>
       </c>
@@ -5234,7 +5519,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6">
       <c r="A58" t="s">
         <v>44</v>
       </c>
@@ -5254,7 +5539,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6">
       <c r="A59" t="s">
         <v>182</v>
       </c>
@@ -5274,7 +5559,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6">
       <c r="A60" t="s">
         <v>79</v>
       </c>
@@ -5294,7 +5579,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6">
       <c r="A61" t="s">
         <v>187</v>
       </c>
@@ -5314,7 +5599,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6">
       <c r="A62" t="s">
         <v>88</v>
       </c>
@@ -5334,7 +5619,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6">
       <c r="A63" t="s">
         <v>118</v>
       </c>
@@ -5354,7 +5639,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6">
       <c r="A64" t="s">
         <v>193</v>
       </c>
@@ -5374,7 +5659,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6">
       <c r="A65" t="s">
         <v>196</v>
       </c>
@@ -5394,7 +5679,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6">
       <c r="A66" t="s">
         <v>175</v>
       </c>
@@ -5414,7 +5699,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6">
       <c r="A67" t="s">
         <v>201</v>
       </c>
@@ -5434,7 +5719,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6">
       <c r="A68" t="s">
         <v>44</v>
       </c>
@@ -5454,7 +5739,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6">
       <c r="A69" t="s">
         <v>112</v>
       </c>
@@ -5474,7 +5759,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6">
       <c r="A70" t="s">
         <v>37</v>
       </c>
@@ -5494,7 +5779,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6">
       <c r="A71" t="s">
         <v>85</v>
       </c>
@@ -5514,7 +5799,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6">
       <c r="A72" t="s">
         <v>212</v>
       </c>
@@ -5534,7 +5819,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6">
       <c r="A73" t="s">
         <v>215</v>
       </c>
@@ -5554,7 +5839,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6">
       <c r="A74" t="s">
         <v>218</v>
       </c>
@@ -5574,7 +5859,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6">
       <c r="A75" t="s">
         <v>221</v>
       </c>
@@ -5594,7 +5879,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6">
       <c r="A76" t="s">
         <v>175</v>
       </c>
@@ -5614,7 +5899,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6">
       <c r="A77" t="s">
         <v>182</v>
       </c>
@@ -5634,7 +5919,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6">
       <c r="A78" t="s">
         <v>76</v>
       </c>
@@ -5654,7 +5939,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6">
       <c r="A79" t="s">
         <v>229</v>
       </c>
@@ -5674,7 +5959,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6">
       <c r="A80" t="s">
         <v>145</v>
       </c>
@@ -5694,7 +5979,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:6">
       <c r="A81" t="s">
         <v>187</v>
       </c>
@@ -5714,7 +5999,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:6">
       <c r="A82" t="s">
         <v>34</v>
       </c>
@@ -5734,7 +6019,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:6">
       <c r="A83" t="s">
         <v>237</v>
       </c>
@@ -5754,7 +6039,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:6">
       <c r="A84" t="s">
         <v>121</v>
       </c>
@@ -5774,7 +6059,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:6">
       <c r="A85" t="s">
         <v>242</v>
       </c>
@@ -5794,7 +6079,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:6">
       <c r="A86" t="s">
         <v>175</v>
       </c>
@@ -5814,7 +6099,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:6">
       <c r="A87" t="s">
         <v>71</v>
       </c>
@@ -5834,7 +6119,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:6">
       <c r="A88" t="s">
         <v>162</v>
       </c>
@@ -5854,7 +6139,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:6">
       <c r="A89" t="s">
         <v>44</v>
       </c>
@@ -5874,7 +6159,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:6">
       <c r="A90" t="s">
         <v>251</v>
       </c>
@@ -5894,7 +6179,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:6">
       <c r="A91" t="s">
         <v>103</v>
       </c>
@@ -5914,7 +6199,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:6">
       <c r="A92" t="s">
         <v>256</v>
       </c>
@@ -5934,7 +6219,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:6">
       <c r="A93" t="s">
         <v>259</v>
       </c>
@@ -5954,7 +6239,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:6">
       <c r="A94" t="s">
         <v>215</v>
       </c>
@@ -5974,7 +6259,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:6">
       <c r="A95" t="s">
         <v>88</v>
       </c>
@@ -5994,7 +6279,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:6">
       <c r="A96" t="s">
         <v>41</v>
       </c>
@@ -6014,7 +6299,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:6">
       <c r="A97" t="s">
         <v>68</v>
       </c>
@@ -6034,7 +6319,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:6">
       <c r="A98" t="s">
         <v>269</v>
       </c>
@@ -6054,7 +6339,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:6">
       <c r="A99" t="s">
         <v>82</v>
       </c>
@@ -6074,7 +6359,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:6">
       <c r="A100" t="s">
         <v>79</v>
       </c>
@@ -6094,7 +6379,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:6">
       <c r="A101" t="s">
         <v>79</v>
       </c>
@@ -6114,7 +6399,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:6">
       <c r="A102" t="s">
         <v>118</v>
       </c>
@@ -6134,7 +6419,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:6">
       <c r="A103" t="s">
         <v>279</v>
       </c>
@@ -6154,7 +6439,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:6">
       <c r="A104" t="s">
         <v>282</v>
       </c>
@@ -6174,7 +6459,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:6">
       <c r="A105" t="s">
         <v>285</v>
       </c>
@@ -6194,7 +6479,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:6">
       <c r="A106" t="s">
         <v>162</v>
       </c>
@@ -6214,7 +6499,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:6">
       <c r="A107" t="s">
         <v>44</v>
       </c>
@@ -6234,7 +6519,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:6">
       <c r="A108" t="s">
         <v>124</v>
       </c>
@@ -6251,7 +6536,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:6">
       <c r="A109" t="s">
         <v>121</v>
       </c>
@@ -6268,7 +6553,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:6">
       <c r="A110" t="s">
         <v>294</v>
       </c>
@@ -6285,7 +6570,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:6">
       <c r="A111" t="s">
         <v>175</v>
       </c>
@@ -6302,7 +6587,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:6">
       <c r="A112" t="s">
         <v>131</v>
       </c>
@@ -6319,7 +6604,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:6">
       <c r="A113" t="s">
         <v>301</v>
       </c>
@@ -6336,7 +6621,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:6">
       <c r="A114" t="s">
         <v>304</v>
       </c>
@@ -6353,7 +6638,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:6">
       <c r="A115" t="s">
         <v>256</v>
       </c>
@@ -6370,7 +6655,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:6">
       <c r="A116" t="s">
         <v>212</v>
       </c>
@@ -6387,7 +6672,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:6">
       <c r="A117" t="s">
         <v>112</v>
       </c>
@@ -6404,7 +6689,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:6">
       <c r="A118" t="s">
         <v>85</v>
       </c>
@@ -6421,7 +6706,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:6">
       <c r="A119" t="s">
         <v>79</v>
       </c>
@@ -6438,7 +6723,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:6">
       <c r="A120" t="s">
         <v>76</v>
       </c>
@@ -6455,7 +6740,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:6">
       <c r="A121" t="s">
         <v>85</v>
       </c>
@@ -6472,7 +6757,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:6">
       <c r="A122" t="s">
         <v>107</v>
       </c>
@@ -6489,7 +6774,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:6">
       <c r="A123" t="s">
         <v>44</v>
       </c>
@@ -6506,7 +6791,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:6">
       <c r="A124" t="s">
         <v>215</v>
       </c>
@@ -6523,7 +6808,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:6">
       <c r="A125" t="s">
         <v>294</v>
       </c>
@@ -6540,7 +6825,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:6">
       <c r="A126" t="s">
         <v>68</v>
       </c>
@@ -6557,7 +6842,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:6">
       <c r="A127" t="s">
         <v>82</v>
       </c>
@@ -6574,7 +6859,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:6">
       <c r="A128" t="s">
         <v>279</v>
       </c>
@@ -6591,7 +6876,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:6">
       <c r="A129" t="s">
         <v>334</v>
       </c>
@@ -6608,7 +6893,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:6">
       <c r="A130" t="s">
         <v>282</v>
       </c>
@@ -6625,7 +6910,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:6">
       <c r="A131" t="s">
         <v>339</v>
       </c>
@@ -6642,7 +6927,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:6">
       <c r="A132" t="s">
         <v>212</v>
       </c>
@@ -6659,7 +6944,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:6">
       <c r="A133" t="s">
         <v>294</v>
       </c>
@@ -6676,7 +6961,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:6">
       <c r="A134" t="s">
         <v>182</v>
       </c>
@@ -6693,7 +6978,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:6">
       <c r="A135" t="s">
         <v>221</v>
       </c>
@@ -6710,7 +6995,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:6">
       <c r="A136" t="s">
         <v>215</v>
       </c>
@@ -6727,7 +7012,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:6">
       <c r="A137" t="s">
         <v>282</v>
       </c>
@@ -6744,7 +7029,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:6">
       <c r="A138" t="s">
         <v>76</v>
       </c>
@@ -6761,7 +7046,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:6">
       <c r="A139" t="s">
         <v>256</v>
       </c>
@@ -6778,7 +7063,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:6">
       <c r="A140" t="s">
         <v>175</v>
       </c>
@@ -6795,7 +7080,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:6">
       <c r="A141" t="s">
         <v>301</v>
       </c>
@@ -6812,7 +7097,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:6">
       <c r="A142" t="s">
         <v>107</v>
       </c>
@@ -6829,7 +7114,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:6">
       <c r="A143" t="s">
         <v>68</v>
       </c>
@@ -6846,7 +7131,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:6">
       <c r="A144" t="s">
         <v>115</v>
       </c>
@@ -6863,7 +7148,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:6">
       <c r="A145" t="s">
         <v>259</v>
       </c>
@@ -6880,7 +7165,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:6">
       <c r="A146" t="s">
         <v>150</v>
       </c>
@@ -6897,7 +7182,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:6">
       <c r="A147" t="s">
         <v>145</v>
       </c>
@@ -6914,7 +7199,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:6">
       <c r="A148" t="s">
         <v>88</v>
       </c>
@@ -6931,7 +7216,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:6">
       <c r="A149" t="s">
         <v>279</v>
       </c>
@@ -6948,7 +7233,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:6">
       <c r="A150" t="s">
         <v>49</v>
       </c>
@@ -6965,7 +7250,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:6">
       <c r="A151" t="s">
         <v>256</v>
       </c>
@@ -6982,7 +7267,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:6">
       <c r="A152" t="s">
         <v>166</v>
       </c>
@@ -6999,7 +7284,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:6">
       <c r="A153" t="s">
         <v>256</v>
       </c>
@@ -7016,7 +7301,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:6">
       <c r="A154" t="s">
         <v>103</v>
       </c>
@@ -7033,7 +7318,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:6">
       <c r="A155" t="s">
         <v>112</v>
       </c>
@@ -7050,7 +7335,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:6">
       <c r="A156" t="s">
         <v>390</v>
       </c>
@@ -7067,7 +7352,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:6">
       <c r="A157" t="s">
         <v>304</v>
       </c>
@@ -7084,7 +7369,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:6">
       <c r="A158" t="s">
         <v>156</v>
       </c>
@@ -7104,7 +7389,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:6">
       <c r="A159" t="s">
         <v>215</v>
       </c>
@@ -7121,7 +7406,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:6">
       <c r="A160" t="s">
         <v>37</v>
       </c>
@@ -7138,7 +7423,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:6">
       <c r="A161" t="s">
         <v>85</v>
       </c>
@@ -7155,7 +7440,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:6">
       <c r="A162" t="s">
         <v>118</v>
       </c>
@@ -7172,7 +7457,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:6">
       <c r="A163" t="s">
         <v>150</v>
       </c>
@@ -7189,7 +7474,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:6">
       <c r="A164" t="s">
         <v>259</v>
       </c>
@@ -7206,7 +7491,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:6">
       <c r="A165" t="s">
         <v>409</v>
       </c>
@@ -7223,7 +7508,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:6">
       <c r="A166" t="s">
         <v>269</v>
       </c>
@@ -7240,7 +7525,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:6">
       <c r="A167" t="s">
         <v>412</v>
       </c>
@@ -7257,7 +7542,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:6">
       <c r="A168" t="s">
         <v>49</v>
       </c>
@@ -7274,7 +7559,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:6">
       <c r="A169" t="s">
         <v>259</v>
       </c>
@@ -7291,7 +7576,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:6">
       <c r="A170" t="s">
         <v>339</v>
       </c>
@@ -7308,7 +7593,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:6">
       <c r="A171" t="s">
         <v>237</v>
       </c>
@@ -7325,7 +7610,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:6">
       <c r="A172" t="s">
         <v>215</v>
       </c>
@@ -7342,7 +7627,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:6">
       <c r="A173" t="s">
         <v>30</v>
       </c>
@@ -7359,7 +7644,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:6">
       <c r="A174" t="s">
         <v>41</v>
       </c>
@@ -7376,7 +7661,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:6">
       <c r="A175" t="s">
         <v>53</v>
       </c>
@@ -7393,7 +7678,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:6">
       <c r="A176" t="s">
         <v>68</v>
       </c>
@@ -7410,7 +7695,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:6">
       <c r="A177" t="s">
         <v>88</v>
       </c>
@@ -7427,7 +7712,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:6">
       <c r="A178" t="s">
         <v>435</v>
       </c>
@@ -7444,7 +7729,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:6">
       <c r="A179" t="s">
         <v>115</v>
       </c>
@@ -7461,7 +7746,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:6">
       <c r="A180" t="s">
         <v>182</v>
       </c>
@@ -7478,7 +7763,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:6">
       <c r="A181" t="s">
         <v>44</v>
       </c>
@@ -7495,7 +7780,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:6">
       <c r="A182" t="s">
         <v>44</v>
       </c>
@@ -7512,7 +7797,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:6">
       <c r="A183" t="s">
         <v>61</v>
       </c>
@@ -7529,7 +7814,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:6">
       <c r="A184" t="s">
         <v>150</v>
       </c>
@@ -7546,7 +7831,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:6">
       <c r="A185" t="s">
         <v>107</v>
       </c>
@@ -7563,7 +7848,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:6">
       <c r="A186" t="s">
         <v>215</v>
       </c>
@@ -7580,7 +7865,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:6">
       <c r="A187" t="s">
         <v>76</v>
       </c>
@@ -7597,7 +7882,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:6">
       <c r="A188" t="s">
         <v>103</v>
       </c>
@@ -7614,7 +7899,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:6">
       <c r="A189" t="s">
         <v>456</v>
       </c>
@@ -7631,7 +7916,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:6">
       <c r="A190" t="s">
         <v>459</v>
       </c>
@@ -7648,7 +7933,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:6">
       <c r="A191" t="s">
         <v>221</v>
       </c>
@@ -7665,7 +7950,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:6">
       <c r="A192" t="s">
         <v>251</v>
       </c>
@@ -7682,7 +7967,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:6">
       <c r="A193" t="s">
         <v>162</v>
       </c>
@@ -7699,7 +7984,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:6">
       <c r="A194" t="s">
         <v>150</v>
       </c>
@@ -7716,7 +8001,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:6">
       <c r="A195" t="s">
         <v>470</v>
       </c>
@@ -7733,7 +8018,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:6">
       <c r="A196" t="s">
         <v>53</v>
       </c>
@@ -7750,7 +8035,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:6">
       <c r="A197" t="s">
         <v>215</v>
       </c>
@@ -7767,7 +8052,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:6">
       <c r="A198" t="s">
         <v>98</v>
       </c>
@@ -7784,7 +8069,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:6">
       <c r="A199" t="s">
         <v>153</v>
       </c>
@@ -7801,7 +8086,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:6">
       <c r="A200" t="s">
         <v>481</v>
       </c>
@@ -7818,7 +8103,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:6">
       <c r="A201" t="s">
         <v>88</v>
       </c>
@@ -7835,7 +8120,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:6">
       <c r="A202" t="s">
         <v>285</v>
       </c>
@@ -7852,7 +8137,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:6">
       <c r="A203" t="s">
         <v>282</v>
       </c>
@@ -7869,7 +8154,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:6">
       <c r="A204" t="s">
         <v>107</v>
       </c>
@@ -7886,7 +8171,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:6">
       <c r="A205" t="s">
         <v>215</v>
       </c>
@@ -7903,7 +8188,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:6">
       <c r="A206" t="s">
         <v>304</v>
       </c>
@@ -7920,7 +8205,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:6">
       <c r="A207" t="s">
         <v>145</v>
       </c>
@@ -7937,7 +8222,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:6">
       <c r="A208" t="s">
         <v>150</v>
       </c>
@@ -7954,7 +8239,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:6">
       <c r="A209" t="s">
         <v>390</v>
       </c>
@@ -7971,7 +8256,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:6">
       <c r="A210" t="s">
         <v>212</v>
       </c>
@@ -7988,7 +8273,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:6">
       <c r="A211" t="s">
         <v>221</v>
       </c>
@@ -8005,7 +8290,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:6">
       <c r="A212" t="s">
         <v>215</v>
       </c>
@@ -8022,7 +8307,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:6">
       <c r="A213" t="s">
         <v>118</v>
       </c>
@@ -8039,7 +8324,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:6">
       <c r="A214" t="s">
         <v>215</v>
       </c>
@@ -8056,7 +8341,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:6">
       <c r="A215" t="s">
         <v>41</v>
       </c>
@@ -8073,7 +8358,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:6">
       <c r="A216" t="s">
         <v>514</v>
       </c>
@@ -8090,7 +8375,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:6">
       <c r="A217" t="s">
         <v>79</v>
       </c>
@@ -8107,7 +8392,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="218" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:6">
       <c r="A218" t="s">
         <v>519</v>
       </c>
@@ -8124,7 +8409,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:6">
       <c r="A219" t="s">
         <v>121</v>
       </c>
@@ -8141,7 +8426,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="220" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:6">
       <c r="A220" t="s">
         <v>524</v>
       </c>
@@ -8158,7 +8443,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:6">
       <c r="A221" t="s">
         <v>53</v>
       </c>
@@ -8175,7 +8460,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="222" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:6">
       <c r="A222" t="s">
         <v>88</v>
       </c>
@@ -8192,7 +8477,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="223" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:6">
       <c r="A223" t="s">
         <v>107</v>
       </c>
@@ -8209,7 +8494,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="224" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:6">
       <c r="A224" t="s">
         <v>41</v>
       </c>
@@ -8226,7 +8511,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:6">
       <c r="A225" t="s">
         <v>175</v>
       </c>
@@ -8243,7 +8528,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:6">
       <c r="A226" t="s">
         <v>237</v>
       </c>
@@ -8260,7 +8545,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:6">
       <c r="A227" t="s">
         <v>251</v>
       </c>
@@ -8277,7 +8562,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="228" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:6">
       <c r="A228" t="s">
         <v>212</v>
       </c>
@@ -8294,7 +8579,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="229" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:6">
       <c r="A229" t="s">
         <v>542</v>
       </c>
@@ -8311,7 +8596,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="230" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:6">
       <c r="A230" t="s">
         <v>37</v>
       </c>
@@ -8328,7 +8613,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="231" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:6">
       <c r="A231" t="s">
         <v>304</v>
       </c>
@@ -8345,7 +8630,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="232" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:6">
       <c r="A232" t="s">
         <v>548</v>
       </c>
@@ -8362,7 +8647,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="233" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:6">
       <c r="A233" t="s">
         <v>124</v>
       </c>
@@ -8379,7 +8664,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="234" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:6">
       <c r="A234" t="s">
         <v>412</v>
       </c>
@@ -8396,7 +8681,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="235" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:6">
       <c r="A235" t="s">
         <v>555</v>
       </c>
@@ -8413,7 +8698,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="236" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:6">
       <c r="A236" t="s">
         <v>68</v>
       </c>
@@ -8430,7 +8715,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="237" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:6">
       <c r="A237" t="s">
         <v>79</v>
       </c>
@@ -8447,7 +8732,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="238" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:6">
       <c r="A238" t="s">
         <v>118</v>
       </c>
@@ -8464,7 +8749,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="239" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:6">
       <c r="A239" t="s">
         <v>563</v>
       </c>
@@ -8481,7 +8766,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="240" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:6">
       <c r="A240" t="s">
         <v>41</v>
       </c>
@@ -8498,7 +8783,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="241" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:6">
       <c r="A241" t="s">
         <v>76</v>
       </c>
@@ -8515,7 +8800,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="242" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:6">
       <c r="A242" t="s">
         <v>145</v>
       </c>
@@ -8532,7 +8817,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="243" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:6">
       <c r="A243" t="s">
         <v>41</v>
       </c>
@@ -8549,7 +8834,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="244" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:6">
       <c r="A244" t="s">
         <v>166</v>
       </c>
@@ -8566,7 +8851,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="245" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:6">
       <c r="A245" t="s">
         <v>118</v>
       </c>
@@ -8583,7 +8868,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="246" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:6">
       <c r="A246" t="s">
         <v>115</v>
       </c>
@@ -8600,7 +8885,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="247" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:6">
       <c r="A247" t="s">
         <v>334</v>
       </c>
@@ -8617,7 +8902,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="248" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:6">
       <c r="A248" t="s">
         <v>390</v>
       </c>
@@ -8634,7 +8919,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="249" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:6">
       <c r="A249" t="s">
         <v>68</v>
       </c>
@@ -8651,7 +8936,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="250" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:6">
       <c r="A250" t="s">
         <v>118</v>
       </c>
@@ -8668,7 +8953,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="251" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:6">
       <c r="A251" t="s">
         <v>71</v>
       </c>
@@ -8685,7 +8970,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="252" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:6">
       <c r="A252" t="s">
         <v>166</v>
       </c>
@@ -8702,7 +8987,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="253" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:6">
       <c r="A253" t="s">
         <v>242</v>
       </c>
@@ -8719,7 +9004,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="254" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:6">
       <c r="A254" t="s">
         <v>187</v>
       </c>
@@ -8736,7 +9021,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="255" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:6">
       <c r="A255" t="s">
         <v>44</v>
       </c>
@@ -8753,7 +9038,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="256" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:6">
       <c r="A256" t="s">
         <v>153</v>
       </c>
@@ -8770,7 +9055,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="257" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:6">
       <c r="A257" t="s">
         <v>597</v>
       </c>
@@ -8787,7 +9072,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="258" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:6">
       <c r="A258" t="s">
         <v>124</v>
       </c>
@@ -8804,7 +9089,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="259" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:6">
       <c r="A259" t="s">
         <v>242</v>
       </c>
@@ -8821,7 +9106,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="260" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:6">
       <c r="A260" t="s">
         <v>118</v>
       </c>
@@ -8838,7 +9123,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="261" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:6">
       <c r="A261" t="s">
         <v>606</v>
       </c>
@@ -8855,7 +9140,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="262" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:6">
       <c r="A262" t="s">
         <v>44</v>
       </c>
@@ -8872,7 +9157,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="263" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:6">
       <c r="A263" t="s">
         <v>103</v>
       </c>
@@ -8889,7 +9174,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="264" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:6">
       <c r="A264" t="s">
         <v>229</v>
       </c>
@@ -8906,7 +9191,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="265" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:6">
       <c r="A265" t="s">
         <v>215</v>
       </c>
@@ -8923,7 +9208,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="266" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:6">
       <c r="A266" t="s">
         <v>88</v>
       </c>
@@ -8943,7 +9228,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="267" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:6">
       <c r="A267" t="s">
         <v>88</v>
       </c>
@@ -8963,7 +9248,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="268" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:6">
       <c r="A268" t="s">
         <v>88</v>
       </c>
@@ -8980,7 +9265,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="269" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:6">
       <c r="A269" t="s">
         <v>88</v>
       </c>
@@ -8997,7 +9282,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="270" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:6">
       <c r="A270" t="s">
         <v>187</v>
       </c>
@@ -9014,7 +9299,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="271" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:6">
       <c r="A271" t="s">
         <v>68</v>
       </c>
@@ -9031,7 +9316,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="272" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:6">
       <c r="A272" t="s">
         <v>629</v>
       </c>
@@ -9048,7 +9333,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="273" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:6">
       <c r="A273" t="s">
         <v>606</v>
       </c>
@@ -9065,7 +9350,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="274" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:6">
       <c r="A274" t="s">
         <v>159</v>
       </c>
@@ -9082,7 +9367,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="275" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:6">
       <c r="A275" t="s">
         <v>251</v>
       </c>
@@ -9099,7 +9384,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="276" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:6">
       <c r="A276" t="s">
         <v>162</v>
       </c>
@@ -9116,7 +9401,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="277" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:6">
       <c r="A277" t="s">
         <v>166</v>
       </c>
@@ -9133,7 +9418,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="278" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:6">
       <c r="A278" t="s">
         <v>294</v>
       </c>
@@ -9153,7 +9438,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="279" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:6">
       <c r="A279" t="s">
         <v>44</v>
       </c>
@@ -9170,7 +9455,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="280" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:6">
       <c r="A280" t="s">
         <v>182</v>
       </c>
@@ -9187,7 +9472,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="281" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:6">
       <c r="A281" t="s">
         <v>606</v>
       </c>
@@ -9204,7 +9489,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="282" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:6">
       <c r="A282" t="s">
         <v>44</v>
       </c>
@@ -9221,7 +9506,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="283" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:6">
       <c r="A283" t="s">
         <v>301</v>
       </c>
@@ -9238,7 +9523,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="284" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:6">
       <c r="A284" t="s">
         <v>435</v>
       </c>
@@ -9255,7 +9540,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="285" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:6">
       <c r="A285" t="s">
         <v>215</v>
       </c>
@@ -9275,7 +9560,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="286" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:6">
       <c r="A286" t="s">
         <v>215</v>
       </c>
@@ -9292,7 +9577,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="287" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:6">
       <c r="A287" t="s">
         <v>435</v>
       </c>
@@ -9312,7 +9597,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="288" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:6">
       <c r="A288" t="s">
         <v>662</v>
       </c>
@@ -9332,7 +9617,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="289" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:6">
       <c r="A289" t="s">
         <v>118</v>
       </c>
@@ -9349,7 +9634,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="290" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:6">
       <c r="A290" t="s">
         <v>269</v>
       </c>
@@ -9369,7 +9654,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="291" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:6">
       <c r="A291" t="s">
         <v>669</v>
       </c>
@@ -9389,7 +9674,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="292" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:6">
       <c r="A292" t="s">
         <v>112</v>
       </c>
@@ -9406,7 +9691,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="293" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:6">
       <c r="A293" t="s">
         <v>669</v>
       </c>
@@ -9423,7 +9708,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="294" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:6">
       <c r="A294" t="s">
         <v>256</v>
       </c>
@@ -9440,7 +9725,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="295" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:6">
       <c r="A295" t="s">
         <v>115</v>
       </c>
@@ -9460,7 +9745,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="296" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:6">
       <c r="A296" t="s">
         <v>44</v>
       </c>
@@ -9477,7 +9762,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="297" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:6">
       <c r="A297" t="s">
         <v>53</v>
       </c>
@@ -9497,7 +9782,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="298" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:6">
       <c r="A298" t="s">
         <v>44</v>
       </c>
@@ -9514,7 +9799,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="299" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:6">
       <c r="A299" t="s">
         <v>85</v>
       </c>
@@ -9534,7 +9819,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="300" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:6">
       <c r="A300" t="s">
         <v>107</v>
       </c>
@@ -9554,7 +9839,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="301" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:6">
       <c r="A301" t="s">
         <v>606</v>
       </c>
@@ -9571,7 +9856,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="302" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:6">
       <c r="A302" t="s">
         <v>269</v>
       </c>
@@ -9591,7 +9876,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="303" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:6">
       <c r="A303" t="s">
         <v>44</v>
       </c>
@@ -9611,7 +9896,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="304" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:6">
       <c r="A304" t="s">
         <v>44</v>
       </c>
@@ -9628,7 +9913,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="305" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:6">
       <c r="A305" t="s">
         <v>121</v>
       </c>
@@ -9645,7 +9930,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="306" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:6">
       <c r="A306" t="s">
         <v>339</v>
       </c>
@@ -9665,7 +9950,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="307" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:6">
       <c r="A307" t="s">
         <v>524</v>
       </c>
@@ -9685,7 +9970,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="308" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:6">
       <c r="A308" t="s">
         <v>294</v>
       </c>
@@ -9705,7 +9990,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="309" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:6">
       <c r="A309" t="s">
         <v>68</v>
       </c>
@@ -9722,7 +10007,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="310" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:6">
       <c r="A310" t="s">
         <v>524</v>
       </c>
@@ -9739,7 +10024,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="311" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:6">
       <c r="A311" t="s">
         <v>71</v>
       </c>
@@ -9759,7 +10044,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="312" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:6">
       <c r="A312" t="s">
         <v>68</v>
       </c>
@@ -9779,7 +10064,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="313" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:6">
       <c r="A313" t="s">
         <v>251</v>
       </c>
@@ -9799,7 +10084,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="314" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:6">
       <c r="A314" t="s">
         <v>150</v>
       </c>
@@ -9819,7 +10104,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="315" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:6">
       <c r="A315" t="s">
         <v>715</v>
       </c>
@@ -9839,7 +10124,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="316" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:6">
       <c r="A316" t="s">
         <v>121</v>
       </c>
@@ -9859,7 +10144,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="317" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:6">
       <c r="A317" t="s">
         <v>720</v>
       </c>
@@ -9876,7 +10161,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="318" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:6">
       <c r="A318" t="s">
         <v>41</v>
       </c>
@@ -9893,7 +10178,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="319" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:6">
       <c r="A319" t="s">
         <v>187</v>
       </c>
@@ -9910,7 +10195,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="320" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:6">
       <c r="A320" t="s">
         <v>251</v>
       </c>
@@ -9927,7 +10212,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="321" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:6">
       <c r="A321" t="s">
         <v>187</v>
       </c>
@@ -9944,7 +10229,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="322" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:6">
       <c r="A322" t="s">
         <v>112</v>
       </c>
@@ -9961,7 +10246,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="323" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:6">
       <c r="A323" t="s">
         <v>124</v>
       </c>
@@ -9978,7 +10263,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="324" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:6">
       <c r="A324" t="s">
         <v>162</v>
       </c>
@@ -9995,7 +10280,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="325" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:6">
       <c r="A325" t="s">
         <v>162</v>
       </c>
@@ -10012,7 +10297,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="326" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:6">
       <c r="A326" t="s">
         <v>44</v>
       </c>
@@ -10029,7 +10314,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="327" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:6">
       <c r="A327" t="s">
         <v>76</v>
       </c>
@@ -10046,7 +10331,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="328" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:6">
       <c r="A328" t="s">
         <v>49</v>
       </c>
@@ -10063,7 +10348,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="329" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:6">
       <c r="A329" t="s">
         <v>259</v>
       </c>
@@ -10080,7 +10365,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="330" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:6">
       <c r="A330" t="s">
         <v>542</v>
       </c>
@@ -10097,7 +10382,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="331" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:6">
       <c r="A331" t="s">
         <v>175</v>
       </c>
@@ -10114,7 +10399,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="332" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:6">
       <c r="A332" t="s">
         <v>162</v>
       </c>
@@ -10131,7 +10416,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="333" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:6">
       <c r="A333" t="s">
         <v>49</v>
       </c>
@@ -10148,7 +10433,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="334" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:6">
       <c r="A334" t="s">
         <v>752</v>
       </c>
@@ -10165,7 +10450,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="335" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:6">
       <c r="A335" t="s">
         <v>752</v>
       </c>
@@ -10182,7 +10467,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="336" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:6">
       <c r="A336" t="s">
         <v>68</v>
       </c>
@@ -10199,7 +10484,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="337" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:6">
       <c r="A337" t="s">
         <v>44</v>
       </c>
@@ -10216,7 +10501,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="338" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:6">
       <c r="A338" t="s">
         <v>41</v>
       </c>
@@ -10233,7 +10518,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="339" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:6">
       <c r="A339" t="s">
         <v>41</v>
       </c>
@@ -10250,7 +10535,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="340" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:6">
       <c r="A340" t="s">
         <v>156</v>
       </c>
@@ -10267,7 +10552,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="341" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:6">
       <c r="A341" t="s">
         <v>514</v>
       </c>
@@ -10284,7 +10569,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="342" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:6">
       <c r="A342" t="s">
         <v>514</v>
       </c>
@@ -10301,7 +10586,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="343" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:6">
       <c r="A343" t="s">
         <v>242</v>
       </c>
@@ -10318,7 +10603,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="344" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:6">
       <c r="A344" t="s">
         <v>221</v>
       </c>
@@ -10335,7 +10620,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="345" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:6">
       <c r="A345" t="s">
         <v>215</v>
       </c>
@@ -10352,7 +10637,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="346" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:6">
       <c r="A346" t="s">
         <v>88</v>
       </c>
@@ -10369,7 +10654,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="347" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:6">
       <c r="A347" t="s">
         <v>221</v>
       </c>
@@ -10386,7 +10671,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="348" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:6">
       <c r="A348" t="s">
         <v>187</v>
       </c>
@@ -10403,7 +10688,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="349" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:6">
       <c r="A349" t="s">
         <v>221</v>
       </c>
@@ -10420,7 +10705,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="350" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:6">
       <c r="A350" t="s">
         <v>71</v>
       </c>
@@ -10437,7 +10722,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="351" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:6">
       <c r="A351" t="s">
         <v>285</v>
       </c>
@@ -10454,7 +10739,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="352" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:6">
       <c r="A352" t="s">
         <v>44</v>
       </c>
@@ -10471,7 +10756,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="353" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:6">
       <c r="A353" t="s">
         <v>242</v>
       </c>
@@ -10488,7 +10773,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="354" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:6">
       <c r="A354" t="s">
         <v>175</v>
       </c>
@@ -10505,7 +10790,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="355" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:6">
       <c r="A355" t="s">
         <v>251</v>
       </c>
@@ -10522,7 +10807,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="356" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:6">
       <c r="A356" t="s">
         <v>796</v>
       </c>
@@ -10539,7 +10824,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="357" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:6">
       <c r="A357" t="s">
         <v>187</v>
       </c>
@@ -10556,7 +10841,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="358" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:6">
       <c r="A358" t="s">
         <v>801</v>
       </c>
@@ -10573,7 +10858,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="359" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:6">
       <c r="A359" t="s">
         <v>175</v>
       </c>
@@ -10590,7 +10875,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="360" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:6">
       <c r="A360" t="s">
         <v>669</v>
       </c>
@@ -10607,7 +10892,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="361" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:6">
       <c r="A361" t="s">
         <v>251</v>
       </c>
@@ -10624,7 +10909,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="362" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="362" spans="1:6">
       <c r="A362" t="s">
         <v>41</v>
       </c>
@@ -10641,7 +10926,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="363" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:6">
       <c r="A363" t="s">
         <v>606</v>
       </c>
@@ -10658,7 +10943,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="364" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="364" spans="1:6">
       <c r="A364" t="s">
         <v>242</v>
       </c>
@@ -10675,7 +10960,7 @@
         <v>814</v>
       </c>
     </row>
-    <row r="365" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:6">
       <c r="A365" t="s">
         <v>597</v>
       </c>
@@ -10692,7 +10977,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="366" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="366" spans="1:6">
       <c r="A366" t="s">
         <v>817</v>
       </c>
@@ -10709,7 +10994,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="367" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="367" spans="1:6">
       <c r="A367" t="s">
         <v>752</v>
       </c>
@@ -10726,7 +11011,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="368" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:6">
       <c r="A368" t="s">
         <v>822</v>
       </c>
@@ -10743,7 +11028,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="369" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:6">
       <c r="A369" t="s">
         <v>481</v>
       </c>
@@ -10760,7 +11045,7 @@
         <v>826</v>
       </c>
     </row>
-    <row r="370" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="370" spans="1:6">
       <c r="A370" t="s">
         <v>514</v>
       </c>
@@ -10777,7 +11062,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="371" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="371" spans="1:6">
       <c r="A371" t="s">
         <v>285</v>
       </c>
@@ -10794,7 +11079,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="372" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="372" spans="1:6">
       <c r="A372" t="s">
         <v>412</v>
       </c>
@@ -10811,7 +11096,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="373" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="373" spans="1:6">
       <c r="A373" t="s">
         <v>124</v>
       </c>
@@ -10828,7 +11113,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="374" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="374" spans="1:6">
       <c r="A374" t="s">
         <v>470</v>
       </c>
@@ -10845,7 +11130,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="375" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:6">
       <c r="A375" t="s">
         <v>606</v>
       </c>
@@ -10862,7 +11147,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="376" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="376" spans="1:6">
       <c r="A376" t="s">
         <v>715</v>
       </c>
@@ -10875,14 +11160,14 @@
       <c r="D376" s="1">
         <v>44743</v>
       </c>
-      <c r="E376" s="14" t="s">
+      <c r="E376" t="s">
         <v>839</v>
       </c>
       <c r="F376" t="s">
         <v>717</v>
       </c>
     </row>
-    <row r="377" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="377" spans="1:6">
       <c r="A377" t="s">
         <v>715</v>
       </c>
@@ -10895,14 +11180,14 @@
       <c r="D377" s="1">
         <v>44978</v>
       </c>
-      <c r="E377" s="14" t="s">
+      <c r="E377" t="s">
         <v>840</v>
       </c>
       <c r="F377" t="s">
         <v>841</v>
       </c>
     </row>
-    <row r="378" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="378" spans="1:6">
       <c r="A378" t="s">
         <v>715</v>
       </c>
@@ -10915,14 +11200,14 @@
       <c r="D378" s="1">
         <v>45266</v>
       </c>
-      <c r="E378" s="14" t="s">
+      <c r="E378" t="s">
         <v>842</v>
       </c>
       <c r="F378" t="s">
         <v>843</v>
       </c>
     </row>
-    <row r="379" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="379" spans="1:6">
       <c r="A379" t="s">
         <v>715</v>
       </c>
@@ -10935,14 +11220,14 @@
       <c r="D379" s="1">
         <v>45546</v>
       </c>
-      <c r="E379" s="14" t="s">
+      <c r="E379" t="s">
         <v>844</v>
       </c>
       <c r="F379" t="s">
         <v>845</v>
       </c>
     </row>
-    <row r="380" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="380" spans="1:6">
       <c r="A380" t="s">
         <v>846</v>
       </c>
@@ -10955,14 +11240,14 @@
       <c r="D380" s="1">
         <v>45324</v>
       </c>
-      <c r="E380" s="14" t="s">
+      <c r="E380" t="s">
         <v>847</v>
       </c>
       <c r="F380" t="s">
         <v>848</v>
       </c>
     </row>
-    <row r="381" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="381" spans="1:6">
       <c r="A381" t="s">
         <v>846</v>
       </c>
@@ -10975,14 +11260,14 @@
       <c r="D381" s="1">
         <v>45449</v>
       </c>
-      <c r="E381" s="14" t="s">
+      <c r="E381" t="s">
         <v>849</v>
       </c>
       <c r="F381" t="s">
         <v>850</v>
       </c>
     </row>
-    <row r="382" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="382" spans="1:6">
       <c r="A382" t="s">
         <v>846</v>
       </c>
@@ -10995,14 +11280,14 @@
       <c r="D382" s="1">
         <v>45495</v>
       </c>
-      <c r="E382" s="14" t="s">
+      <c r="E382" t="s">
         <v>851</v>
       </c>
       <c r="F382" t="s">
         <v>852</v>
       </c>
     </row>
-    <row r="383" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="383" spans="1:6">
       <c r="A383" t="s">
         <v>662</v>
       </c>
@@ -11015,14 +11300,14 @@
       <c r="D383" s="1">
         <v>44784</v>
       </c>
-      <c r="E383" s="14" t="s">
+      <c r="E383" t="s">
         <v>853</v>
       </c>
       <c r="F383" t="s">
         <v>664</v>
       </c>
     </row>
-    <row r="384" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="384" spans="1:6">
       <c r="A384" t="s">
         <v>662</v>
       </c>
@@ -11035,14 +11320,14 @@
       <c r="D384" s="1">
         <v>45120</v>
       </c>
-      <c r="E384" s="14" t="s">
+      <c r="E384" t="s">
         <v>854</v>
       </c>
       <c r="F384" t="s">
         <v>855</v>
       </c>
     </row>
-    <row r="385" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="385" spans="1:6">
       <c r="A385" t="s">
         <v>662</v>
       </c>
@@ -11055,14 +11340,14 @@
       <c r="D385" s="1">
         <v>45183</v>
       </c>
-      <c r="E385" s="14" t="s">
+      <c r="E385" t="s">
         <v>856</v>
       </c>
       <c r="F385" t="s">
         <v>857</v>
       </c>
     </row>
-    <row r="386" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="386" spans="1:6">
       <c r="A386" t="s">
         <v>662</v>
       </c>
@@ -11075,14 +11360,14 @@
       <c r="D386" s="1">
         <v>45237</v>
       </c>
-      <c r="E386" s="14" t="s">
+      <c r="E386" t="s">
         <v>858</v>
       </c>
       <c r="F386" t="s">
         <v>859</v>
       </c>
     </row>
-    <row r="387" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="387" spans="1:6">
       <c r="A387" t="s">
         <v>662</v>
       </c>
@@ -11095,14 +11380,14 @@
       <c r="D387" s="1">
         <v>45372</v>
       </c>
-      <c r="E387" s="14" t="s">
+      <c r="E387" t="s">
         <v>860</v>
       </c>
       <c r="F387" t="s">
         <v>861</v>
       </c>
     </row>
-    <row r="388" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="388" spans="1:6">
       <c r="A388" t="s">
         <v>662</v>
       </c>
@@ -11115,14 +11400,14 @@
       <c r="D388" s="1">
         <v>45379</v>
       </c>
-      <c r="E388" s="14" t="s">
+      <c r="E388" t="s">
         <v>862</v>
       </c>
       <c r="F388" t="s">
         <v>863</v>
       </c>
     </row>
-    <row r="389" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="389" spans="1:6">
       <c r="A389" t="s">
         <v>662</v>
       </c>
@@ -11135,14 +11420,14 @@
       <c r="D389" s="1">
         <v>45460</v>
       </c>
-      <c r="E389" s="14" t="s">
+      <c r="E389" t="s">
         <v>864</v>
       </c>
       <c r="F389" t="s">
         <v>865</v>
       </c>
     </row>
-    <row r="390" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="390" spans="1:6">
       <c r="A390" t="s">
         <v>662</v>
       </c>
@@ -11155,11 +11440,391 @@
       <c r="D390" s="1">
         <v>45637</v>
       </c>
-      <c r="E390" s="14" t="s">
+      <c r="E390" t="s">
         <v>866</v>
       </c>
       <c r="F390" t="s">
         <v>867</v>
+      </c>
+    </row>
+    <row r="391" spans="1:6">
+      <c r="A391" t="s">
+        <v>868</v>
+      </c>
+      <c r="B391">
+        <v>226060</v>
+      </c>
+      <c r="C391" t="s">
+        <v>50</v>
+      </c>
+      <c r="D391" s="1">
+        <v>44881</v>
+      </c>
+      <c r="E391" t="s">
+        <v>869</v>
+      </c>
+      <c r="F391" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="392" spans="1:6">
+      <c r="A392" t="s">
+        <v>871</v>
+      </c>
+      <c r="B392">
+        <v>232741</v>
+      </c>
+      <c r="C392" t="s">
+        <v>50</v>
+      </c>
+      <c r="D392" s="1">
+        <v>45597</v>
+      </c>
+      <c r="E392" t="s">
+        <v>872</v>
+      </c>
+      <c r="F392" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="393" spans="1:6">
+      <c r="A393" t="s">
+        <v>868</v>
+      </c>
+      <c r="B393">
+        <v>226062</v>
+      </c>
+      <c r="C393" t="s">
+        <v>50</v>
+      </c>
+      <c r="D393" s="1">
+        <v>44881</v>
+      </c>
+      <c r="E393" t="s">
+        <v>874</v>
+      </c>
+      <c r="F393" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="394" spans="1:6">
+      <c r="A394" t="s">
+        <v>876</v>
+      </c>
+      <c r="B394">
+        <v>230529</v>
+      </c>
+      <c r="C394" t="s">
+        <v>38</v>
+      </c>
+      <c r="D394" s="1">
+        <v>45364</v>
+      </c>
+      <c r="E394" t="s">
+        <v>877</v>
+      </c>
+      <c r="F394" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="395" spans="1:6">
+      <c r="A395" t="s">
+        <v>879</v>
+      </c>
+      <c r="B395">
+        <v>231213</v>
+      </c>
+      <c r="C395" t="s">
+        <v>38</v>
+      </c>
+      <c r="D395" s="1">
+        <v>45457</v>
+      </c>
+      <c r="E395" t="s">
+        <v>880</v>
+      </c>
+      <c r="F395" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="396" spans="1:6">
+      <c r="A396" t="s">
+        <v>882</v>
+      </c>
+      <c r="B396">
+        <v>231416</v>
+      </c>
+      <c r="C396" t="s">
+        <v>38</v>
+      </c>
+      <c r="D396" s="1">
+        <v>45461</v>
+      </c>
+      <c r="E396" t="s">
+        <v>883</v>
+      </c>
+      <c r="F396" t="s">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="397" spans="1:6">
+      <c r="A397" t="s">
+        <v>882</v>
+      </c>
+      <c r="B397">
+        <v>231500</v>
+      </c>
+      <c r="C397" t="s">
+        <v>38</v>
+      </c>
+      <c r="D397" s="1">
+        <v>45470</v>
+      </c>
+      <c r="E397" t="s">
+        <v>885</v>
+      </c>
+      <c r="F397" t="s">
+        <v>886</v>
+      </c>
+    </row>
+    <row r="398" spans="1:6">
+      <c r="A398" t="s">
+        <v>879</v>
+      </c>
+      <c r="B398">
+        <v>223894</v>
+      </c>
+      <c r="C398" t="s">
+        <v>38</v>
+      </c>
+      <c r="E398" t="s">
+        <v>887</v>
+      </c>
+      <c r="F398" t="s">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="399" spans="1:6">
+      <c r="A399" t="s">
+        <v>882</v>
+      </c>
+      <c r="B399">
+        <v>223926</v>
+      </c>
+      <c r="C399" t="s">
+        <v>38</v>
+      </c>
+      <c r="E399" t="s">
+        <v>889</v>
+      </c>
+      <c r="F399" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="400" spans="1:6">
+      <c r="A400" t="s">
+        <v>61</v>
+      </c>
+      <c r="B400">
+        <v>224084</v>
+      </c>
+      <c r="C400" t="s">
+        <v>38</v>
+      </c>
+      <c r="E400" t="s">
+        <v>891</v>
+      </c>
+      <c r="F400" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="401" spans="1:6">
+      <c r="A401" t="s">
+        <v>61</v>
+      </c>
+      <c r="B401">
+        <v>224496</v>
+      </c>
+      <c r="C401" t="s">
+        <v>38</v>
+      </c>
+      <c r="E401" t="s">
+        <v>893</v>
+      </c>
+      <c r="F401" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="402" spans="1:6">
+      <c r="A402" t="s">
+        <v>882</v>
+      </c>
+      <c r="B402">
+        <v>225915</v>
+      </c>
+      <c r="C402" t="s">
+        <v>38</v>
+      </c>
+      <c r="E402" t="s">
+        <v>895</v>
+      </c>
+      <c r="F402" t="s">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="403" spans="1:6">
+      <c r="A403" t="s">
+        <v>882</v>
+      </c>
+      <c r="B403">
+        <v>228052</v>
+      </c>
+      <c r="C403" t="s">
+        <v>38</v>
+      </c>
+      <c r="E403" t="s">
+        <v>897</v>
+      </c>
+      <c r="F403" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="404" spans="1:6">
+      <c r="A404" t="s">
+        <v>61</v>
+      </c>
+      <c r="B404">
+        <v>228284</v>
+      </c>
+      <c r="C404" t="s">
+        <v>38</v>
+      </c>
+      <c r="E404" t="s">
+        <v>899</v>
+      </c>
+      <c r="F404" t="s">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="405" spans="1:6">
+      <c r="A405" t="s">
+        <v>876</v>
+      </c>
+      <c r="B405">
+        <v>228316</v>
+      </c>
+      <c r="C405" t="s">
+        <v>38</v>
+      </c>
+      <c r="E405" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="406" spans="1:6">
+      <c r="A406" t="s">
+        <v>882</v>
+      </c>
+      <c r="B406">
+        <v>228994</v>
+      </c>
+      <c r="C406" t="s">
+        <v>38</v>
+      </c>
+      <c r="E406" t="s">
+        <v>902</v>
+      </c>
+      <c r="F406" t="s">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="407" spans="1:6">
+      <c r="A407" t="s">
+        <v>904</v>
+      </c>
+      <c r="B407">
+        <v>229245</v>
+      </c>
+      <c r="C407" t="s">
+        <v>38</v>
+      </c>
+      <c r="E407" t="s">
+        <v>905</v>
+      </c>
+      <c r="F407" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="408" spans="1:6">
+      <c r="A408" t="s">
+        <v>907</v>
+      </c>
+      <c r="B408">
+        <v>230169</v>
+      </c>
+      <c r="C408" t="s">
+        <v>38</v>
+      </c>
+      <c r="E408" t="s">
+        <v>908</v>
+      </c>
+      <c r="F408" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="409" spans="1:6">
+      <c r="A409" t="s">
+        <v>910</v>
+      </c>
+      <c r="C409" t="s">
+        <v>50</v>
+      </c>
+      <c r="E409" t="s">
+        <v>911</v>
+      </c>
+      <c r="F409" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="410" spans="1:6">
+      <c r="A410" t="s">
+        <v>910</v>
+      </c>
+      <c r="C410" t="s">
+        <v>50</v>
+      </c>
+      <c r="E410" t="s">
+        <v>913</v>
+      </c>
+      <c r="F410" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="411" spans="1:6">
+      <c r="A411" t="s">
+        <v>910</v>
+      </c>
+      <c r="C411" t="s">
+        <v>50</v>
+      </c>
+      <c r="E411" t="s">
+        <v>915</v>
+      </c>
+      <c r="F411" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="412" spans="1:6">
+      <c r="A412" t="s">
+        <v>910</v>
+      </c>
+      <c r="C412" t="s">
+        <v>50</v>
+      </c>
+      <c r="E412" t="s">
+        <v>917</v>
+      </c>
+      <c r="F412" t="s">
+        <v>918</v>
       </c>
     </row>
   </sheetData>
@@ -11168,17 +11833,24 @@
       <sortCondition descending="1" ref="D1:D107"/>
     </sortState>
   </autoFilter>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Notes xmlns="b238fc39-fcbb-4f8c-bfd3-e3a789f7784e" xsi:nil="true"/>
+    <ProjectRole xmlns="b238fc39-fcbb-4f8c-bfd3-e3a789f7784e" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b238fc39-fcbb-4f8c-bfd3-e3a789f7784e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="ccd2e96c-ba06-41a4-9d14-ee5d4767a409" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11456,58 +12128,22 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Notes xmlns="b238fc39-fcbb-4f8c-bfd3-e3a789f7784e" xsi:nil="true"/>
-    <ProjectRole xmlns="b238fc39-fcbb-4f8c-bfd3-e3a789f7784e" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b238fc39-fcbb-4f8c-bfd3-e3a789f7784e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="ccd2e96c-ba06-41a4-9d14-ee5d4767a409" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{89D1C6ED-834C-4B9D-827C-3A00957FB85E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3F88ABE-1F09-4246-805E-5B35215270F6}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B9E692F-2B0F-42AD-B3D3-6C71619FC4A6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="ccd2e96c-ba06-41a4-9d14-ee5d4767a409"/>
-    <ds:schemaRef ds:uri="b238fc39-fcbb-4f8c-bfd3-e3a789f7784e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B9E692F-2B0F-42AD-B3D3-6C71619FC4A6}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3F88ABE-1F09-4246-805E-5B35215270F6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b238fc39-fcbb-4f8c-bfd3-e3a789f7784e"/>
-    <ds:schemaRef ds:uri="ccd2e96c-ba06-41a4-9d14-ee5d4767a409"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{89D1C6ED-834C-4B9D-827C-3A00957FB85E}"/>
 </file>
</xml_diff>

<commit_message>
reran bipython with new abstracts
</commit_message>
<xml_diff>
--- a/Faculty_Proposal_Abstracts.xlsx
+++ b/Faculty_Proposal_Abstracts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28706"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28715"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ucirvine.sharepoint.com/sites/BioSci-Contracts&amp;Grants-Team/Shared Documents/BioSci Research Development/Faculty-Keyword-Inventory-Project/faculty-mapped-mesh-terms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2962" documentId="11_D808F5E3348CBFB07090EECA229B558F1A7CE9CF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC3DA726-BCDB-420B-AC82-CF6DE0290F4C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F7CDAC22-A568-417D-88C5-50B69D3D0963}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="-3100" windowWidth="38400" windowHeight="21100" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pre-Award README" sheetId="6" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1675" uniqueCount="919">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1807" uniqueCount="974">
   <si>
     <t>Instructions for Adding Proposals to Spreadsheet</t>
   </si>
@@ -3726,6 +3726,398 @@
   </si>
   <si>
     <t>Ligands; Gene Expression; Software</t>
+  </si>
+  <si>
+    <t>Background: Provide Biological/Technological significance and rationale for the project. 
+Biogen has 2 active TREM2 programs, but currently no validated biomarkers that can be used to confirm the appropriate modulation of human microglia. This presents a challenge for assessing the degree of TREM2 activation and therefore makes it impossible to estimate target engagement and efficacy. The Blurton-Jones lab is one of only 2 labs who have developed and perfected the use of chimeric mouse models of AD that enable functional and transcriptomic studies of human microglia in vivo. This model utilizes engraftment of human induced pluripotent stem cell (iPSC)-derived microglia into the forebrain of xenotransplantation-compatible Alzheimer’s Disease (AD) transgenic mice to examine the interactions between human microglia and amyloid pathology and the impact of therapeutic interventions on human microglial activity, function, and gene expression.  
+Proposal Goal: Examine the effects of TREM2-stimulating antibodies on human microglial gene expression, cytokine production, DAM-markers, beta-amyloid plaque pathology, and dystrophic neurites in hCSF1-5XFAD chimeric mice.</t>
+  </si>
+  <si>
+    <t>Humans; Mice; Animals; Mice, Transgenic; Induced Pluripotent Stem Cells; Microglia; Plaque, Amyloid; Alzheimer Disease; Goals; Neurites; Transplantation, Heterologous; Gene Expression Profiling; Amyloidogenic Proteins; Transcriptome; Biomarkers; Prosencephalon; Cytokines</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Relevance of Conference to CIRM Mission
+Rare diseases represent a tremendous burden to society with one in 10 Americans suffering from one of 7,000 identified indications, 90% of which have no treatment. Research on patient stem cells represent an exciting avenue for the development of new drugs for rare diseases. One of the critical bottlenecks to developing medicines for rare diseases, however, is dialogue with the patient community. How do we put the patients’/caregivers’ unmet needs and personal experiences front-and-center in the development of new medicines, including drug development, clinical trial design and recruitment procedures, when the patient population is small? 
+Rare disease advocacy foundations provide critical networks to connect patients and caregivers to clinical research and development. We need creative new avenues for engagement, education to fuel research and raise awareness.  We want to inform patients deeply about the current state of research while providing them with opportunities to directly participate.  In this conference, we propose to bring together critical stakeholders for the ALSP community: patients and physicians, patient advocates, industry and academic disease researchers and connect them under CIRM’s co-sponsorship to accelerate the development of cellular medicines for rare disease. 
+This conference entitled “Insights and Potential of Cell-Based Therapies for the Treatment of Leukodystrophies” represents a unique partnership between a CIRM funded center for stem cell research at UCI and an emerging global patient advocacy group (Sisters’ Hope) focused on a recently recognized rare and fatal genetic disease of the brain’s white matter. Adult-onset leukoencephalopathy with axonal spheroids and pigmented glia (ALSP) is a devastating neurological disorder dominated by white matter involvement and caused by heterozygous mutations in the Colony Stimulating Factor 1 Receptor (CSF1R) gene. CSF1R is involved in microglia development and maintenance. Hence, ALSP is also known as CSF1R-related leukoencephalopathy and considered a primary microgliopathy. Since the causal role of CSF1R-mutations was discovered only in 2011, the disease is still underdiagnosed, with important repercussions on patients and their families. Much is unknown about disease progression and its underlying mechanisms.
+Patients and caregivers report that the lack of knowledge on the disease and the limited access to experts presents a major challenge. For this reason, the proposed conference will be crucial to connecting patients and families with specialists on the disease. The research on leukodystrophies such as ALSP is still at its early stages and the role of CSF1R-mutated microglia needs to be clarified. This is a limiting step to understand the pathophysiology of the disease and foresee therapeutic strategies. The goal of the conference is to launch a conversation among stakeholders about the lessons learned with better characterized leukodystrophies to better chart the optimal path for developing a cell-based approach to ALSP.
+The proposed conference will be held at the CIRM supported Stem Cell Research Center at the University of California, Irvine and will be co-organized by Sisters’ Hope Foundation and UC Irvine. By combining scientific talks, patient and caregiver presentations, we expect the conference to consolidate the connection between patients and specialists, increasing awareness on ALSP, and building a strong sense of community. 
+The ALSP Community Conference will serve as an opportunity to help organize the Sisters’ Hope Foundation’s community of &gt;50 US based ALSP patients. We estimate attendance of approximately 10 individuals carrying the CSF1R mutation and congenic controls. If successful, we envision more conference events hosted at UCI and at other sites to grow the community and provide future opportunities for direct participation in research.
+</t>
+  </si>
+  <si>
+    <t>Humans; Adult; Caregivers; Macrophage Colony-Stimulating Factor; Patient Advocacy; Rare Diseases; Stem Cell Research; White Matter; Goals; Microglia; Social Cohesion; Nervous System Diseases; Nervous System Malformations; Disease Progression; Mutation; Drug Development; Physicians</t>
+  </si>
+  <si>
+    <t>3. Introduction and background Genome wide association studies (GWAS) have identified numerous loci that are associated with altered risk of developing Alzheimer’s Disease (AD). Further examination of expression quantitative trait loci (eQTL), functional fine mapping, and mechanistic studies have collectively shown that many of these GWAS risk loci are associated with genes that are highly or even specifically expressed by myeloid cells. As AD is a neurological disorder and changes in microglial morphology, number, and function have been well described, we and many others have hypothesized that GWAS signals are likely mediated via alterations in microglial gene expression and function. As the major brain-resident myeloid cell, genetically influenced differences in microglial function likely contribute substantially to AD risk. Indeed, coding mutations in several microglial expressed genes including TREM2, PILRA, ABI3, and PLCG2 further support this hypothesis. Howe ve r, a growing body of e vidence sugge sts that other pe riphe rally de rive d mye loid ce lls and periphe ral inflammation also affect the deve lopme nt and progre ssion of AD via both indire ct and direct e ffects on the brain. Our newly reformulated Neuroimmune Consortium (NIC) will therefore employ highly collaborative and cutting-edge approaches to investigate the contributions of peripheral immune cells and peripheral inflammation to the development and progression of AD and to identify the mechanisms that underlie these peripherally mediated effects. Inflammation contributes to the development or progression of virtually every human disease. While the brain is considered immune privileged, a growing body of evidence has shown that peripheral inflammation can influence the development of Parkinson’s disease, Multiple Sclerosis, Frontotemporal Dementia, and AD. Yet the mechanisms and cell types that mediate these effects remain unclear. While peripheral inflammation can arise from a variety of conditions including viral, bacterial, or fungal infections, liver disease, obesity, diabetes, and autoimmune disease, accurately modeling these inflammatory conditions in mice can be extremely challenging and often provides highly variable results. For example, a mouse model of C9ORF72-mediated frontotemporal dementia was shown to exhibit highly differing mortality and disease progression in response to differing housing conditions and microbial burden Burberry, 2020 #1}. An alternative and highly reproducible approach to model peripheral inflammation instead employees the intraperitoneal injection of the bacterial toxin Lipopolysaccharide (LPS). Importantly, the effects of LPS on brain are indirect as LPS fails to cross the blood brain barrier{Banks, 2010 #3}. In addition, the effects of LPS are mediated via TLR4 signaling, a receptor that is highly expressed by peripheral monocytes and macrophages, cells that express many of the same candidate GWAS genes as microglia.</t>
+  </si>
+  <si>
+    <t>Humans; Animals; Mice; Quantitative Trait Loci; Genome-Wide Association Study; Lipopolysaccharides; Microglia; Blood-Brain Barrier; Toll-Like Receptor 4; Multiple Sclerosis; Frontotemporal Dementia; Injections, Intraperitoneal; Alzheimer Disease; C9orf72 Protein; Housing Quality; Monocytes; Parkinson Disease; Brain; Myeloid Cells; Liver Diseases; Macrophages; Mycoses; Mutation; Disease Progression; Gene Expression; Diabetes Mellitus; Obesity</t>
+  </si>
+  <si>
+    <t>UCI Blurton-Jones Lab Scope of Work The overarching goal of this project is to determine the impact of tau mutations on human microglial function and to determine whether microglial-expressed tau influences the development and progression of Frontotemporal Dementia (FTD). As MPI of this proposal, Dr. Blurton-Jones' group will work closely with Dr. Karch and her team on all aspects of the proposed studies. The Blurton-Jones lab has expertise with the generation and use of induced pluripotent stem cell-derived microglia (iMG) and the subsequent transplantation of iMGs into mice to generate chimeric mouse models of Alzheimer’s Disease, aging, and FTD. In Aim 1, we will assist Dr. Karch and her lab in the analysis of the cell intrinsic defects that occur in human iMGs that express FTD-associated mutations in tau (MAPT gene). Isogenic iPSC lines will be examined including the IVS10+16 mutation that increases 4R tau splicing and several MAPT coding mutations; R5H, P301L, P301S, V337M, G389R, R406W, IVS9-10 and isogenic controls. Aim 1 will specifically examine the impact of these tau mutations on human microglia transcriptional states, cytoskeletal organization, phagocytosis, cytokine production, and TREM2 signaling. We will also determine the impact of mutant iMG on neuronal health and function in co-culture systems. Aim 2 will then be led by the Blurton-Jones lab and utilize our hCSF1 and PS19-hCSF1 chimeric mouse models to examine the impact of MAPT mutations on microglia function and the interactions between mutant microglia and neuronal tau pathology in vivo. For each of these experiments we will continue to discuss the design, progress, and interpretation with Dr. Karch and her colleagues as detailed in our MPI plan. In addition, both labs will work closely together to write and submit all progress reports and manuscripts detailing our findings.</t>
+  </si>
+  <si>
+    <t>Humans; Female; Animals; Mice; Research Report; Frontotemporal Dementia; Microglia; Induced Pluripotent Stem Cells; Alzheimer Disease; Coculture Techniques; Goals; Pick Disease of the Brain; Mutation; Cytokines</t>
+  </si>
+  <si>
+    <t>Donovan, Peter</t>
+  </si>
+  <si>
+    <t>PROJECT SUMMARY In the 21st century it has become clear that many of the major problems facing humanity will need to be addressed by biologists carrying out biomedical research. In order for the US biomedical research community to succeed in combating the major challenges facing our world, scientists will have to operate with high efficiency and develop solutions to many different unique problems. A broad number of studies have now concluded that teams and organizations that are diverse and inclusive are more successful at these endeavors. Moreover, if public funding is to be used to support biomedical research, in order for it to be equitable, it should allow access to students from all backgrounds and represent the diversity in the US population. Success as a scientist requires more than just skill at a lab bench and there are special barriers facing students from underrepresented groups. Therefore, our comprehensive approach will implement (1) enhanced educational and research outreach to minority-serving institutions, (2) recruitment activities to help students transition to our university, (3) advanced start activities to help students transition readily to the next stage in their training, (4) coursework and activities that are relevant to their underserved communities and themselves, (5) faculty- AND peer-mentoring support, coupled with culturally-aware mentor training, (6) UCI research and collaboration visit opportunities for their prior undergraduate mentors who likely inspired them to enter graduate school, (7) funding to support an annual ”reconnection” visit to their alumni institution and community, (8) funding for them to attend conferences, such as SACNAS, ABRCMS and SfN, and (9) training in oral and written communication and leadership skills. Taken together, these opportunities will prepare students for careers inside and outside academia and will advance the NIH goals of enhancing biomedical research in the context of health and human services as a whole.</t>
+  </si>
+  <si>
+    <t>Humans; Mentors; Mentoring; Universities; Leadership; Academia; Goals; Personnel Selection; Students; Faculty; Communication</t>
+  </si>
+  <si>
+    <t>Abstract: X-linked dystonia Parkinsonism (XDP), like other neurodegenerative diseases has clear genetic causation. But like other diseases, the consequence of gene disruption in XDP is not clear. Recent studies suggest that disruption of the general transcription factor, TAF1, might explain the XDP phenotype. We propose a new and innovative theory about how such mutations affect neuronal health. We propose that disruption of genes like TAF1 causes cellular stress and in turn can activate transposable elements (TEs). In other organisms, where TEs are more easily studied, TEs are activated by stress. Indeed, some mammalian TEs (including the short interspersed nuclear elements (SINEs)) are activated by stress. However, a previous review of this proposal led to the question of whether TAF1 itself might directly regulate the transcription of TEs. Another critique was that, if this research indeed shows that TEs might be upregulated in XDP neurons, how might that knowledge lead to potential treatments for XDP. One reviewer noted that inhibitors of some TEs, especially the long-interspersed nuclear elements (LINEs) are available. Therefore, our experiments are now focused on these two major questions. Does TAF1 directly or indirectly regulate expression of TEs and could suppression of TEs, especially the autonomous LINE elements, lead to improvement of neuronal health in XDP patients. TE activation can result in production of TE-derived proteins and RNAs that could affect neuronal function. Our hypothesis is that disruption of the TAF1 gene in XDP patients leads to TE hyperactivation which then affects neuronal health.</t>
+  </si>
+  <si>
+    <t>Humans; Animals; DNA Transposable Elements; Dystonia; Neurodegenerative Diseases; Mutation; Neurons; Parkinsonian Disorders</t>
+  </si>
+  <si>
+    <t>Inlay, Matthew</t>
+  </si>
+  <si>
+    <t>PROJECT SUMMARY Hematopoietic cell transplantation (HCT), also known as blood and marrow transplantation (BMT) is a life-saving procedure that can replace a diseased patient’s blood system with a healthy one from a donor. A major complication to HCT is the development of Graft-versus-Host Disease (GvHD). In GvHD, donor immune cells contained in the graft recognize the host patient’s cells as foreign, and mount a systemic inflammatory response leading to tissue damage, morbidity, and often death. This is known as allogeneic activation, and is instigated by differences in human leukocyte antigen (HLA) genes between donor and patient. Patients suffering from GvHD require powerful immunosuppressive drugs, including glucocorticoids (GCs), to prevent symptoms which can compromise their health and immunity. The risk of GvHD has limited the use of HCT, and prevented the expansion of the donor pool to include haploidentical donors, which include most siblings and all parents. This underscores an urgent need to develop treatments and strategies to prevent GvHD to expand the use of HCT. The long-term goal of this research team is to develop new strategies for improving the safety and efficacy of HCT. To that end, this proposal focuses on a novel strategy to treat the donor cells prior to transplantation, to reduce the immunosuppression given to the patients. The preliminary data reveals that pretreatment of donor cells with the glucocorticoid fluticasone propionate (better known as FLU) can not only reduce allogeneic immune cell activation in a mouse model of GvHD, but also improves HCT engraftment. Based on the finding that a class of immune cells called conventional T cells are suppressed by FLU, while tolerance-inducing regulatory T cells (Tregs) are spared, the central hypothesis of this research proposal is that FLU reduces GvHD by increasing the ratio of tolerogenic Tregs to alloreactive conventional T cells. The overall objective of this proposal is to test this hypothesis by examining the impact of Tregs and conventional T cell activation and response in GvHD after pre-treatment with FLU. The rationale for this project is to establish the mechanism by which GC pre-treatment reduces GVHD in mice, so that a GC pre-treatment strategy that achieves the same effect can be tested in humans. This hypothesis will be tested through two specific aims: 1) To determine whether Tregs are necessary for FLU induced reduction of GVHD. 2) To determine if apoptosis of conventional T cells is necessary for FLU induced reduction of GVHD. The research proposed in this application is conceptually innovative, in the applicant’s opinion, because it represents a substantive departure from the status quo by focusing on treating the donor cells prior to transplantation, rather giving patient’s the immunosuppressive drugs. The research is technically innovative because it employs high dimensional marker analysis using cutting-edge mass cytometry, to examine FLU’s impact on the T cell response in a broader manner not available with traditional methods. The proposed research is significant because it could provide proof-of-principle evidence to lay the groundwork for the design and evaluation of future strategies to treat donor cells with glucocorticoids prior to transplantation to reduce GvHD and thereby expand the donor pool to haploidentical donors, which could greatly benefit patients suffering from blood disorders that could be potentially cured by HCT.</t>
+  </si>
+  <si>
+    <t>Humans; Animals; Mice; Glucocorticoids; Fluticasone; Research Design; T-Lymphocytes, Regulatory; Siblings; Bone Marrow; Goals; Preliminary Data; Immunosuppression Therapy; Graft vs Host Disease; Tissue Donors; Apoptosis; Hematopoietic Stem Cell Transplantation; HLA Antigens; Parents; Systemic Inflammatory Response Syndrome</t>
+  </si>
+  <si>
+    <t>PROJECT SUMMARY Hematopoietic cell transplantation (HCT), also known as blood and marrow transplantation (BMT) is a life-saving procedure that can replace a diseased patient’s blood system with a healthy one from a donor. A major complication to HCT is the development of Graft-versus-Host Disease (GvHD). In GvHD, donor immune cells contained in the graft recognize the host patient’s cells as foreign, and mount a systemic inflammatory response leading to tissue damage, morbidity, and often death. This is known as allogeneic activation, and is instigated by differences in human leukocyte antigen (HLA) genes between donor and patient. Patients suffering from GvHD require powerful immunosuppressive drugs to treat symptoms, including glucocorticoids (GCs), which have side effects that can compromise their health and immunity. The risk of GvHD has limited the use of HCT, and prevented the expansion of the donor pool to include haploidentical donors, which include most siblings and all parents. This underscores an urgent need to develop treatments and strategies to prevent GvHD to expand the use of HCT. The long-term goal of this research team is to develop new strategies for improving the safety and efficacy of HCT. To that end, this proposal focuses on a novel strategy to treat the donor cells prior to transplantation, to reshape the immune response and reduce the amount of immunosuppressive drugs given directly to the patients. The preliminary data reveals that pretreatment of donor cells with the glucocorticoid fluticasone propionate (FLU) reduces allogeneic immune cell activation in a mouse model of GvHD, and also improves HCT engraftment. The data also shows the FLU results in the apoptosis of class of immune cells called conventional T cells (Tconv), but spares tolerance-inducing regulatory T cells (Tregs), resulting in an increase in Tregs:Tconv that may lead to tolerance. The overall objective of this research proposal is to identify combinations of GCs (and other compounds) that can produce a similar effect on human T cells in culture, and to functionally test these combinations in a human-mouse xenograft GvHD model. The rationale is that by first demonstrating these effects in human cells, progress can be made towards a clinical trial to develop a GC pre-treatment strategy to reduce GvHD in patients receiving allo-HCT. The research proposed in this application is conceptually innovative, in the applicant’s opinion, because it represents a substantive departure from the status quo by focusing on treating the donor cells prior to transplantation, rather giving patients the immunosuppressive drugs. The proposed research is significant because it could provide proof-ofprinciple evidence to lay the groundwork for the design and evaluation of future strategies to treat donor cells with glucocorticoids prior to transplantation to reduce GvHD and thereby expand the donor pool to haplo-identical donors, which could greatly benefit patients suffering from blood disorders that could be potentially cured by HCT.</t>
+  </si>
+  <si>
+    <t>PROJECT SUMMARY Hematopoietic cell transplantation (HCT), also known as blood and marrow transplantation (BMT), is a life-saving procedure that can replace a diseased patient’s blood system with a healthy one from a donor. However, a major complication of HCT is the development of Graft-versus-Host Disease (GvHD). In GvHD, donor immune cells contained in the graft recognize the host patient’s cells as foreign and mount a systemic inflammatory response leading to tissue damage, morbidity, and often death. This is known as allogeneic activation and is instigated by differences in human leukocyte antigen (HLA) genes between donor and patient. Patients suffering from GvHD require powerful immunosuppressive drugs, including glucocorticoids (GCs), to prevent symptoms that can compromise their health and immunity. The risk of GvHD has limited the use of HCT and prevented the expansion of the donor pool to include haploidentical donors, which include most siblings and all parents. This underscores an urgent need to develop treatments and strategies to prevent GvHD to expand the use of HCT. The long-term goal of this research team is to develop new strategies for improving the safety and efficacy of HCT. To that end, this proposal focuses on a novel approach to treat the donor cells before transplantation to reduce the immunosuppression given to the patients. The preliminary data reveals that pretreatment of donor cells with the glucocorticoid fluticasone propionate (FLU) can reduce allogeneic immune cell activation in a mouse model of GvHD but also improves HCT engraftment. Based on the finding that a class of immune cells called conventional T cells are suppressed by FLU. In contrast, tolerance-inducing regulatory T cells (Tregs) are spared; the central hypothesis of this research proposal is that FLU reduces GvHD by increasing the ratio of tolerogenic Tregs to alloreactive conventional T cells in the graft. The overall objective of this proposal is to expand on this hypothesis by testing whether further increasing the Treg: Tconv ratio will result in an additional reduction of GvHD and testing the ability of FLU-treated grafts to engage in an anti-cancer response. The rationale for this project is to establish the potential of this strategy to treat GvHD while allowing an anti-cancer response to progress this research to human cells. The research proposed in this application is conceptually innovative, in the applicants’ opinion, because it represents a substantive departure from the status quo by focusing on conditioning the donor graft before transplantation, as opposed to treating the patients with immunosuppressive drugs. Furthermore, the proposed research is significant because it could provide proof-of-principle evidence to lay the groundwork for designing and evaluating future strategies to treat human donor cells with glucocorticoids before transplantation to reduce GvHD. This could expand the donor pool to haploidentical donors, which could greatly benefit patients suffering from blood disorders that HCT could potentially cure.</t>
+  </si>
+  <si>
+    <t>PROJECT SUMMARY Hematopoietic cell transplantation (HCT), also known as blood and marrow transplantation (BMT) is a life-saving procedure that can replace a diseased patient’s blood system with a healthy one from a donor. A major complication to HCT is the development of Graft-versus-Host Disease (GvHD). In GvHD, donor immune cells contained in the graft recognize the host patient’s cells as foreign, and mount a systemic inflammatory response leading to tissue damage, morbidity, and often death. This is known as allogeneic activation, and is instigated by differences in human leukocyte antigen (HLA) genes between donor and patient. Patients suffering from GvHD require powerful immunosuppressive drugs to treat symptoms, including glucocorticoids (GCs), which have side effects that can compromise their health and immunity. This underscores an urgent need to develop treatments and strategies to prevent GvHD to expand the use of HCT. The long-term goal of this research team is to develop new strategies for improving the safety and efficacy of HCT. To that end, this proposal focuses on a novel strategy called graft conditioning, whereby donor cells are treated with compounds prior to transplantation, to reshape the immune response and reduce the amount of immunosuppressive drugs given directly to the patients. The study team’s recent publication reveals that pretreatment of donor cells with the glucocorticoid fluticasone propionate (FLU) reduces allogeneic immune cell activation in a mouse model of GvHD, and also improves HCT engraftment (PMID: 37538042). The data also shows the FLU results in the apoptosis of a class of immune cells called conventional T cells (Tcon), but spares tolerance-inducing regulatory T cells (Tregs), resulting in an increase in Tregs:Tcons that may lead to tolerance. The overall objective of this research proposal is to identify combinations compounds, including GCs, BCL2 inhibitors, cytokines, and mTOR inhibitors, that can produce a similar effect on human T cells in culture, and to functionally test these combinations in a human-mouse xenograft GvHD model. The rationale is that by first demonstrating these effects in human cells, progress can be made towards a clinical trial to develop a graft conditioning strategy to reduce GvHD in patients receiving allo-HCT. The research proposed in this application is conceptually innovative, in the applicant’s opinion, because it represents a substantive departure from the status quo by focusing on treating the donor cells prior to transplantation, rather giving patients the immunosuppressive drugs. The proposed research is significant because it could provide proof-of-principle evidence to lay the groundwork for the design and evaluation of future strategies to treat donor cells with glucocorticoids prior to transplantation to reduce GvHD and thereby expand the donor pool to haplo-identical donors, which could greatly benefit patients suffering from blood disorders that could be potentially cured by HCT. PROJECT SUMMARY Hematopoietic cell transplantation (HCT), also known as blood and marrow transplantation (BMT), is a life-saving procedure that can replace a diseased patient’s blood system with a healthy one from a donor. However, a major complication of HCT is the development of Graft-versus-Host Disease (GvHD). In GvHD, donor immune cells contained in the graft recognize the host patient’s cells as foreign and mount a systemic inflammatory response leading to tissue damage, morbidity, and often death. This is known as allogeneic activation and is instigated by differences in human leukocyte antigen (HLA) genes between donor and patient. Patients suffering from GvHD require powerful immunosuppressive drugs, including glucocorticoids (GCs), to prevent symptoms that can compromise their health and immunity. The risk of GvHD has limited the use of HCT and prevented the expansion of the donor pool to include haploidentical donors, which include most siblings and all parents. This underscores an urgent need to develop treatments and strategies to prevent GvHD to expand the use of HCT. The long-term goal of this research team is to develop new strategies for improving the safety and efficacy of HCT. To that end, this proposal focuses on a novel approach to treat the donor cells before transplantation to reduce the immunosuppression given to the patients. The preliminary data reveals that pretreatment of donor cells with the glucocorticoid fluticasone propionate (FLU) can reduce allogeneic immune cell activation in a mouse model of GvHD but also improves HCT engraftment. Based on the finding that a class of immune cells called conventional T cells are suppressed by FLU. In contrast, tolerance-inducing regulatory T cells (Tregs) are spared; the central hypothesis of this research proposal is that FLU reduces GvHD by increasing the ratio of tolerogenic Tregs to alloreactive conventional T cells in the graft. The overall objective of this proposal is to expand on this hypothesis by testing whether further increasing the Treg: Tconv ratio will result in an additional reduction of GvHD and testing the ability of FLU-treated grafts to engage in an anti-cancer response. The rationale for this project is to establish the potential of this strategy to treat GvHD while allowing an anti-cancer response to progress this research to human cells. The research proposed in this application is conceptually innovative, in the applicants’ opinion, because it represents a substantive departure from the status quo by focusing on conditioning the donor graft before transplantation, as opposed to treating the patients with immunosuppressive drugs. Furthermore, the proposed research is significant because it could provide proof-of-principle evidence to lay the groundwork for designing and evaluating future strategies to treat human donor cells with glucocorticoids before transplantation to reduce GvHD. This could expand the donor pool to haploidentical donors, which could greatly benefit patients suffering from blood disorders that HCT could potentially cure.</t>
+  </si>
+  <si>
+    <t>PROJECT SUMMARY Hematopoietic cell transplantation (HCT), also known as blood and marrow transplantation (BMT) is a life-saving procedure that can replace a diseased patient’s blood system with a healthy one from a donor. A major complication to HCT is the development of Graft-versus-Host Disease (GVHD). In GVHD, donor immune cells contained in the graft recognize the host patient’s cells as foreign, and mount a systemic inflammatory response leading to tissue damage, morbidity, and often death. This is known as allogeneic activation, and is instigated by differences in human leukocyte antigen (HLA) genes between donor and patient. Patients suffering from GVHD require powerful immunosuppressive drugs, including glucocorticoids (GCs), to prevent symptoms which can compromise their health and immunity. Post-transplant cyclophosphamide (PTCY) is a procedure to inject high dose cyclophosphamide shortly after HCT, and has shown great potential in reducing GVHD severity, so much so that individuals that are partially matched to patients (haploidentical) can be used effectively as donors. Despite this progress, the risk of GVHD remains, and cyclophosphamide can have powerful side effects and leave patients with increased susceptibility to infections. Thus, new strategies are needed to improve further reduce GVHD and other complications that result from HCT, to better improve the survival of patients receiving this therapy. The long-term goal of this research team is to develop new strategies for improving the safety and efficacy of HCT. To that end, this proposal focuses on a novel strategy called “graft conditioning before transplantation” or GCBT. In GCBT, the donor grafts are treated outside the body with drugs and compounds to reshape the immune response. These drugs and compounds are not given to the patients. The preliminary data reveals that a combination of compounds including the glucocorticoid fluticasone propionate (FLU), the BCL2 inhibitor Venetoclax (VEN), and the cytokine IL2, are uniquely capable of removing immune cells that cause GVHD, while sparing stem cells and the immune cells important for tolerance. The overall objective of this proposal is to compare GCBT with PTCY in a mouse model to determine if GCBT, either alone or in combination with PTCY is able to better protect recipient mice from GVHD, and whether the immune cells are able to engage in an anti-cancer response. The rationale for this project is to establish the potential of GCBT to treat GvHD while allowing an anti-cancer response, in order to progress this research to human cells. The research proposed in this application is conceptually innovative, in the applicants’ opinion, because it represents a substantive departure from the status quo by focusing on conditioning the donor graft prior to transplantation, as opposed to treating the patients with immunosuppressive drugs. The proposed research is significant because it could provide proof-ofprinciple evidence to lay the groundwork for the design and evaluation of future strategies to treat human donor cells with glucocorticoids prior to transplantation to reduce GvHD. This could in turn expand the donor pool to haplo-identical donors, which could greatly benefit patients suffering from blood disorders that could be potentially cured by HCT.</t>
+  </si>
+  <si>
+    <t>How will the proposed candidate impact an unmet medical need?
+Post-transplant cyclophosphamide (PTCY) has emerged as the gold standard prophylactic treatment for
+graft-versus-host disease (GVHD) in allogeneic hematopoietic stem cell transplantation (allo-HSCT). By
+injecting CY into graft recipients shortly after transplantation (days 3 and 4), donor immune cells that are
+allogeneically activated immediately after transplantation and rapidly proliferating, will be specifically
+targeted and destroyed by CY, sparing non-alloreactive immune cells and hematopoietic stem cells
+(HSCs). PTCY has reduced the incidence and severity of GVHD, which has allowed the use of
+haploidentical donors when fully matched donors are unavailable, greatly expanding the donor pool.
+However, GVHD incidence still remains at approximately 20%, and one year survival rates are still well
+below 50% for many diseases (refs). In addition, CY is highly toxic, and can cause adverse side effects.
+Thus, there remains a critical unmet need to improve upon PTCY and currently prophylactic strategies to
+reduce GVHD, complications due to PTCY, and disease relapse.
+How will this project lead to or aid in the development of therapies that could improve patient care?
+Our proposal seeks to utilize a window of opportunity to manipulate the donor immune repertoire after
+collection but prior to transplantation. By treating grafts during this window, the compounds needed to
+manipulate the immune response are not given directly to patients, potentially avoiding any toxic or
+unintended side effects these compounds may cause. By treating the grafts in the collection bags, the
+sterility of the grafts is maintained, potentially avoiding logistical complications and delays that may occur
+if a GMP facility is required to process the grafts. This method could be combined with PTCY or existing
+prophylactic strategies, or possibly reduce the amount of drugs given directly to the patient.
+Beyond advancing a candidate, does the proposed research have the potential to provide new insights
+that could advance regenerative medicine?
+Other methods of manipulating grafts outside the body include depletion of T cells using antibodies, or
+sorting of T cell populations by magnetic or flow cytometry to reduce conventional T cells and increase
+Tregs. While valuable, these strategies are primarily a cell enrichment or depletion approach. Our focus
+on treating the grafts with compounds that have a variety of effects can achieve similar enrichment/
+depletion effects, but has the potential to alter the graft in additional ways. For example, treatment of
+cord blood HSCs with glucocorticoids can increase CXCR4 expression and lead to increase bone marrow
+homing in xenograft transplantation. IL2 can stimulate Tregs. If successful, our strategy could be
+expanded upon by others seeking to use different compounds to manipulate the graft cells in different
+ways prior to transplantation.
+How does the proposed research distinguish itself from current and alternative approaches?
+Our main focus is on conditioning the grafts between the time when they are collected from a donor and
+when they are transplanted into a patient. This window allows us to experiment with compounds or
+combinations of compounds that might be considered too toxic for testing in a patient. PTCY, while
+incredibly successful and an important advance in GVHD prevention, requires injection of CY into patients
+which can have toxic side effects. PTCY does not eliminate GVHD entirely, but reduces it to a level such
+that haploidentical transplantation becomes feasible from a safety perspective. Disease relapse after
+PTCY can be further improved. Our strategy could be combined with PTCY or to eventually reduce the
+dose of CY necessary to give to patients. While other methods for manipulating grafts outside the patient
+exist, such as antibody based depletion of T cells, cell sorting, or ex vivo expansion of Tregs, many of
+these strategies require extensive manipulation outside the body, and require a GMP facility and/or a
+lengthy incubation period. Our approach focuses on conditioning the graft while minimizing the time
+between collection and delivery, and doing so while avoiding exposing the grafts to potential contamination that would necessitate processing in a GMP facility.
+How do you envision the progression from successful candidate discovery to translation?
+Our preliminary data will show a potential drug combination that combines the glucocorticoid
+prednisolone, the BCL2 inhibitor venetoclax, and the cytokine IL2, to reduce conventional T cells and
+increase the percentage of Tregs in human peripheral blood mononuclear cells (PBMCs) to 15% of total
+CD4 T cells. This percentage may by itself be sufficient to move forward, but the purpose of this proposal
+is to identify a combination of compounds that can achieve a Treg percentage approaching 50%, in as
+short a culture time as possible. We can already achieve this in mouse models in a 6 hour culture in a
+completely closed system. We intend to demonstrate the combination can reduce GVHD in a xenograft
+model, while still eliminating tumors in a xeno-GVL model. By the end of the funding period, we envision
+having a final cocktail and conditioning protocol, and demonstrating success on real patient grafts
+cultured in an apheresis bag. Our next steps would be apply for a TRAN1 grant to perform additional
+tests using a GMP facility (at the UCI campus) and develop a quality control assay based on the ratios of
+conventional T cells to Tregs to quickly identify whether a conditioned graft would be suitable for
+transplantation. In addition, to further develop a protocol to condition grafts without removing the cells
+from the apheresis bags or breaking sterility. Once we can achieve consistency with either a GMP
+dependent or independent approach, we intend to perform a clinical trial on patients suffering from
+aplastic anemia, which require allo-HSCT but does not depend on a strong GVL approach. If successful,
+we would then attempt this strategy on patients with blood cancers.</t>
+  </si>
+  <si>
+    <t>Humans; Animals; Mice; Glucocorticoids; Pharmaceutical Preparations; Prednisolone; venetoclax; Interleukin-2; Bone Marrow; Anemia, Aplastic; Transplantation, Heterologous; Flow Cytometry; Cytokines; CD4-Positive T-Lymphocytes; Transplantation, Haploidentical; Fetal Blood; Heterografts; Incidence; Leukocytes, Mononuclear; Preliminary Data; Regenerative Medicine; Survival Rate; T-Lymphocytes, Regulatory; Patient Care; Neoplasms; Blood Component Removal; Graft vs Host Disease; Hematologic Neoplasms; Hematopoietic Stem Cells; Hematopoietic Stem Cell Transplantation; Cyclophosphamide; Tissue Donors; Drug Combinations; Immunity; Infertility; Magnetic Phenomena; Proto-Oncogene Proteins c-bcl-2</t>
+  </si>
+  <si>
+    <t>PROJECT SUMMARY Hematopoietic cell transplantation (HCT), also known as blood and marrow transplantation (BMT) is a life-saving procedure that can replace a diseased patient’s blood system with a healthy one from a donor. A major complication to HCT is the development of Graft-versus-Host Disease (GVHD). In GVHD, donor immune cells contained in the graft recognize the host patient’s cells as foreign, and mount a systemic inflammatory response leading to tissue damage, morbidity, and often death. This is known as allogeneic activation, and is instigated by differences in human leukocyte antigen (HLA) genes between donor and patient. Patients receiving an allogeneic HCT (allo-HCT), often require powerful immunosuppressants to prevent or treat GVHD, which have side effects that can compromise their health and immunity. This underscores an urgent need to develop new treatments and strategies to reduce the drug burden needed to prevent or reduce GVHD in allo-HCT patients. The long-term goal of this research team is to develop new strategies for improving the safety and efficacy of HCT. To that end, this proposal focuses on a novel strategy called graft conditioning, whereby donor cells are treated with a combination of compounds prior to transplantation, to reshape the immune response and reduce the amount of immunosuppressive drugs given directly to the patients. The study team’s recent publication reveals that pretreatment of donor cells with the glucocorticoid fluticasone propionate (FLU) reduces allogeneic immune cell activation in a mouse model of GVHD, and also improves HCT engraftment (PMID: 37538042). The data also shows the FLU results in the apoptosis of a class of immune cells called conventional T cells (Tcon), but spares tolerance-inducing regulatory T cells (Tregs), resulting in an increase in Tregs:Tcons that may lead to tolerance. The overall objective of this research proposal is to test a graft conditioning protocol on human immune cells, to determine if they can reduce or prevent GVHD when transplanted into immunodeficient mice. The second goal of this proposal to test this graft conditioning protocol on its ability to mediate a graft-versus-leukemia (GVL) response, an important anti-cancer benefit of allo-HCT. The rationale is that by first demonstrating these effects in human cells, progress can be made towards a clinical trial to develop a graft conditioning strategy to reduce GVHD in patients receiving allo-HCT. The research proposed in this application is conceptually innovative, in the applicants’ opinion, because it represents a substantive departure from the status quo by focusing on treating the donor cells prior to transplantation, rather giving patients the immunosuppressive drugs. The proposed research is significant because it could provide proof-of-principle evidence to lay the groundwork for the design and evaluation of future strategies to treat donor cells with glucocorticoids prior to transplantation to reduce GvHD and thereby expand the donor pool to haplo-identical donors, which could greatly benefit patients suffering from blood disorders that could be potentially cured by HCT.</t>
+  </si>
+  <si>
+    <t>Abstract:
+This network will build human skin cell atlas spanning three developmentally, anatomically, and physiologically
+distinct body sites. A collaborative effort by a team of experts from the University of California, Irvine and the
+University of Michigan, this network will explore ancestral differences in skin cell states across African American,
+Hispanic, Middle Eastern and Asian populations. Building on expertise in skin biology, skin disease, single-cell
+biology, and support by two NIH-funded Skin Biology and Disease Resource Centers, the network will define
+skin complexity by analyzing gene expression and gene regulatory states in all skin cell types and will initiate
+mapping of these features across body sites.
+Skin diseases often have disproportionate effects in different ethnic groups; their manifestations are also
+commonly body location specific. These differences likely relate to ancestral influences on the underlying normal
+skin cell states. Differences in skin pigmentation, epidermal thickness, hair density, texture and pigmentation are
+ancestrally linked to disease susceptibility, yet related epithelial, mesenchymal, pigment and immune cell
+features remain unknown. To help explain ancestral differences in skin biology and pathology, the network will
+generate comprehensive skin cell atlas through single-cell genomic approach on 72 adults, ages 18 years and
+above, and will archive skin samples for future multiomic and spatial transcriptomics studies.
+The network will engage the community in the project. In consultation with a community engagement advisory
+board, the network will use a variety of approaches, including community engagement studios, to ensure
+fairness, obtain feedback, and disseminate information to the community.</t>
+  </si>
+  <si>
+    <t>Humans; Adult; Skin Pigmentation; Black or African American; Feedback; Disease Susceptibility; Ethnicity; Multiomics; Skin Diseases; Genomics; Hispanic or Latino; Gene Expression Profiling; Referral and Consultation; Gene Expression; Hair</t>
+  </si>
+  <si>
+    <t>Project Summary/Abstract
+Synthetic lethality screens hold great promise for cancer therapy since they enable the identification of
+chemical compounds that selectively target tumor cells while sparing normal tissue. This approach presumes
+that cancer cells harboring a specific mutation will be more sensitive to manipulation of certain pathways than
+normal cells that lack the mutation. The von Hippel-Lindau (VHL) tumor-suppressor gene is functionally lost in
+about 90% of Clear Cell Renal Cell Carcinomas (ccRCCs). Because VHL-deficient ccRCCs resist current
+therapies and frequently metastasize, identifying effective new therapies will be crucial for achieving longlasting responses. This project’s long-term goal is to therapeutically target VHL-deficient ccRCCs using a
+synthetic lethality approach, and to move the most promising therapeutics to clinical trials. Here we propose
+to investigate cyclin-dependent kinase (CDK) inhibitors as synthetic lethality-based therapeutics for targeting
+ccRCC. We have validated a multi-CDK inhibitor—Dinaciclib—as a therapeutic candidate with potent in vivo
+activity in a patient-derived xenograft (PDX)-based orthotopic mouse model of ccRCC. Our preliminary data
+indicate that several specific CDK9 inhibitors (CDK9i)—AZD4573, NVP-2, and KB-0742—mimic Dinaciclibinduced death of VHL-deficient cells in vitro. CDK9 represents a promising therapeutic target since: (1) it is a
+non-canonical CDK regulating RNA polymerase II-mediated transcription; (2) multiple CDK9i have been
+developed, with several undergoing clinical trials in cancers other than ccRCC. Accordingly, our goal is to
+evaluate AZD4573 as a potential therapeutic for ccRCC. Our objectives are to dissect the mechanism of
+synthetic lethality in vitro, and assess AZD4573 efficacy in vivo, including its effects on anti-tumor immunity.
+We propose the following Specific Aims: 1) Dissect the mechanism of synthetic lethality of CDK9 inhibition
+with VHL loss in vitro, where we will test the hypothesis that there is a cross-talk between VHL and CDK9
+pathways, affecting each other’s activity. We will also test the involvement of several candidate pathways
+downstream of CDK9 (MCL-1 and Bfl-1 pro-survival proteins) and VHL (HIF-1 and HIF-2) in synthetic lethality
+to determine the biomarkers of tumor response; and 2) Evaluate CDK inhibitor AZD4573 as a potential
+therapeutic in an orthotopic PDX-based and immunocompetent models of ccRCC, the latter conducted in
+combination with immune checkpoint inhibitor (ICI)—anti-PD1. ICIs represent a current front-line treatment for
+ccRCC, and literature indicates that CDK inhibition by Dinaciclib and a specific CDK9i induce anti-tumor
+immunity, potentiating their anti-tumor effects. Accordingly, our working hypothesis is that CDK9i will slow the
+tumor growth in immunodeficient model and cause tumor regression in immunocompetent model, especially
+when combined with ICI. Successful completion of the experimental plan will provide an efficient therapeutic
+strategy for VHL-deficient ccRCC—CDK9i + ICI combination treatment. Dissecting the mechanism of synthetic
+lethality will allow for patient stratification into potential responders and non-responders.</t>
+  </si>
+  <si>
+    <t>Humans; Animals; Mice; Carcinoma, Renal Cell; dinaciclib; Immune Checkpoint Inhibitors; Myeloid Cell Leukemia Sequence 1 Protein; RNA Polymerase II; Synthetic Lethal Mutations; Genes, Suppressor; Goals; Heterografts; Preliminary Data; Biomarkers; Cyclin-Dependent Kinases; Basic Helix-Loop-Helix Transcription Factors</t>
+  </si>
+  <si>
+    <t>Project Summary/Abstract
+Up to 39,000 women are diagnosed with triple-negative type of breast cancer (TNBC) yearly in US, with a survival rate of only 12% for metastatic patients. While there are effective treatment options for localized tumors, there remains a strong need to better understand molecular events leading to spreading of the tumor to distant sites to develop effective therapies for patients with metastatic breast cancer. We have identified CUB-domain containing protein 1 (CDCP1) to be overexpressed and drive TNBC metastasis in vivo. Its expression also negatively correlates with survival of basal-like breast cancer patients. Our data further show that CDCP1 activates Src kinase, which translocates to the mitochondria, where it promotes oxidative phosphorylation (OxPhos), fueling TNBC migration. Moreover, we could restore OxPhos in CDCP1 knockdown cells by overexpressing constitutively active mitochondria-targeted Src. Importantly, OxPhos is a top transcription signature that distinguishes TNBC metastatic lesions from the primary tumors, and is a driver of metastasis and therapeutic resistance in TNBC animal models. The goal of this proposal is to define the molecular events and components that mediate the metastasis-promoting activity of CDCP1, focusing on CDCP1-activated mitochondrial Src family kinases (SFKs). Our central hypothesis is that CDCP1/mitochondrial-SFK/electron transport chain pathway promotes OxPhos driving TNBC metastasis when oxygen is available. Here we will pursue the following Specific Aims: 1) Dissect the mechanism of Src translocation to mitochondria and its regulation by hypoxia, focusing on Tomm/Timm translocation system responsible for 90% of transport, and accessory protein AKAP1 known to anchor Src to mitochondrial surface; 2) Determine the mitochondrial SFK substrates upregulating CDCP1-mediated OxPhos; 3) Evaluate CDCP1/mitochondrial-SFK pathway in TNBC metastasis in vivo, including the impact of this pathway on OxPhos in vivo, as measured by phasor approach to fluorescent lifetime imaging microscopy (FLIM). Our findings will apply to 30% of TNBC patients since we have shown activity of the CDCP1/SFK pathway in 30% of patient primary tumor specimens. These three complementary Aims will help us to understand the mechanism of metabolic dysregulation of TNBC stimulating metastasis and therapeutic resistance. The results will advance the current trends in therapeutic development involving OxPhos inhibitors, novel Src inhibitors with greater specificity, and possibilities of small molecule delivery to mitochondria in vivo, accompanied by the search for biomarkers of therapeutic response.</t>
+  </si>
+  <si>
+    <t>Humans; Female; Animals; Oxidative Phosphorylation; Oxygen; Microscopy; Survival Rate; Drug Resistance, Neoplasm; Electron Transport; Goals; Triple Negative Breast Neoplasms; Mitochondria; Hypoxia; Biomarkers</t>
+  </si>
+  <si>
+    <t>Scientific Summary of Project:
+Clear Cell Renal Cell Carcinoma (ccRCC) remains one of the deadliest forms of kidney cancer. The recent front-line therapeutic combination consisting of a receptor tyrosine kinase inhibitor and an immune checkpoint inhibitor (ICI) represents a significant improvement over the previous regimens, but achieves only 16% complete response rate. Likewise, novel hypoxia-inducible factor 2 (HIF2) inhibitor—belzutifan—shows a lot of promise, but acquired drug resistance seems inevitable. Our overarching goal is to develop effective therapeutics specifically targeting ccRCC and sparing the normal tissue, thus ensuring the therapeutic window. The specificity towards ccRCC will be achieved by synthetic lethality approach. Since 90% of ccRCC tumors are driven by the loss of the von Hippel-Lindau (VHL) tumor suppressor, we have conducted a synthetic lethality screen selecting small molecules selectively killing VHLdeficient ccRCC and sparing VHL-expressing cells, including normal cells. My laboratory has validated several compounds (see our recent publications) and gearing one of the compounds towards clinical trials. Despite these successes, we recognize that the in vitro systems we and others use for discovery of synthetic lethality interactions are not ideal since the tumor microenvironment is not factored in. The in vivo systems currently in use rely on genetic manipulation of the cells prior to implantation into mice, which still does not put cells into the right microenvironment, and actually puts them into stress of transition from tissue culture to avascular microenvironment. Here I propose to implant VHL-expressing ccRCC cells transduced with CRISPR/Cas9 library, grow tumors, and then turn off VHL expression in an established tumor by using a VHL expression construct repressed by tetracycline. 786-O ccRCC cells have been reported to form tumors both in their original VHL-deficient state, and when VHL has been re-expressed. Accordingly, my Aim is to set up the in vivo system with Tetracycline-Off (Tet-Off) VHL for indirect CRISPR/Cas9 screening of vulnerabilities of VHL-deficient cancer cells. Successful completion of the experimental plan will provide hits for validation, which will represent potential therapeutic targets for VHL-deficient ccRCC. The broader impact is the adaptation of the set up system to other tumor suppressor loss driven cancers.</t>
+  </si>
+  <si>
+    <t>Animals; Mice; Carcinoma, Renal Cell; endothelial PAS domain-containing protein 1; Immune Checkpoint Inhibitors; Tyrosine Kinase Inhibitors; Tumor Microenvironment; belzutifan; CRISPR-Cas Systems; Goals; Synthetic Lethal Mutations; Kidney Neoplasms; Tetracyclines</t>
+  </si>
+  <si>
+    <t>Project Summary
+Up to 39,000 women are diagnosed with triple-negative type of breast cancer (TNBC) yearly in US, with a survival rate of only 12% for metastatic patients. Thus, novel therapeutic strategies are urgently needed. Recently, several studies, including our own, have established oxidative phosphorylation (OxPhos) as a driver of metastasis in TNBC. To achieve a therapeutic window, we propose to target a cancer-specific OxPhos-driving pathway in stratified patients. We established CUB-domain containing protein 1 (CDCP1) as a potent inducer of OxPhos, which acts through activation of Src in mitochondria. Our central First Name Rebecca E-mail rtyler1@uci.edu City Irvine State CA Address University of California, Irvine Office of Research 160 Aldrich Hall Irvine, CA 92697-7600 hypothesis is that CDCP1/mitochondrial-Src/electron transport chain pathway induces OxPhos driving TNBC metastasis. Our Specific Aims are: 1) Identify biomarkers of elevated OxPhos in TNBC based on phosphorylation of the mitochondrial Src substrates (compatible with immunohistochemistry) and 2) Evaluate the impact of blocking mitochondrial Src activity on OxPhos and TNBC metastasis. If successful, these two complementary aims will establish biomarkers of high Src-driven OxPhos in TNBC and justify mitochondrial Src as a cancer-specific target to reduce OxPhos and metastasis. These aims are expected to deliver the basis for patient stratification and testing of novel Src inhibitors for TNBC treatment, possibly with mitochondrial delivery of the inhibitors. This research plan aligns well with our long-term goal to develop targeted therapeutics for TNBC, reducing normal tissue toxicity and improving survival rates.</t>
+  </si>
+  <si>
+    <t>PROJECT SUMMARY
+Stem cell medicine promises to revolutionize the treatment of human diseases and injuries, and has captured
+the hopes of the scientific community and the public alike. Perhaps nowhere is the potential of stem cells to
+treat human disease and injury more promising than for neurologic disorders. Traveling a path from “bench to
+bedside” is still a relatively new opportunity for researchers and provides novel challenges for training graduate
+students. Historically, pre-doctoral neuroscience students were trained in understanding the basic biological
+mechanisms underlying how the brain functions and guides behavior, learning and memory, movement, and to
+identify the processes that become dysregulated and result in neurological disease. Indeed, the biological
+mechanisms and causes for many neurological diseases have been identified, paving the way for the
+generation of transgenic animals and model systems to study neurological disorders. Critically, these
+advances, combined with the advent of stem cell biology, open a path to treat neurologic diseases with
+transplantation of stem cell derived cell populations or to develop treatment strategies in stem-cell derived cell
+models. This is a path that requires training beyond basic science. Accordingly, the goal of our Training
+Program in Stem Cell Translational Medicine for Neurological Disorders is to provide opportunities for
+pre-doctoral trainees to perform translational "bench" research that could treat human neurological disease
+and injury, in the spirit of the NIH vision for translational medicine. Additionally however, to meet the challenges
+presented by the advent of this new frontier, we provide opportunities for trainees in the clinical aspects of the
+disease they are studying. These opportunities enable identification of therapeutic targets with the greatest
+relevance to human disease, inform preclinical safety and efficacy testing, and define preclinical outcome
+measures that parallel clinical metrics. Furthermore, this program familiarizes trainees with the complexities of
+the regulatory processes required for human clinical trials and the business of taking research products to
+patients. A novel, and highly successful, aspect of the training is coaching in communication, conflict
+resolution, interpersonal and group interactions skills. These skills are important both for success in working in
+interdisciplinary teams and for helping in the success and retention of underrepresented minority students.
+Taken together, these opportunities will prepare students for careers inside and outside academia and will
+advance the NIH goals of enhancing biomedical research in the context of health and human services as a
+whole. The program we have implemented thus fills a significant training gap in the translational application of
+stem cell biology to neurological disorders, not typically met by traditional neurobiology, stem cell or clinical
+graduate programs.</t>
+  </si>
+  <si>
+    <t>Humans; Animals; Mentoring; Animals, Genetically Modified; Goals; Neurobiology; Negotiating; Academia; Translational Science, Biomedical; Students; Biomedical Research; Nervous System Diseases; Outcome Assessment, Health Care; Brain</t>
+  </si>
+  <si>
+    <t>Identify disease targets and perturbagens that modulate XDP-disease phenotypes with robotic microscopy and OMICS in human in vitro XDP cell models X-Linked Dystonia-Parkinsonism (XDP) is caused by a SINE-VNTR-Alu (SVA) retrotransposon insertion into the TBPassociated factor 1 (TAF1) gene reducing its transcription and leading to dysfunction and degeneration of medium spiny neurons (MSNs). Despite understanding the genetic cause of disease, a molecular understanding of MSN degeneration is lacking. During our previous grant period, we identified genes and proteins differentially expressed in XDP hiPSC-derived MSNs as potential therapeutic targets and laid groundwork for a screening platform to evaluate potential therapeutic targets using robotic microscopy (RM) and OMICS analysis. Here, we expand this work with a CRISPRi screen to evaluate a focused set of potential therapeutic targets to alleviate disease phenotypes using RM and transcriptomic approaches.</t>
+  </si>
+  <si>
+    <t>Humans; Dystonia 3, Torsion, X-Linked; Retroelements; Induced Pluripotent Stem Cells; Medium Spiny Neurons; Microscopy; Robotic Surgical Procedures; Gene Expression Profiling</t>
+  </si>
+  <si>
+    <t>An effective treatment for any genetic neurodegenerative disease depends on the comprehensive understanding of the causative disease protein functions and the disruption of those functions in the presence of disease-causing mutations. Huntington’s disease (HD) is a devastating genetically inherited neurodegenerative disease typically striking individuals in midlife and progressing over 15-20 years before patients succumb to disease [1]. There are also juvenile cases of the disease. Symptoms include uncontrolled movements that increase in severity over time, cognitive decline leading to difficulties with daily tasks and psychiatric manifestations including depression and dementia. Current FDA approved HD treatments are strictly palliative and cannot delay onset or slow the inevitable disease progression. Given the relatively slow progression of HD, the costs of care- giving stretch over 10 or more years after the patient loses independence, having a profound financial and emotional impact on families and health systems. In the US, &gt;30,000 people have HD and ~150,000 have a 50% chance of developing the disease. The cost for HD in the US is estimated to be $2.5 billion/year, including the costs of care for the patient and the loss of income for the patient and their families (Personal communication, HDSA). HD clinicians in California commonly encounter HD patients who are homeless, incarcerated, need prolonged hospitalization awaiting placement, or require long-term psychiatric placement. As the disease progresses, patients become dependent on family and caregivers, who in turn have a huge burden managing the physical, cognitive and psychiatric manifestations of HD.
+HTT is essential for normal cellular functions and serves as a critical scaffold for cellular protein interactions. It is ubiquitously expressed in human cells and is a required protein for brain function in general. However, the mutation selectively affects distinct regions and cell types of the brain. mHTT causes selective degeneration of medium spiny neurons (MSNs) in the striatum and atrophy of the cortex, but other areas such as cerebellum are preserved. Further, mHTT causes dysregulation of non-neuronal cells of the brain—astrocytes (cells that provide support to the neurons) and microglia (the immune cells of the brain). HD is also associated with dysfunction of tissues outside of the brain including the heart and the gut. There is a current gap in knowledge about cell-type specific functions of HTT, including the consequences of mHTT throughout human tissues. The selective vulnerability of specific neuronal populations and the distinct pathways altered in non-neuronal cell types by the presence of the HD mutation suggests cell-type specificity in HTT function and in mHTT’s ability to disrupt those functions. Understanding these fundamental differences will shed insights into the mechanisms by which mHTT drives disease pathology and inform future therapeutic strategies. The approach will also provide insight into the critical role of normal HTT function that may be important to disease mechanisms underlying more common neurodegenerative diseases.</t>
+  </si>
+  <si>
+    <t>Humans; Microglia; Astrocytes; Caregivers; Depression; Medium Spiny Neurons; Neurodegenerative Diseases; Neurons; Brain; Cerebellum; Atrophy; Cognitive Dysfunction; Hospitalization; Prisoners; Cognition; Dementia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The conference will focus on key challenges in surgical delivery, immunosuppression and clinical trial design for viral-based therapies and stem cell-derived products for Huntington’s disease (HD) that can advance CIRM’s mission to deliver transformative regenerative medicine treatments in an equitable manner.  The meeting is an extension of our original Stem Cells for Huntington’s Disease (SC4HD) meeting funded by CIRM in 2018.  This network brings together experts in stem cell biology, viral therapies, stem cell transplantation, HD, industry, surgical interventions and delivery and clinical trial design to accelerate the progression of viral and stem cell-based therapies to clinical therapy and build upon the expertise of the different groups. Over the last decade there have been major advances in understanding the pathogenic processes underlying HD, some of which have progressed to clinical trials.  Importantly, many of the most promising emerging therapies to date use Advanced Therapeutic Medicinal Products (ATMPs), which involve direct manipulation of genes or RNA, or delivery of cells to achieve tissue repair.   A small number of gene therapy products are now in early phase trials, and the biology of stem cells as a donor cell source for HD has advanced considerably and is approaching the point of first-in-man studies. However, there are many clinical translational challenges to address. Many of these challenges are common to gene and cell therapies, and bringing together experts working in many areas relevant to this mission will allow sharing of knowledge and experience, leading to greater coherence across specialty and geographical boundaries to accelerate progress to the clinic. This is in line with CIRM’s mission to speed up the development of stem cell treatments, increase the likelihood of successful clinical translation, and fill an unmet clinical need. Of note, HD is widely regarded as a model neurodegenerative condition, given that the genetic mutation is known, and thus, success in development of stem cell therapies for HD is highly likely to have relevance for other neurodegenerative conditions.
+ </t>
+  </si>
+  <si>
+    <t>Regenerative Medicine; RNA; Stem Cell Transplantation; Immunosuppression Therapy; Neurodegenerative Diseases; Mutation; Genetic Therapy; Biology</t>
+  </si>
+  <si>
+    <t>Effective neurorestorative or neuroregenerative strategies based on human stem cell products offer a potential treatment option to modulate disease pathology in a complex tissue such as the brain1. Huntington’s disease (HD) is a potential indication for regenerative medicine given it is a devastating neurodegenerative disorder that currently has no FDA approved treatment that changes the onset or course of disease, creating a significant unmet need. Several genetic approaches to treat HD have been tested in clinical trials or are being tested. Reducing levels of the Huntingtin (HTT) protein through Anti-Sense Oligonucleotides (ASOs) or through gene therapy approaches has had mixed results, in one case failing in a Phase 3 trial (Roche, ASO). However, a recent early phase gene therapy trial (UniQure) is showing benefit. Recent HD research supports targeting genes that modify age-of-onset (e.g. MSH3) or production of Huntingtin exon 1 protein (HTT1a). Our proposed allogeneic, off-the-shelf hNSC-01 cell therapy and clinical trial represents a unique, safe and potentially therapeutic and neurorestorative approach in HD that could also be complementary to other emerging approaches.
+HD, which has an estimated prevalence of 10-13/100,000 in the U.S., is devastating for HD sufferers and their families. HD is autosomal dominant and children of existing patients have a 50% risk of developing the disease2, thus affecting multiple generations. HD diagnosis is typically made when an individual is in the prime of life between the ages of 35-50, have families and are at the peak of their careers. There is also a juvenile-onset form of HD. HD sufferers show a triad of symptoms that progress over time: a movement disorder, most often chorea or rigidity, cognitive impairment with an inability to carry out daily tasks, and psychiatric symptoms, including depression and suicidality3. Further, the disease profoundly impacts families, with HD patients showing progressive disease symptoms for 10-20 years before individuals pass from complications of the disease. However, there is relatively focal and specific loss of striatal medium spiny neurons and loss of cortico- striatal circuitry, supporting the possibility that transplantation of neural stem cells might provide neuroprotective or neurorestorative outcomes. Initial evidence of safety in humans of this approach arose from human fetal-cell transplants in HD patients showing overall feasibility and safety1,4. Cell-based approaches for treatment of neurodegenerative and neurological diseases have the potential to modulate neuropathology, as suggested by promising preclinical studies5-8 and recent promising early-stage clinical studies. BlueRock Therapeutics/Bayer (https://www.bluerocktx.com/) recently received RMAT designation following a Phase 1 clinical trial of ESC-derived dopaminergic neuron precursors in Parkinson’s disease patients, that showed both safety and increase in F-DOPA PET imaging signal after stopping immune suppression therapy at 12 months, showing that transplanted cells survive and engraft in human brain. Neurona (https://www.neuronatherapeutics.com/) has shown safety and efficacy with significant seizure suppression in a Phase I/II clinical trial of ESC-derived GABA-ergic interneurons for chronic focal epilepsy.</t>
+  </si>
+  <si>
+    <t>Humans; Child; Child, Preschool; Chorea; Oligonucleotides, Antisense; Regenerative Medicine; Medium Spiny Neurons; Depression; Dopaminergic Neurons; Feasibility Studies; Parkinson Disease; Prevalence; Neurodegenerative Diseases; Epilepsies, Partial; Seizures; Brain; Cell- and Tissue-Based Therapy; Cognitive Dysfunction; Neural Stem Cells; Hematopoietic Stem Cell Transplantation; Dihydroxyphenylalanine; gamma-Aminobutyric Acid</t>
+  </si>
+  <si>
+    <t>ALS is a relentlessly progressive, degenerative disease that destroys the nerve cells that control voluntary muscle movement, with an average life expectancy range from two to five years after clinical diagnosis1, 2. The vast majority of ALS patients have no family history of the disease and do not have pathogenic variants in the genes known to cause ALS. There are several fundamental challenges to treatments for ALS. First, ALS is not a single disease. Even familial ALS (fALS) has roughly 30 different genetic causes3, and importantly, clinical examination, demographics, or standard biofluid measures do not distinguish among these different initiating pathogenic causes. Sporadic ALS (sALS) is clinically indistinguishable from fALS and represents up to 90% of ALS cases. After many years of numerous clinical trials, only two drugs, riluzole4 and edaravone5, are approved for ALS but only have minor benefit. More recently, the antisense oligonucleotide tofersen6, has been approved for the treatment of SOD1-ALS. At this time, diagnosis of ALS is based on clinical findings, including the ALS functional rating scale, and there can be a significant delay from when an individual begins to manifest symptoms until when they are diagnosed. Diagnosis is primarily based on disease exclusion, which can make it difficult to diagnose early. This results in an unacceptable situation given the median life expectancy is only 3.5 years. This delayed diagnosis may close the therapeutic window, such that disease has progressed beyond when benefit can occur, or benefits may be reduced. Although there are several new biomarkers or biomarker candidates that have been developed in recent years, such as (neurofilament light chain) NfL, C9orf72 dipeptide repeat proteins, SOD1, Ataxin2 and TDP-43 associated RNAs or proteins7, these are typically detected later in disease or are specific for certain familial ALS mutations. Identifying potential biomarkers that can detect ALS in its early, treatable stages is crucial for advancing cell and gene therapies aimed at delaying disease progression. These biomarkers could also stratify patients into subgroups with predictable outcomes, significantly enhancing the evaluation of ALS treatment efficacy. Therefore, there is an urgent need for novel molecular biomarkers to determine early stages of ALS early stage with high sensitivity and specificity.</t>
+  </si>
+  <si>
+    <t>Humans; Salts; Superoxide Dismutase-1; Oligonucleotides, Antisense; C9orf72 Protein; Delayed Diagnosis; Intermediate Filaments; Treatment Outcome; Sodium Chloride; Muscle, Skeletal; Disease Progression; Biomarkers; Mutation; Neurons; Demography</t>
+  </si>
+  <si>
+    <t>ALS is a relentlessly progressive, degenerative disease that destroys the nerve cells that control voluntary muscle movement, with an average life expectancy of two to five years after clinical diagnosis. The majority of ALS patients have no family history of the disease and do not have pathogenic variants in the genes known to cause familial ALS (fALS). There are several fundamental challenges to treatments for ALS. First, ALS is not a single disease. Even fALS has at least 30 different genetic causes, and importantly, clinical examination, demographics, or standard biofluid measures do not distinguish among these different initiating pathogenic causes. Sporadic ALS (sALS) is clinically indistinguishable from fALS and represents up to 90% of ALS cases. As the diagnosis of ALS is based on clinical findings, there can be a significant delay from when an individual begins to manifest symptoms until diagnosis. Hence diagnosis is primarily based on disease exclusion, which can make ALS diagnosis difficult and lengthy. This delayed diagnosis may close the therapeutic window because the disease has progressed beyond when benefit can occur, or benefits may be reduced. Although there are several new biomarkers or biomarker candidates that have been developed in recent years, these are typically detected later in disease and/or are specific for certain familial ALS mutations. Our proposal represents a pivotal transition from basic science research to clinical application, with the goal of developing cell-free DNA (cfDNA) methylation biomarkers for ALS early detection and prognosis, with potential to also stratify ALS patient subgroups. Here we propose to create a human fluid based “liquid biopsy” biomarker designed specifically for ALS. Our proposed studies will test plasma samples from a diverse clinical cohort of patients from the ALS Center at Emory University and an independent validation clinical cohort from the Answer ALS program. The genetic and clinical information available will allow us to determine if cfDNA methylation outcomes can separate patient subgroups with known mutations and permit monitoring of disease progression. R61 phase. Retrospective study of cfDNA from 500 coded samples from the Emory ALS Center. Following targeted Enzymatic Methyl-seq (EM-seq) on plasma cfDNA, we will integrate multiple epigenetic modalities, namely cfDNA methylation and nucleosome occupancy, into a Multimodal Epigenetic Sequencing Analysis (MESA) model for ALS early detection and prognosis. R33 phase: Validation of cfDNA epigenetic signature from 250 coded ALS samples from the Answer ALS program including multiple time points and controls and clinical validation to test utility of the biomarker. We will test an independent clinical cohort from the Answer ALS program to determine reproducibility of plasma cfDNA as a diagnostic and prognostic ALS biomarker. Additionally, we will correlate these cfDNA signatures with clinical measures and compare them to NfL levels in blood, demonstrating the enhanced clinical utility of cfDNA signatures.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABSTRACT Striatal medium spiny neuron (MSN) dysfunction and degeneration is a hallmark feature of XDP, the underlying molecular mechanisms of which remain unclear. In a MPI CCXDP grant with the Finkbeiner lab, we developed an omics and cellbased screening platform using robotic microscopy (RM) and bioinformatics analyses, which identified increased cell death, longer neurites and altered genetic pathways in XDP iPSC-derived MSNs (iMSNs). We generated and validated two XDPCRISPRi lines, setting the foundation for unbiased genetic screening. Here we propose to extend these results and investigate additional spatial signatures in XDP by performing TDP-43 staining and spatial transcriptomics of post-mortem brain as well as a CRISPR-pooled screen, in a collaborative effort with the Finkbeiner lab (see co-submitted Finkbeiner application). </t>
+  </si>
+  <si>
+    <t>Medium Spiny Neurons; Clustered Regularly Interspaced Short Palindromic Repeats; Induced Pluripotent Stem Cells; Microscopy; Neurites; Robotic Surgical Procedures; Brain; Gene Expression Profiling; Cell Death</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Objective – The overall objective of this proposal is to explore the means by which human neural precursor 
+cell (hNPC)-induced regulatory T cells (Tregs) promote remyelination and clinical recovery following hNPC 
+transplantation into mouse models of multiple sclerosis. These mouse models include mice infected with 
+the neurotropic JHM strain of mouse hepatitis virus (JHMV) and mice undergoing experimental autoimmune 
+encephalomyelitis (EAE). Persistent infection of mice with JHMV is characterized by ongoing demyelination 
+mediated by inflammatory T cells and macrophages that is similar both clinically and histologically with the 
+human demyelinating disease multiple sclerosis (MS). The use of viral models of demyelination are clinically 
+relevant as the etiology of MS is enigmatic and infectious agents such as viruses have long-been 
+considered important in triggering MS. Indeed, recent reports demonstrate a strong link between infection 
+with Epstein-Barr Virus (EBV) and MS susceptibility [12]. Therefore, use of a viral model of demyelination 
+is relevant not only to study molecular and cellular mechanisms contributing to white matter damage but 
+also provides an important model to evaluate novel therapeutic approaches to initiate remyelination. EAE 
+is an autoimmune model of MS and is appropriate to employ when the goal is to understand the 
+immunoregulatory features of regenerative therapies such as hNPC transplantation. Used together, these 
+JHMV and EAE MS models will allow us to determine the immunomodulatory influence of hNPC 
+transplantation, knowledge that will be vital to the development of stem cell-based therapies for MS patients. </t>
+  </si>
+  <si>
+    <t>Humans; Animals; Mice; Herpesvirus 4, Human; Multiple Sclerosis; Encephalomyelitis, Autoimmune, Experimental; T-Lymphocytes, Regulatory; White Matter; Murine hepatitis virus; Epstein-Barr Virus Infections; Goals; Persistent Infection; Remyelination; Macrophages; Stem Cells</t>
+  </si>
+  <si>
+    <t>Objective: The overall objective of this proposal is to explore mechanisms by which hNPC-induced regulatory T cells (Tregs) promote remyelination and clinical recovery following hNPC transplantation into mouse models of multiple sclerosis that include 1) mice infected with JHMV and 2) mice undergoing EAE following immunization with encephalitogenic peptide myelin oligodendrocyte glycoprotein (MOG)33-55. The use of viral models of demyelination are clinically relevant as the etiology of MS is enigmatic and infectious agents such as viruses have long-been considered important in triggering MS. Indeed, recent reports demonstrate a strong link between infection with Epstein-Barr Virus (EBV) and MS susceptibility [10]. Therefore, use of a viral model of demyelination is relevant not only to study molecular and cellular mechanisms contributing to white matter damage but also provides an important model to evaluate novel therapeutic approaches to initiate remyelination. EAE is an autoimmune model of MS and is appropriate to employ when the goal is to understand the immunoregulatory features of regenerative therapies such as hNPC transplantation. Used together, these JHMV and EAE MS models will allow us to determine the immunomodulatory influence of hNPC transplantation, knowledge that will be vital to the development of stem cell-based therapies for MS patients.
+Specific Aims: An important unmet clinical need for MS patients is an effective method for promoting remyelination that can ameliorate clinical symptoms associated with demyelination and restore motor function while limiting immune cell infiltration into the CNS. Using the well-accepted JHMV model of demyelination, we have clearly demonstrated that intraspinal transplantation of hNPCs promotes clinical recovery that is accompanied by reduced T cell and macrophage infiltration into the CNS, limited spread of demyelination, and increased remyelination. Although hNPCs are rejected within 8 days post-transplant (p.t.), the therapeutic benefit is sustained out to at least six months following transplantation, indicating that hNPCs manipulate the local microenvironment allowing for a long-term favorable outcome. Similarly, in the EAE model, we have discovered that hNPC intraspinal transplants decrease demyelination and enhance remyelination, providing key support to the hypothesis that hNPC transplantation may be a viable treatment option for MS patients. Importantly, compelling preliminary data using these pre-clinical MS models demonstrates that recovery is associated with the emergence of Tregs that dampen neuroinflammation and limit ongoing demyelination as well as promoting the maturation of endogenous oligodendrocyte progenitor cells (OPCs) into myelin-competent oligodendrocytes. Oligodendrocytes and microglia are both known to be important for the process of remyelination, but the influence of hNPCs and Tregs on these CNS cell types is poorly understood. This proposal revolves around two interrelated Specific Aims that are designed to evaluate mechanisms associated with the improved clinical outcome in response to hNPC transplantation and to use these findings as guideposts in the identification of novel therapies that are most effective in promoting remyelination and clinical recovery following JHMV-induced and autoimmune demyelination:
+Aim 1: The influence of CNS antigen expression by hNPCs in the generation and function of Tregs for promoting remyelination in MS mouse models. Co-culture of T cells with antigen presenting cells in the presence of hNPCs leads to a significant expansion of Tregs, and we have found that this depends on expression of CNS antigens by these hNPCs. Thus, we wish to extend these studies to the in vivo influence of hNPC transplants. First, we will determine if Tregs recruited into the CNS following instraspinal transplantation of hNPCs are antigen specific. Next, we will assess the impact of transplanting non-viable hNPCs on Treg recruitment and remyelination in mouse MS models. Lastly, we will evaluate the impact of adoptive transfer of hNPC induced Tregs generated ex vivo on remyelination and clinical recovery in mouse MS models.
+Aim 2: Characterizing mechanisms by which hNPC-induced Tregs enhance remyelination. Experiments in this aim are focused on evaluating mechanisms by which hNPC-induced Tregs influence remyelination. We will first determine how hNPC transplantation into mice with established demyelination impacts emergence of OPCs through use of mice in which expression of a red fluorescent protein (DsRed.T1) is under control of mouse NG2 (OPC marker) promoter. We will adoptively transfer in vitro hNPC-expanded Tregs into mice with established demyelination and evaluate the effects on clinical disease, demyelination and remyelination using established methods. We will also assess the functional role of secreted Transglutaminase 2 (Tgm2, TG2) by hNPC-induced Tregs through us of transgenic mice developed in which Tgm2 has been selectively ablated in Tregs by both evaluating clinical disease, demyelination and remyelination in hNPC-transplanted mice and determine the influence of Tregs on
+microglial gene expression and function in mouse models of MS.</t>
+  </si>
+  <si>
+    <t>The UC Irvine Sue &amp; Bill Gross Stem
+Cell Research Center (SCRC)
+proposes to develop a Shared
+Resources Laboratory to offer
+essential technologies and training
+for the development of novel stem
+cell-based modeling. In addition to
+providing access to cutting-edge
+technologies and training for stem
+cell researchers at UC Irvine, these
+vital tools and training opportunities
+will be offered to the broader
+community of stem cell researchers
+across California. This SRL will offer
+the following core service access
+and training opportunities:
+Technologies and Core Services
+1. 3D Bioengineering and
+Organoid Core (3BOC) for use of
+cutting-edge methods (including
+bioprinting and high-throughput
+photo patterning using a PRIMO
+system) for the development of novel
+tissue engineered 2-D and 3-D in vitro models.
+2. iPSC/CRISPR Core for CRISPR targeting of induced pluripotent stem cell (iPSC) and other cell lines as
+well as the generation and banking of a diverse set of iPSC lines for CRISPR studies.
+3. High-Dimensional and Spatial Analysis Core (HDSA) Facility that offers imaging mass cytometry
+(IMC), CyTOF and spatial transcriptomics studies.
+4. Foundational Technology Core Facility that offers flow Cytometry, flow sorting, automated magnetic
+sorting, microscopy/imaging and tissue culture hoods, incubators and equipment necessary for conducting
+stem cell modeling studies.
+Training in Stem Cell Techniques
+Our proposed SRL will continue to provide a two-week hands-on Stem Cell Techniques course (offered
+three times a year). This highly regarded course (see Course Evaluations attached to the Stem Cell
+Techniques Course Syllabus section) has been in existence since 2007 and has trained over 400
+students from a wide variety of institutions. Complementing this very successful course, the following new
+training, which will be available to investigators both within and outside UCI, will be offered through the
+SRL:
+i) a 5-day Bioengineering/Bioprinting/Organoids Bootcamp
+ii) a two-week course on CRISPR modification of human iPSC and embryonic stem cell (ESC) cell lines
+iii) a 5-day intensive course on CyTOF/mass cytometry
+v) a 5-day intensive course on imaging mass cytometry.
+The UCI SRL will leverage these instrumentation, technology and training offerings to enhance knowledge
+sharing and collaboration among stem cell modeling researchers at UCI and across California. To do so,
+we will build on our existing CIRM Bridges and COMPASS programs, the newly launched LA basin
+Regenerative Medicine Consortium (LA-RMC, described below), and emerging SRL Network, as well as
+established relationships with the UCI Center for Applied Innovation and local biotech startups.</t>
+  </si>
+  <si>
+    <t>Humans; Induced Pluripotent Stem Cells; Microscopy; Stem Cell Research; Bioprinting; Regenerative Medicine; Clustered Regularly Interspaced Short Palindromic Repeats; Flow Cytometry; Incubators; Bioengineering; Students; Embryonic Stem Cells; Organoids; Gene Expression Profiling; Image Cytometry; Magnetic Phenomena; Biotechnology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Objective: The overall objective of this proposal is to explore mechanisms by which hNSC-induced 
+regulatory T cells (Tregs) promote remyelination and clinical recovery following hNSC transplantation into 
+mouse models of MS that include 1) mice infected with JHMV and 2) mice undergoing EAE following 
+immunization with encephalitogenic peptide myelin oligodendrocyte glycoprotein (MOG)33-55. The use of 
+viral models of demyelination are clinically relevant as the etiology of MS is enigmatic and infectious agents 
+such as viruses have long-been considered important in triggering MS. Indeed, recent reports demonstrate 
+a strong link between infection with Epstein-Barr Virus (EBV) and MS susceptibility (18). Therefore, use of 
+a viral model of demyelination is relevant not only to study molecular and cellular mechanisms contributing 
+to white matter damage but also provides an important model to evaluate novel therapeutic approaches to 
+initiate remyelination. EAE is the prototypic autoimmune model of MS and is appropriate to employ when 
+the goal is to understand the immunoregulatory features of regenerative therapies such as hNSC 
+transplantation. Used together, these JHMV and EAE MS models will allow us to determine the 
+immunomodulatory influence of hNSC transplantation, knowledge that will be vital to the development of 
+stem cell-based therapies for MS patients. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Background: Provide Biological/Technological significance and rationale for the project. Targazyme has produced the drug TZ101, a kit comprised of recombinant fucosyltransferase VI and its substrate, GDP-fucose that targets therapeutic cells to selectins. The selectins are carbohydrate-binding cell adhesion molecules constitutively expressed on bone marrow endothelia and skin; they are also up regulated in other tissues under conditions of inflammation in the CNS tissue injury or ischemia. As these conditions are present in a variety of diseases, it is possible to use selectin-mediated homing to target a variety of cell types to the appropriate therapeutic sites in different disease states. The selectin ligands are fucosylated structures and this process is catalyzed by alpha (1,3)-fucosyltransferase VI (FUT6 or FUTVI) and the engraftment efficiency is directly proportional to the level of fucosylation of selectin ligands. Preclinical and clinical data from our group and others support that diminished homing of cells might result, in part, from defective post translational fucosylation and Targazyme's proprietary TZ101 technology works at this critical juncture to transform the homing of TZ101 regulatory T cells (Tregs) to the CNS with improved residence time. Targazyme’s phase 3 off-the-shelf enzyme product TZ101 has already been proven safe and efficacious in phase 2 hematopoietic stem cell trials for blood cancer patients at MD Anderson Cancer Center where TZ101 is proven to accelerate stem cell engraftment/hematopoietic reconstitution and reduces post-transplant morbidities such as cGVHD, engraftment failure, infections with a 22 percent improvement in patient survival, resulting in an FDA phase 3 Special Protocol award. Treg preclinical studies published in blood also demonstrate that TZ101 improves the homing of Tregs to sites of alloreactive T-cell attack with improved residence time in sites of GVHD resulting in reduced GVHD scores and improved survival in mice. Given the enhanced recruitment of Tregs into the CNS and reduced GVHD in patients and mice following aPBSCT, we are interested in the potential that TZ101 may be beneficial for Relapsing Remitting Multiple Sclerosis (RRMS) patients. To address this hypothesis, we will use TZ101 treatment along with GVHD in an RRMS mouse model called experimental autoimmune encephalomyelitis (EAE) involving immunization of MOG35-55 peptides plus adjuvants. We believe that TZ101 will improve engraftment efficiency and Treg recruitment and function within the CNS of EAE mice, and studies described here will help us to address this hypothesis. </t>
+  </si>
+  <si>
+    <t>Humans; Animals; Mice; Bone Marrow; T-Lymphocytes, Regulatory; Fucose; Encephalomyelitis, Autoimmune, Experimental; S Phase; Fucosyltransferases; Multiple Sclerosis, Relapsing-Remitting; Multiple Sclerosis; Immunization; Adjuvants, Immunologic; Hematopoietic Stem Cells; Hematologic Neoplasms; Inflammation; Ischemia; Cell Adhesion Molecules; Hematopoietic Stem Cell Transplantation; Graft vs Host Disease; Clinical Trials, Phase II as Topic</t>
   </si>
 </sst>
 </file>
@@ -4372,10 +4764,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AF44EFF-A679-48DE-87D3-4A4765F6BA38}">
-  <dimension ref="A1:F412"/>
+  <dimension ref="A1:F445"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A392" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F412" sqref="F412"/>
+    <sheetView tabSelected="1" topLeftCell="A424" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F445" sqref="F445"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -4384,7 +4776,7 @@
     <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="255.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -11825,6 +12217,567 @@
       </c>
       <c r="F412" t="s">
         <v>918</v>
+      </c>
+    </row>
+    <row r="413" spans="1:6">
+      <c r="A413" t="s">
+        <v>907</v>
+      </c>
+      <c r="B413">
+        <v>225179</v>
+      </c>
+      <c r="C413" t="s">
+        <v>38</v>
+      </c>
+      <c r="E413" t="s">
+        <v>919</v>
+      </c>
+      <c r="F413" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="414" spans="1:6">
+      <c r="A414" t="s">
+        <v>907</v>
+      </c>
+      <c r="B414">
+        <v>225968</v>
+      </c>
+      <c r="C414" t="s">
+        <v>38</v>
+      </c>
+      <c r="E414" t="s">
+        <v>921</v>
+      </c>
+      <c r="F414" t="s">
+        <v>922</v>
+      </c>
+    </row>
+    <row r="415" spans="1:6">
+      <c r="A415" t="s">
+        <v>907</v>
+      </c>
+      <c r="B415">
+        <v>229228</v>
+      </c>
+      <c r="C415" t="s">
+        <v>38</v>
+      </c>
+      <c r="E415" t="s">
+        <v>923</v>
+      </c>
+      <c r="F415" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="416" spans="1:6">
+      <c r="A416" t="s">
+        <v>907</v>
+      </c>
+      <c r="B416">
+        <v>232377</v>
+      </c>
+      <c r="C416" t="s">
+        <v>38</v>
+      </c>
+      <c r="E416" t="s">
+        <v>925</v>
+      </c>
+      <c r="F416" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="417" spans="1:6">
+      <c r="A417" t="s">
+        <v>927</v>
+      </c>
+      <c r="B417">
+        <v>225453</v>
+      </c>
+      <c r="C417" t="s">
+        <v>50</v>
+      </c>
+      <c r="E417" t="s">
+        <v>928</v>
+      </c>
+      <c r="F417" t="s">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="418" spans="1:6">
+      <c r="A418" t="s">
+        <v>927</v>
+      </c>
+      <c r="B418">
+        <v>226076</v>
+      </c>
+      <c r="C418" t="s">
+        <v>50</v>
+      </c>
+      <c r="E418" t="s">
+        <v>930</v>
+      </c>
+      <c r="F418" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="419" spans="1:6">
+      <c r="A419" t="s">
+        <v>932</v>
+      </c>
+      <c r="B419">
+        <v>224791</v>
+      </c>
+      <c r="C419" t="s">
+        <v>31</v>
+      </c>
+      <c r="E419" t="s">
+        <v>933</v>
+      </c>
+      <c r="F419" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="420" spans="1:6">
+      <c r="A420" t="s">
+        <v>932</v>
+      </c>
+      <c r="B420">
+        <v>225707</v>
+      </c>
+      <c r="C420" t="s">
+        <v>31</v>
+      </c>
+      <c r="E420" t="s">
+        <v>935</v>
+      </c>
+      <c r="F420" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="421" spans="1:6">
+      <c r="A421" t="s">
+        <v>932</v>
+      </c>
+      <c r="B421">
+        <v>226723</v>
+      </c>
+      <c r="C421" t="s">
+        <v>31</v>
+      </c>
+      <c r="E421" t="s">
+        <v>936</v>
+      </c>
+      <c r="F421" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="422" spans="1:6">
+      <c r="A422" t="s">
+        <v>932</v>
+      </c>
+      <c r="B422">
+        <v>229458</v>
+      </c>
+      <c r="C422" t="s">
+        <v>31</v>
+      </c>
+      <c r="E422" t="s">
+        <v>937</v>
+      </c>
+      <c r="F422" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="423" spans="1:6">
+      <c r="A423" t="s">
+        <v>932</v>
+      </c>
+      <c r="B423">
+        <v>230237</v>
+      </c>
+      <c r="C423" t="s">
+        <v>31</v>
+      </c>
+      <c r="E423" t="s">
+        <v>938</v>
+      </c>
+      <c r="F423" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="424" spans="1:6">
+      <c r="A424" t="s">
+        <v>932</v>
+      </c>
+      <c r="B424">
+        <v>230979</v>
+      </c>
+      <c r="C424" t="s">
+        <v>31</v>
+      </c>
+      <c r="E424" t="s">
+        <v>939</v>
+      </c>
+      <c r="F424" t="s">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="425" spans="1:6">
+      <c r="A425" t="s">
+        <v>932</v>
+      </c>
+      <c r="B425">
+        <v>231392</v>
+      </c>
+      <c r="C425" t="s">
+        <v>31</v>
+      </c>
+      <c r="E425" t="s">
+        <v>941</v>
+      </c>
+      <c r="F425" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="426" spans="1:6">
+      <c r="A426" t="s">
+        <v>932</v>
+      </c>
+      <c r="B426">
+        <v>232438</v>
+      </c>
+      <c r="C426" t="s">
+        <v>31</v>
+      </c>
+      <c r="E426" t="s">
+        <v>938</v>
+      </c>
+      <c r="F426" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="427" spans="1:6">
+      <c r="A427" t="s">
+        <v>256</v>
+      </c>
+      <c r="B427">
+        <v>222909</v>
+      </c>
+      <c r="C427" t="s">
+        <v>50</v>
+      </c>
+      <c r="E427" t="s">
+        <v>942</v>
+      </c>
+      <c r="F427" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="428" spans="1:6">
+      <c r="A428" t="s">
+        <v>187</v>
+      </c>
+      <c r="B428">
+        <v>226686</v>
+      </c>
+      <c r="C428" t="s">
+        <v>31</v>
+      </c>
+      <c r="E428" t="s">
+        <v>944</v>
+      </c>
+      <c r="F428" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="429" spans="1:6">
+      <c r="A429" t="s">
+        <v>187</v>
+      </c>
+      <c r="B429">
+        <v>227718</v>
+      </c>
+      <c r="C429" t="s">
+        <v>31</v>
+      </c>
+      <c r="E429" t="s">
+        <v>946</v>
+      </c>
+      <c r="F429" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="430" spans="1:6">
+      <c r="A430" t="s">
+        <v>187</v>
+      </c>
+      <c r="B430">
+        <v>229898</v>
+      </c>
+      <c r="C430" t="s">
+        <v>31</v>
+      </c>
+      <c r="E430" t="s">
+        <v>948</v>
+      </c>
+      <c r="F430" t="s">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="431" spans="1:6">
+      <c r="A431" t="s">
+        <v>187</v>
+      </c>
+      <c r="B431">
+        <v>233160</v>
+      </c>
+      <c r="C431" t="s">
+        <v>31</v>
+      </c>
+      <c r="E431" t="s">
+        <v>950</v>
+      </c>
+      <c r="F431" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="432" spans="1:6">
+      <c r="A432" t="s">
+        <v>61</v>
+      </c>
+      <c r="B432">
+        <v>224221</v>
+      </c>
+      <c r="C432" t="s">
+        <v>38</v>
+      </c>
+      <c r="E432" t="s">
+        <v>951</v>
+      </c>
+      <c r="F432" t="s">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="433" spans="1:6">
+      <c r="A433" t="s">
+        <v>61</v>
+      </c>
+      <c r="B433">
+        <v>225871</v>
+      </c>
+      <c r="C433" t="s">
+        <v>38</v>
+      </c>
+      <c r="E433" t="s">
+        <v>953</v>
+      </c>
+      <c r="F433" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="434" spans="1:6">
+      <c r="A434" t="s">
+        <v>61</v>
+      </c>
+      <c r="B434">
+        <v>229233</v>
+      </c>
+      <c r="C434" t="s">
+        <v>38</v>
+      </c>
+      <c r="E434" t="s">
+        <v>955</v>
+      </c>
+      <c r="F434" t="s">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="435" spans="1:6">
+      <c r="A435" t="s">
+        <v>61</v>
+      </c>
+      <c r="B435">
+        <v>229570</v>
+      </c>
+      <c r="C435" t="s">
+        <v>38</v>
+      </c>
+      <c r="E435" t="s">
+        <v>957</v>
+      </c>
+      <c r="F435" t="s">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="436" spans="1:6">
+      <c r="A436" t="s">
+        <v>61</v>
+      </c>
+      <c r="B436">
+        <v>230321</v>
+      </c>
+      <c r="C436" t="s">
+        <v>38</v>
+      </c>
+      <c r="E436" t="s">
+        <v>959</v>
+      </c>
+      <c r="F436" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="437" spans="1:6">
+      <c r="A437" t="s">
+        <v>61</v>
+      </c>
+      <c r="B437">
+        <v>231086</v>
+      </c>
+      <c r="C437" t="s">
+        <v>38</v>
+      </c>
+      <c r="E437" t="s">
+        <v>961</v>
+      </c>
+      <c r="F437" t="s">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="438" spans="1:6">
+      <c r="A438" t="s">
+        <v>61</v>
+      </c>
+      <c r="B438">
+        <v>231344</v>
+      </c>
+      <c r="C438" t="s">
+        <v>38</v>
+      </c>
+      <c r="E438" t="s">
+        <v>963</v>
+      </c>
+      <c r="F438" t="s">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="439" spans="1:6">
+      <c r="A439" t="s">
+        <v>61</v>
+      </c>
+      <c r="B439">
+        <v>232748</v>
+      </c>
+      <c r="C439" t="s">
+        <v>38</v>
+      </c>
+      <c r="E439" t="s">
+        <v>964</v>
+      </c>
+      <c r="F439" t="s">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="440" spans="1:6">
+      <c r="A440" t="s">
+        <v>269</v>
+      </c>
+      <c r="B440">
+        <v>224437</v>
+      </c>
+      <c r="C440" t="s">
+        <v>31</v>
+      </c>
+      <c r="E440" t="s">
+        <v>966</v>
+      </c>
+      <c r="F440" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="441" spans="1:6">
+      <c r="A441" t="s">
+        <v>269</v>
+      </c>
+      <c r="B441">
+        <v>225939</v>
+      </c>
+      <c r="C441" t="s">
+        <v>31</v>
+      </c>
+      <c r="E441" t="s">
+        <v>968</v>
+      </c>
+      <c r="F441" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="442" spans="1:6">
+      <c r="A442" t="s">
+        <v>269</v>
+      </c>
+      <c r="B442">
+        <v>228577</v>
+      </c>
+      <c r="C442" t="s">
+        <v>31</v>
+      </c>
+      <c r="E442" t="s">
+        <v>969</v>
+      </c>
+      <c r="F442" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="443" spans="1:6">
+      <c r="A443" t="s">
+        <v>269</v>
+      </c>
+      <c r="B443">
+        <v>229256</v>
+      </c>
+      <c r="C443" t="s">
+        <v>31</v>
+      </c>
+      <c r="E443" t="s">
+        <v>971</v>
+      </c>
+      <c r="F443" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="444" spans="1:6">
+      <c r="A444" t="s">
+        <v>269</v>
+      </c>
+      <c r="B444">
+        <v>229796</v>
+      </c>
+      <c r="C444" t="s">
+        <v>31</v>
+      </c>
+      <c r="E444" t="s">
+        <v>972</v>
+      </c>
+      <c r="F444" t="s">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="445" spans="1:6">
+      <c r="A445" t="s">
+        <v>269</v>
+      </c>
+      <c r="B445">
+        <v>232020</v>
+      </c>
+      <c r="C445" t="s">
+        <v>31</v>
+      </c>
+      <c r="E445" t="s">
+        <v>972</v>
+      </c>
+      <c r="F445" t="s">
+        <v>973</v>
       </c>
     </row>
   </sheetData>
@@ -11841,19 +12794,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Notes xmlns="b238fc39-fcbb-4f8c-bfd3-e3a789f7784e" xsi:nil="true"/>
-    <ProjectRole xmlns="b238fc39-fcbb-4f8c-bfd3-e3a789f7784e" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b238fc39-fcbb-4f8c-bfd3-e3a789f7784e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="ccd2e96c-ba06-41a4-9d14-ee5d4767a409" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002B87155CDAEBE54E8A991CDFF09FE870" ma:contentTypeVersion="21" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="07d22f826efb92a1b7f7a52cdc9ab0c0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ccd2e96c-ba06-41a4-9d14-ee5d4767a409" xmlns:ns3="b238fc39-fcbb-4f8c-bfd3-e3a789f7784e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8f50f4dd1661db9c8120150ec829b0b2" ns2:_="" ns3:_="">
     <xsd:import namespace="ccd2e96c-ba06-41a4-9d14-ee5d4767a409"/>
@@ -12127,6 +13067,19 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Notes xmlns="b238fc39-fcbb-4f8c-bfd3-e3a789f7784e" xsi:nil="true"/>
+    <ProjectRole xmlns="b238fc39-fcbb-4f8c-bfd3-e3a789f7784e" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b238fc39-fcbb-4f8c-bfd3-e3a789f7784e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="ccd2e96c-ba06-41a4-9d14-ee5d4767a409" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -12137,11 +13090,11 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3F88ABE-1F09-4246-805E-5B35215270F6}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B9E692F-2B0F-42AD-B3D3-6C71619FC4A6}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B9E692F-2B0F-42AD-B3D3-6C71619FC4A6}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3F88ABE-1F09-4246-805E-5B35215270F6}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>